<commit_message>
added stock to watchlist file
</commit_message>
<xml_diff>
--- a/input/Watchlist.xlsx
+++ b/input/Watchlist.xlsx
@@ -1,30 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sivac\Documents\Analytics\us-stocks-analysis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{6E1C2BE8-C219-4F37-B9FE-44AAFDD9C31D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00432006-A320-4D68-8FB1-70155BB7901E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C20CFB-FE03-452E-9027-14D29E3DA195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="32281" windowHeight="13148" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fund List" sheetId="1" r:id="rId1"/>
     <sheet name="Stock List" sheetId="2" r:id="rId2"/>
     <sheet name="Strategy" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
@@ -40,13 +38,13 @@
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="56">
+  <futureMetadata name="XLRICHVALUE" count="57">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -439,13 +437,20 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="225"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="56">
+  <valueMetadata count="57">
     <bk>
       <rc t="2" v="0"/>
     </bk>
@@ -613,6 +618,9 @@
     </bk>
     <bk>
       <rc t="2" v="55"/>
+    </bk>
+    <bk>
+      <rc t="2" v="56"/>
     </bk>
   </valueMetadata>
 </metadata>
@@ -824,10 +832,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -881,14 +889,14 @@
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -930,7 +938,7 @@
         <name val="Source Sans Pro"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -948,7 +956,7 @@
         <name val="Source Sans Pro"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -984,7 +992,7 @@
         <name val="Source Sans Pro"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -1002,7 +1010,7 @@
         <name val="Source Sans Pro"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -1020,7 +1028,7 @@
         <name val="Source Sans Pro"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -1038,7 +1046,7 @@
         <name val="Source Sans Pro"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -1222,7 +1230,7 @@
         <name val="Source Sans Pro"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -1240,7 +1248,7 @@
         <name val="Source Sans Pro"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -1276,7 +1284,7 @@
         <name val="Source Sans Pro"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -1294,7 +1302,7 @@
         <name val="Source Sans Pro"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -1312,7 +1320,7 @@
         <name val="Source Sans Pro"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -1330,7 +1338,7 @@
         <name val="Source Sans Pro"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -1577,7 +1585,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="220">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="226">
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a25bqh&amp;q=ARCX%3aVHT&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
@@ -4568,11 +4576,80 @@
   <rv s="2">
     <v>218</v>
   </rv>
+  <rv s="0">
+    <v>http://en.wikipedia.org/wiki/Costco</v>
+    <v>Wikipedia</v>
+  </rv>
+  <rv s="9">
+    <v>103</v>
+    <v>220</v>
+  </rv>
+  <rv s="14">
+    <v>Powered by Refinitiv</v>
+    <v>34</v>
+    <v>https://www.bing.com/th?id=AMMS_90a82bf7d9bf620ad2bd5ec79a4882af&amp;qlt=95</v>
+    <v>221</v>
+    <v>https://www.bing.com/images/search?form=xlimg&amp;q=costco</v>
+    <v>Image of COSTCO WHOLESALE CORPORATION</v>
+    <v/>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1q6k2&amp;q=XNAS%3aCOST&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="15">
+    <v>en-US</v>
+    <v>a1q6k2</v>
+    <v>268435456</v>
+    <v>268435457</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>31</v>
+    <v>COSTCO WHOLESALE CORPORATION (XNAS:COST)</v>
+    <v>21</v>
+    <v>32</v>
+    <v>Finance</v>
+    <v>33</v>
+    <v>329.32</v>
+    <v>262.70999999999998</v>
+    <v>0.68510000000000004</v>
+    <v>-0.34</v>
+    <v>-1.047E-3</v>
+    <v>USD</v>
+    <v>Costco Wholesale Corporation is engaged in the operation of membership warehouses in the United States and Puerto Rico, Canada, the United Kingdom, Mexico, Japan, Australia, Spain, and through its subsidiaries in Taiwan and Korea. As of August 28, 2016, the Company operated 715 warehouses across the world. The Company's average warehouse space is approximately 144,000 square feet. The Company's warehouses on average operate on a seven-day, 70-hour week. The Company offers merchandise in various categories, which include foods (including dry foods, packaged foods and groceries); sundries (including snack foods, candy, alcoholic and nonalcoholic beverages, and cleaning supplies); hardlines (including appliances, electronics, health and beauty aids, hardware, and garden and patio); fresh foods (including meat, produce, deli and bakery); softlines (including apparel and small appliances), and other (including gas stations and pharmacy).</v>
+    <v>149000</v>
+    <v>Nasdaq Stock Market</v>
+    <v>XNAS</v>
+    <v>XNAS</v>
+    <v>999 Lake Dr, ISSAQUAH, WA, 98027-8990 US</v>
+    <v>325.19</v>
+    <v>222</v>
+    <v>Diversified Retail</v>
+    <v>Stock</v>
+    <v>44032.56600875</v>
+    <v>223</v>
+    <v>324.14999999999998</v>
+    <v>COSTCO WHOLESALE CORPORATION</v>
+    <v>COSTCO WHOLESALE CORPORATION</v>
+    <v>325</v>
+    <v>38.588999999999999</v>
+    <v>324.79000000000002</v>
+    <v>324.45</v>
+    <v>441523700</v>
+    <v>COST</v>
+    <v>COSTCO WHOLESALE CORPORATION (XNAS:COST)</v>
+    <v>68771</v>
+    <v>2601846</v>
+    <v>1987</v>
+  </rv>
+  <rv s="2">
+    <v>224</v>
+  </rv>
 </rvData>
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="14">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="16">
   <s t="_hyperlink">
     <k n="Address" t="s"/>
     <k n="Text" t="s"/>
@@ -4955,12 +5032,66 @@
     <k n="Volume average"/>
     <k n="Year incorporated"/>
   </s>
+  <s t="_imageurl">
+    <k n="%ProviderInfo" t="s"/>
+    <k n="_Flags" t="spb"/>
+    <k n="Address" t="s"/>
+    <k n="Attribution" t="r"/>
+    <k n="More Images Address" t="s"/>
+    <k n="Text" t="s"/>
+    <k n="Blip Identifier" t="s"/>
+  </s>
+  <s t="_linkedentitycore">
+    <k n="%EntityCulture" t="s"/>
+    <k n="%EntityId" t="s"/>
+    <k n="%EntityServiceId"/>
+    <k n="%EntitySubDomainId"/>
+    <k n="%IsRefreshable" t="b"/>
+    <k n="%ProviderInfo" t="s"/>
+    <k n="_Display" t="spb"/>
+    <k n="_DisplayString" t="s"/>
+    <k n="_Flags" t="spb"/>
+    <k n="_Format" t="spb"/>
+    <k n="_Icon" t="s"/>
+    <k n="_SubLabel" t="spb"/>
+    <k n="52 week high"/>
+    <k n="52 week low"/>
+    <k n="Beta"/>
+    <k n="Change"/>
+    <k n="Change (%)"/>
+    <k n="Currency" t="s"/>
+    <k n="Description" t="s"/>
+    <k n="Employees"/>
+    <k n="Exchange" t="s"/>
+    <k n="Exchange abbreviation" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Headquarters" t="s"/>
+    <k n="High"/>
+    <k n="Image" t="r"/>
+    <k n="Industry" t="s"/>
+    <k n="Instrument type" t="s"/>
+    <k n="Last trade time"/>
+    <k n="LearnMoreOnLink" t="r"/>
+    <k n="Low"/>
+    <k n="Name" t="s"/>
+    <k n="Official name" t="s"/>
+    <k n="Open"/>
+    <k n="P/E"/>
+    <k n="Previous close"/>
+    <k n="Price"/>
+    <k n="Shares outstanding"/>
+    <k n="Ticker symbol" t="s"/>
+    <k n="UniqueName" t="s"/>
+    <k n="Volume"/>
+    <k n="Volume average"/>
+    <k n="Year incorporated"/>
+  </s>
 </rvStructures>
 </file>
 
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
-  <spbArrays count="9">
+  <spbArrays count="10">
     <a count="35">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
@@ -5320,8 +5451,53 @@
       <v t="s">%ProviderInfo</v>
       <v t="s">_Display</v>
     </a>
+    <a count="43">
+      <v t="s">%EntityServiceId</v>
+      <v t="s">_Format</v>
+      <v t="s">%EntitySubDomainId</v>
+      <v t="s">%EntityCulture</v>
+      <v t="s">%IsRefreshable</v>
+      <v t="s">%EntityId</v>
+      <v t="s">_Icon</v>
+      <v t="s">Name</v>
+      <v t="s">_SubLabel</v>
+      <v t="s">Price</v>
+      <v t="s">Exchange</v>
+      <v t="s">Official name</v>
+      <v t="s">Last trade time</v>
+      <v t="s">Ticker symbol</v>
+      <v t="s">Exchange abbreviation</v>
+      <v t="s">Change</v>
+      <v t="s">Change (%)</v>
+      <v t="s">Currency</v>
+      <v t="s">Previous close</v>
+      <v t="s">Open</v>
+      <v t="s">High</v>
+      <v t="s">Low</v>
+      <v t="s">52 week high</v>
+      <v t="s">52 week low</v>
+      <v t="s">Volume</v>
+      <v t="s">Volume average</v>
+      <v t="s">Beta</v>
+      <v t="s">P/E</v>
+      <v t="s">Shares outstanding</v>
+      <v t="s">Description</v>
+      <v t="s">Employees</v>
+      <v t="s">Headquarters</v>
+      <v t="s">Industry</v>
+      <v t="s">Instrument type</v>
+      <v t="s">Year incorporated</v>
+      <v t="s">_Flags</v>
+      <v t="s">UniqueName</v>
+      <v t="s">_DisplayString</v>
+      <v t="s">LearnMoreOnLink</v>
+      <v t="s">Image</v>
+      <v t="s">ExchangeID</v>
+      <v t="s">%ProviderInfo</v>
+      <v t="s">_Display</v>
+    </a>
   </spbArrays>
-  <spbData count="31">
+  <spbData count="35">
     <spb s="0">
       <v>0</v>
     </spb>
@@ -5662,12 +5838,49 @@
       <v>1</v>
       <v>5</v>
     </spb>
+    <spb s="0">
+      <v>9</v>
+    </spb>
+    <spb s="20">
+      <v>1</v>
+      <v>2</v>
+      <v>2</v>
+      <v>1</v>
+      <v>3</v>
+      <v>1</v>
+      <v>10</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>4</v>
+      <v>5</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>7</v>
+      <v>8</v>
+      <v>9</v>
+      <v>11</v>
+      <v>9</v>
+      <v>4</v>
+    </spb>
+    <spb s="21">
+      <v>Real-Time Nasdaq Last Sale</v>
+      <v>from previous close</v>
+      <v>from previous close</v>
+      <v>Source: Nasdaq Last Sale</v>
+      <v>GMT</v>
+    </spb>
+    <spb s="22">
+      <v>1</v>
+    </spb>
   </spbData>
 </supportingPropertyBags>
 </file>
 
 <file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
-<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="20">
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="23">
   <s>
     <k n="^Order" t="spba"/>
   </s>
@@ -5939,6 +6152,40 @@
     <k n="Change (Extended hours)" t="i"/>
     <k n="Change % (Extended hours)" t="i"/>
   </s>
+  <s>
+    <k n="Low" t="i"/>
+    <k n="P/E" t="i"/>
+    <k n="Beta" t="i"/>
+    <k n="High" t="i"/>
+    <k n="Name" t="i"/>
+    <k n="Open" t="i"/>
+    <k n="Image" t="i"/>
+    <k n="Price" t="i"/>
+    <k n="Change" t="i"/>
+    <k n="Volume" t="i"/>
+    <k n="Employees" t="i"/>
+    <k n="Change (%)" t="i"/>
+    <k n="52 week low" t="i"/>
+    <k n="52 week high" t="i"/>
+    <k n="Previous close" t="i"/>
+    <k n="Volume average" t="i"/>
+    <k n="_DisplayString" t="i"/>
+    <k n="Last trade time" t="i"/>
+    <k n="%EntityServiceId" t="i"/>
+    <k n="Year incorporated" t="i"/>
+    <k n="%EntitySubDomainId" t="i"/>
+    <k n="Shares outstanding" t="i"/>
+  </s>
+  <s>
+    <k n="Price" t="s"/>
+    <k n="Change" t="s"/>
+    <k n="Change (%)" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Last trade time" t="s"/>
+  </s>
+  <s>
+    <k n="%ProviderInfo" t="spb"/>
+  </s>
 </spbStructures>
 </file>
 
@@ -5946,7 +6193,7 @@
 <richStyleSheet xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <dxfs count="9">
     <x:dxf>
-      <x:numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <x:numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </x:dxf>
     <x:dxf>
       <x:numFmt numFmtId="4" formatCode="#,##0.00"/>
@@ -5958,10 +6205,10 @@
       <x:numFmt numFmtId="14" formatCode="0.00%"/>
     </x:dxf>
     <x:dxf>
-      <x:numFmt numFmtId="164" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;_);_(@_)"/>
+      <x:numFmt numFmtId="165" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;_);_(@_)"/>
     </x:dxf>
     <x:dxf>
-      <x:numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <x:numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </x:dxf>
     <x:dxf>
       <x:numFmt numFmtId="2" formatCode="0.00"/>
@@ -5970,7 +6217,7 @@
       <x:numFmt numFmtId="1" formatCode="0"/>
     </x:dxf>
     <x:dxf>
-      <x:numFmt numFmtId="175" formatCode="_-[$¥-411]* #,##0_-;\-[$¥-411]* #,##0_-;_-[$¥-411]* &quot;-&quot;_-;_-@_-"/>
+      <x:numFmt numFmtId="164" formatCode="_-[$¥-411]* #,##0_-;\-[$¥-411]* #,##0_-;_-[$¥-411]* &quot;-&quot;_-;_-@_-"/>
     </x:dxf>
   </dxfs>
   <richProperties>
@@ -6047,8 +6294,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D0CAA086-D84C-4EA4-B5F1-7030749A7F3E}" name="Table13" displayName="Table13" ref="A1:N25" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:N25" xr:uid="{7148AA24-1D57-4322-B6E6-30CB6857B1C8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D0CAA086-D84C-4EA4-B5F1-7030749A7F3E}" name="Table13" displayName="Table13" ref="A1:N26" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:N26" xr:uid="{7148AA24-1D57-4322-B6E6-30CB6857B1C8}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N2">
     <sortCondition ref="N1:N2"/>
   </sortState>
@@ -6395,21 +6642,21 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6" max="9" width="11.42578125" style="1"/>
-    <col min="10" max="10" width="11.42578125" style="3"/>
-    <col min="11" max="12" width="11.42578125" style="1"/>
-    <col min="13" max="13" width="11.42578125" style="3"/>
-    <col min="14" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="41.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="1"/>
+    <col min="4" max="4" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6" max="9" width="11.44140625" style="1"/>
+    <col min="10" max="10" width="11.44140625" style="3"/>
+    <col min="11" max="12" width="11.44140625" style="1"/>
+    <col min="13" max="13" width="11.44140625" style="3"/>
+    <col min="14" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6450,7 +6697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -6497,11 +6744,11 @@
         <v>138.11000000000001</v>
       </c>
       <c r="M2" s="3">
-        <f>(K2-I2)/K2</f>
+        <f t="shared" ref="M2:M32" si="0">(K2-I2)/K2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
@@ -6548,11 +6795,11 @@
         <v>35.74</v>
       </c>
       <c r="M3" s="3">
-        <f>(K3-I3)/K3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
@@ -6599,11 +6846,11 @@
         <v>14.809699999999999</v>
       </c>
       <c r="M4" s="3">
-        <f>(K4-I4)/K4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
@@ -6650,11 +6897,11 @@
         <v>183.25</v>
       </c>
       <c r="M5" s="3">
-        <f>(K5-I5)/K5</f>
+        <f t="shared" si="0"/>
         <v>2.6959991372798675E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
@@ -6701,11 +6948,11 @@
         <v>108.08</v>
       </c>
       <c r="M6" s="3">
-        <f>(K6-I6)/K6</f>
+        <f t="shared" si="0"/>
         <v>4.6072911334812351E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
@@ -6752,11 +6999,11 @@
         <v>73.540000000000006</v>
       </c>
       <c r="M7" s="3">
-        <f>(K7-I7)/K7</f>
+        <f t="shared" si="0"/>
         <v>9.5165588123334605E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
@@ -6803,11 +7050,11 @@
         <v>13.99</v>
       </c>
       <c r="M8" s="3">
-        <f>(K8-I8)/K8</f>
+        <f t="shared" si="0"/>
         <v>1.2135761589404119E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
@@ -6854,11 +7101,11 @@
         <v>29.02</v>
       </c>
       <c r="M9" s="3">
-        <f>(K9-I9)/K9</f>
+        <f t="shared" si="0"/>
         <v>1.8174043190079141E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
@@ -6905,11 +7152,11 @@
         <v>26.19</v>
       </c>
       <c r="M10" s="3">
-        <f>(K10-I10)/K10</f>
+        <f t="shared" si="0"/>
         <v>2.225963337074444E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
@@ -6956,11 +7203,11 @@
         <v>41.99</v>
       </c>
       <c r="M11" s="3">
-        <f>(K11-I11)/K11</f>
+        <f t="shared" si="0"/>
         <v>2.5619982158786879E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
@@ -7007,11 +7254,11 @@
         <v>10.86</v>
       </c>
       <c r="M12" s="3">
-        <f>(K12-I12)/K12</f>
+        <f t="shared" si="0"/>
         <v>2.7520435967302588E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
@@ -7058,11 +7305,11 @@
         <v>96</v>
       </c>
       <c r="M13" s="3">
-        <f>(K13-I13)/K13</f>
+        <f t="shared" si="0"/>
         <v>3.1220836566518754E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
@@ -7109,11 +7356,11 @@
         <v>20.36</v>
       </c>
       <c r="M14" s="3">
-        <f>(K14-I14)/K14</f>
+        <f t="shared" si="0"/>
         <v>3.1667576394522348E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
@@ -7160,11 +7407,11 @@
         <v>53</v>
       </c>
       <c r="M15" s="3">
-        <f>(K15-I15)/K15</f>
+        <f t="shared" si="0"/>
         <v>3.2638888888888974E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="e" vm="16">
         <v>#VALUE!</v>
       </c>
@@ -7211,11 +7458,11 @@
         <v>68.099999999999994</v>
       </c>
       <c r="M16" s="3">
-        <f>(K16-I16)/K16</f>
+        <f t="shared" si="0"/>
         <v>3.3448778709442233E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
@@ -7262,11 +7509,11 @@
         <v>179.45</v>
       </c>
       <c r="M17" s="3">
-        <f>(K17-I17)/K17</f>
+        <f t="shared" si="0"/>
         <v>3.3511147585829612E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
@@ -7313,11 +7560,11 @@
         <v>68.948099999999997</v>
       </c>
       <c r="M18" s="3">
-        <f>(K18-I18)/K18</f>
+        <f t="shared" si="0"/>
         <v>3.4228193468375336E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="e" vm="19">
         <v>#VALUE!</v>
       </c>
@@ -7364,11 +7611,11 @@
         <v>24</v>
       </c>
       <c r="M19" s="3">
-        <f>(K19-I19)/K19</f>
+        <f t="shared" si="0"/>
         <v>4.0619120916709425E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="e" vm="20">
         <v>#VALUE!</v>
       </c>
@@ -7415,11 +7662,11 @@
         <v>81.5</v>
       </c>
       <c r="M20" s="3">
-        <f>(K20-I20)/K20</f>
+        <f t="shared" si="0"/>
         <v>5.4384615384615392E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="e" vm="21">
         <v>#VALUE!</v>
       </c>
@@ -7466,11 +7713,11 @@
         <v>200.55</v>
       </c>
       <c r="M21" s="3">
-        <f>(K21-I21)/K21</f>
+        <f t="shared" si="0"/>
         <v>5.7671940691292958E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="e" vm="22">
         <v>#VALUE!</v>
       </c>
@@ -7517,11 +7764,11 @@
         <v>220.2756</v>
       </c>
       <c r="M22" s="3">
-        <f>(K22-I22)/K22</f>
+        <f t="shared" si="0"/>
         <v>5.7837332575524418E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="e" vm="23">
         <v>#VALUE!</v>
       </c>
@@ -7568,11 +7815,11 @@
         <v>109.49</v>
       </c>
       <c r="M23" s="3">
-        <f>(K23-I23)/K23</f>
+        <f t="shared" si="0"/>
         <v>5.839645751222651E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="e" vm="24">
         <v>#VALUE!</v>
       </c>
@@ -7619,11 +7866,11 @@
         <v>45</v>
       </c>
       <c r="M24" s="3">
-        <f>(K24-I24)/K24</f>
+        <f t="shared" si="0"/>
         <v>6.1834769386720674E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="e" vm="25">
         <v>#VALUE!</v>
       </c>
@@ -7670,11 +7917,11 @@
         <v>40.494999999999997</v>
       </c>
       <c r="M25" s="3">
-        <f>(K25-I25)/K25</f>
+        <f t="shared" si="0"/>
         <v>6.5107521553859807E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="e" vm="26">
         <v>#VALUE!</v>
       </c>
@@ -7721,11 +7968,11 @@
         <v>12.36</v>
       </c>
       <c r="M26" s="3">
-        <f>(K26-I26)/K26</f>
+        <f t="shared" si="0"/>
         <v>6.7270375161707724E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="e" vm="27">
         <v>#VALUE!</v>
       </c>
@@ -7772,11 +8019,11 @@
         <v>40.494999999999997</v>
       </c>
       <c r="M27" s="3">
-        <f>(K27-I27)/K27</f>
+        <f t="shared" si="0"/>
         <v>6.8514517887226192E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="e" vm="28">
         <v>#VALUE!</v>
       </c>
@@ -7823,11 +8070,11 @@
         <v>18.989999999999998</v>
       </c>
       <c r="M28" s="3">
-        <f>(K28-I28)/K28</f>
+        <f t="shared" si="0"/>
         <v>9.4224924012158068E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="e" vm="29">
         <v>#VALUE!</v>
       </c>
@@ -7874,11 +8121,11 @@
         <v>38.825000000000003</v>
       </c>
       <c r="M29" s="3">
-        <f>(K29-I29)/K29</f>
+        <f t="shared" si="0"/>
         <v>0.10292142377434524</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
@@ -7925,11 +8172,11 @@
         <v>60.07</v>
       </c>
       <c r="M30" s="3">
-        <f>(K30-I30)/K30</f>
+        <f t="shared" si="0"/>
         <v>0.14189331646637143</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="e" vm="31">
         <v>#VALUE!</v>
       </c>
@@ -7976,11 +8223,11 @@
         <v>130.04</v>
       </c>
       <c r="M31" s="3">
-        <f>(K31-I31)/K31</f>
+        <f t="shared" si="0"/>
         <v>0.31564870601448652</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="e" vm="32">
         <v>#VALUE!</v>
       </c>
@@ -8027,7 +8274,7 @@
         <v>22.88</v>
       </c>
       <c r="M32" s="3">
-        <f>(K32-I32)/K32</f>
+        <f t="shared" si="0"/>
         <v>0.40864833675293299</v>
       </c>
     </row>
@@ -8048,28 +8295,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B40D47B-739C-4A46-AE44-24FC67F0C8A6}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7" max="10" width="11.42578125" style="1"/>
-    <col min="11" max="11" width="11.42578125" style="3"/>
-    <col min="12" max="13" width="11.42578125" style="1"/>
-    <col min="14" max="14" width="11.42578125" style="3"/>
-    <col min="15" max="16384" width="11.42578125" style="1"/>
+    <col min="4" max="4" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7" max="10" width="11.44140625" style="1"/>
+    <col min="11" max="11" width="11.44140625" style="3"/>
+    <col min="12" max="13" width="11.44140625" style="1"/>
+    <col min="14" max="14" width="11.44140625" style="3"/>
+    <col min="15" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8113,7 +8360,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="e" vm="33">
         <v>#VALUE!</v>
       </c>
@@ -8154,20 +8401,20 @@
         <f t="array" ref="K2">_FV(A2,"Change (%)",TRUE)</f>
         <v>-2.0031E-2</v>
       </c>
-      <c r="L2" s="2" cm="1">
-        <f t="array" ref="L2">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>54.75</v>
-      </c>
-      <c r="M2" s="2" cm="1">
-        <f t="array" ref="M2">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>22</v>
-      </c>
-      <c r="N2" s="3">
-        <f>(L2-J2)/L2</f>
-        <v>0.54429223744292243</v>
+      <c r="L2" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L2" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M2" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M2" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N2" s="3" t="e">
+        <f t="shared" ref="N2:N25" ca="1" si="0">(L2-J2)/L2</f>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
@@ -8207,20 +8454,20 @@
         <f t="array" ref="K3">_FV(A3,"Change (%)",TRUE)</f>
         <v>-5.0419999999999996E-3</v>
       </c>
-      <c r="L3" s="2" cm="1">
-        <f t="array" ref="L3">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>49.3</v>
-      </c>
-      <c r="M3" s="2" cm="1">
-        <f t="array" ref="M3">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>17.75</v>
-      </c>
-      <c r="N3" s="3">
-        <f>(L3-J3)/L3</f>
-        <v>0.31947261663286008</v>
+      <c r="L3" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L3" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M3" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M3" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N3" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="e" vm="35">
         <v>#VALUE!</v>
       </c>
@@ -8258,20 +8505,20 @@
         <f t="array" ref="K4">_FV(A4,"Change (%)",TRUE)</f>
         <v>-4.607E-3</v>
       </c>
-      <c r="L4" s="2" cm="1">
-        <f t="array" ref="L4">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>39.700000000000003</v>
-      </c>
-      <c r="M4" s="2" cm="1">
-        <f t="array" ref="M4">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>26.08</v>
-      </c>
-      <c r="N4" s="3">
-        <f>(L4-J4)/L4</f>
-        <v>0.23803526448362725</v>
+      <c r="L4" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L4" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M4" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M4" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N4" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="e" vm="36">
         <v>#VALUE!</v>
       </c>
@@ -8309,20 +8556,20 @@
         <f t="array" ref="K5">_FV(A5,"Change (%)",TRUE)</f>
         <v>1.4518E-2</v>
       </c>
-      <c r="L5" s="2" cm="1">
-        <f t="array" ref="L5">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>60.13</v>
-      </c>
-      <c r="M5" s="2" cm="1">
-        <f t="array" ref="M5">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>36.270000000000003</v>
-      </c>
-      <c r="N5" s="3">
-        <f>(L5-J5)/L5</f>
-        <v>0.22135373357724933</v>
+      <c r="L5" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L5" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M5" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M5" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N5" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="e" vm="37">
         <v>#VALUE!</v>
       </c>
@@ -8363,20 +8610,20 @@
         <f t="array" ref="K6">_FV(A6,"Change (%)",TRUE)</f>
         <v>-2.9670000000000002E-2</v>
       </c>
-      <c r="L6" s="2" cm="1">
-        <f t="array" ref="L6">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>35.72</v>
-      </c>
-      <c r="M6" s="2" cm="1">
-        <f t="array" ref="M6">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>17.95</v>
-      </c>
-      <c r="N6" s="3">
-        <f>(L6-J6)/L6</f>
-        <v>0.34994400895856664</v>
+      <c r="L6" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L6" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M6" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M6" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N6" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="e" vm="38">
         <v>#VALUE!</v>
       </c>
@@ -8417,20 +8664,20 @@
         <f t="array" ref="K7">_FV(A7,"Change (%)",TRUE)</f>
         <v>-1.8498000000000001E-2</v>
       </c>
-      <c r="L7" s="2" cm="1">
-        <f t="array" ref="L7">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>141.1</v>
-      </c>
-      <c r="M7" s="2" cm="1">
-        <f t="array" ref="M7">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>76.91</v>
-      </c>
-      <c r="N7" s="3">
-        <f>(L7-J7)/L7</f>
-        <v>0.30432317505315376</v>
+      <c r="L7" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L7" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M7" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M7" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N7" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="e" vm="39">
         <v>#VALUE!</v>
       </c>
@@ -8471,20 +8718,20 @@
         <f t="array" ref="K8">_FV(A8,"Change (%)",TRUE)</f>
         <v>-4.2915999999999996E-2</v>
       </c>
-      <c r="L8" s="2" cm="1">
-        <f t="array" ref="L8">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>54.05</v>
-      </c>
-      <c r="M8" s="2" cm="1">
-        <f t="array" ref="M8">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>9</v>
-      </c>
-      <c r="N8" s="3">
-        <f>(L8-J8)/L8</f>
-        <v>0.69879740980573535</v>
+      <c r="L8" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L8" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M8" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M8" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N8" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="e" vm="40">
         <v>#VALUE!</v>
       </c>
@@ -8524,20 +8771,20 @@
         <f t="array" ref="K9">_FV(A9,"Change (%)",TRUE)</f>
         <v>-1.1849E-2</v>
       </c>
-      <c r="L9" s="2" cm="1">
-        <f t="array" ref="L9">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>67.75</v>
-      </c>
-      <c r="M9" s="2" cm="1">
-        <f t="array" ref="M9">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>22.02</v>
-      </c>
-      <c r="N9" s="3">
-        <f>(L9-J9)/L9</f>
-        <v>0.37225092250922509</v>
+      <c r="L9" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L9" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M9" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M9" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N9" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="e" vm="41">
         <v>#VALUE!</v>
       </c>
@@ -8578,20 +8825,20 @@
         <f t="array" ref="K10">_FV(A10,"Change (%)",TRUE)</f>
         <v>-3.9191999999999998E-2</v>
       </c>
-      <c r="L10" s="2" cm="1">
-        <f t="array" ref="L10">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>67.13</v>
-      </c>
-      <c r="M10" s="2" cm="1">
-        <f t="array" ref="M10">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>20.84</v>
-      </c>
-      <c r="N10" s="3">
-        <f>(L10-J10)/L10</f>
-        <v>0.40473707731267683</v>
+      <c r="L10" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L10" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M10" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M10" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N10" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="e" vm="42">
         <v>#VALUE!</v>
       </c>
@@ -8632,20 +8879,20 @@
         <f t="array" ref="K11">_FV(A11,"Change (%)",TRUE)</f>
         <v>-1.7024999999999998E-2</v>
       </c>
-      <c r="L11" s="2" cm="1">
-        <f t="array" ref="L11">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>64.33</v>
-      </c>
-      <c r="M11" s="2" cm="1">
-        <f t="array" ref="M11">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>21.254999999999999</v>
-      </c>
-      <c r="N11" s="3">
-        <f>(L11-J11)/L11</f>
-        <v>0.48841908907197268</v>
+      <c r="L11" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L11" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M11" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M11" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N11" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="e" vm="43">
         <v>#VALUE!</v>
       </c>
@@ -8686,20 +8933,20 @@
         <f t="array" ref="K12">_FV(A12,"Change (%)",TRUE)</f>
         <v>-1.7163999999999999E-2</v>
       </c>
-      <c r="L12" s="2" cm="1">
-        <f t="array" ref="L12">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>76.05</v>
-      </c>
-      <c r="M12" s="2" cm="1">
-        <f t="array" ref="M12">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>30.11</v>
-      </c>
-      <c r="N12" s="3">
-        <f>(L12-J12)/L12</f>
-        <v>0.42774490466798154</v>
+      <c r="L12" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L12" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M12" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M12" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N12" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="e" vm="44">
         <v>#VALUE!</v>
       </c>
@@ -8740,20 +8987,20 @@
         <f t="array" ref="K13">_FV(A13,"Change (%)",TRUE)</f>
         <v>-1.9618E-2</v>
       </c>
-      <c r="L13" s="2" cm="1">
-        <f t="array" ref="L13">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>101.99</v>
-      </c>
-      <c r="M13" s="2" cm="1">
-        <f t="array" ref="M13">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>31</v>
-      </c>
-      <c r="N13" s="3">
-        <f>(L13-J13)/L13</f>
-        <v>0.45612314932836551</v>
+      <c r="L13" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L13" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M13" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M13" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N13" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="e" vm="45">
         <v>#VALUE!</v>
       </c>
@@ -8794,20 +9041,20 @@
         <f t="array" ref="K14">_FV(A14,"Change (%)",TRUE)</f>
         <v>-1.3241000000000001E-2</v>
       </c>
-      <c r="L14" s="2" cm="1">
-        <f t="array" ref="L14">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>127</v>
-      </c>
-      <c r="M14" s="2" cm="1">
-        <f t="array" ref="M14">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>51.6</v>
-      </c>
-      <c r="N14" s="3">
-        <f>(L14-J14)/L14</f>
-        <v>0.31346456692913388</v>
+      <c r="L14" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L14" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M14" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M14" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N14" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="e" vm="46">
         <v>#VALUE!</v>
       </c>
@@ -8848,20 +9095,20 @@
         <f t="array" ref="K15">_FV(A15,"Change (%)",TRUE)</f>
         <v>-2.1968000000000001E-2</v>
       </c>
-      <c r="L15" s="2" cm="1">
-        <f t="array" ref="L15">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>53.13</v>
-      </c>
-      <c r="M15" s="2" cm="1">
-        <f t="array" ref="M15">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>13.74</v>
-      </c>
-      <c r="N15" s="3">
-        <f>(L15-J15)/L15</f>
-        <v>0.42179559570863923</v>
+      <c r="L15" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L15" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M15" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M15" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N15" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="e" vm="47">
         <v>#VALUE!</v>
       </c>
@@ -8902,20 +9149,20 @@
         <f t="array" ref="K16">_FV(A16,"Change (%)",TRUE)</f>
         <v>-2.0518999999999999E-2</v>
       </c>
-      <c r="L16" s="2" cm="1">
-        <f t="array" ref="L16">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>74.290000000000006</v>
-      </c>
-      <c r="M16" s="2" cm="1">
-        <f t="array" ref="M16">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>33.299999999999997</v>
-      </c>
-      <c r="N16" s="3">
-        <f>(L16-J16)/L16</f>
-        <v>0.34459550410553247</v>
+      <c r="L16" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L16" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M16" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M16" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N16" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="e" vm="48">
         <v>#VALUE!</v>
       </c>
@@ -8956,20 +9203,20 @@
         <f t="array" ref="K17">_FV(A17,"Change (%)",TRUE)</f>
         <v>-2.9287000000000001E-2</v>
       </c>
-      <c r="L17" s="2" cm="1">
-        <f t="array" ref="L17">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>59.52</v>
-      </c>
-      <c r="M17" s="2" cm="1">
-        <f t="array" ref="M17">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>8.75</v>
-      </c>
-      <c r="N17" s="3">
-        <f>(L17-J17)/L17</f>
-        <v>0.65473790322580638</v>
+      <c r="L17" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L17" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M17" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M17" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N17" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="e" vm="49">
         <v>#VALUE!</v>
       </c>
@@ -9010,20 +9257,20 @@
         <f t="array" ref="K18">_FV(A18,"Change (%)",TRUE)</f>
         <v>-1.4047E-2</v>
       </c>
-      <c r="L18" s="2" cm="1">
-        <f t="array" ref="L18">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>28.504999999999999</v>
-      </c>
-      <c r="M18" s="2" cm="1">
-        <f t="array" ref="M18">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>11.290100000000001</v>
-      </c>
-      <c r="N18" s="3">
-        <f>(L18-J18)/L18</f>
-        <v>0.48289773723908086</v>
+      <c r="L18" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L18" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M18" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M18" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N18" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="e" vm="50">
         <v>#VALUE!</v>
       </c>
@@ -9064,20 +9311,20 @@
         <f t="array" ref="K19">_FV(A19,"Change (%)",TRUE)</f>
         <v>-7.9430000000000004E-3</v>
       </c>
-      <c r="L19" s="2" cm="1">
-        <f t="array" ref="L19">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>29.44</v>
-      </c>
-      <c r="M19" s="2" cm="1">
-        <f t="array" ref="M19">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>19.38</v>
-      </c>
-      <c r="N19" s="3">
-        <f>(L19-J19)/L19</f>
-        <v>0.10903532608695654</v>
+      <c r="L19" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L19" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M19" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M19" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N19" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="e" vm="51">
         <v>#VALUE!</v>
       </c>
@@ -9118,20 +9365,20 @@
         <f t="array" ref="K20">_FV(A20,"Change (%)",TRUE)</f>
         <v>-8.6169999999999997E-3</v>
       </c>
-      <c r="L20" s="2" cm="1">
-        <f t="array" ref="L20">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>53.81</v>
-      </c>
-      <c r="M20" s="2" cm="1">
-        <f t="array" ref="M20">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>19.989999999999998</v>
-      </c>
-      <c r="N20" s="3">
-        <f>(L20-J20)/L20</f>
-        <v>0.14476863036610294</v>
+      <c r="L20" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L20" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M20" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M20" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N20" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="e" vm="52">
         <v>#VALUE!</v>
       </c>
@@ -9172,20 +9419,20 @@
         <f t="array" ref="K21">_FV(A21,"Change (%)",TRUE)</f>
         <v>-8.8000000000000005E-3</v>
       </c>
-      <c r="L21" s="2" cm="1">
-        <f t="array" ref="L21">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>108.58</v>
-      </c>
-      <c r="M21" s="2" cm="1">
-        <f t="array" ref="M21">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>49.680999999999997</v>
-      </c>
-      <c r="N21" s="3">
-        <f>(L21-J21)/L21</f>
-        <v>0.19082703997052863</v>
+      <c r="L21" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L21" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M21" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M21" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N21" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="e" vm="53">
         <v>#VALUE!</v>
       </c>
@@ -9226,20 +9473,20 @@
         <f t="array" ref="K22">_FV(A22,"Change (%)",TRUE)</f>
         <v>-6.783E-3</v>
       </c>
-      <c r="L22" s="2" cm="1">
-        <f t="array" ref="L22">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>49.8</v>
-      </c>
-      <c r="M22" s="2" cm="1">
-        <f t="array" ref="M22">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>13.46</v>
-      </c>
-      <c r="N22" s="3">
-        <f>(L22-J22)/L22</f>
-        <v>0.1767068273092369</v>
+      <c r="L22" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L22" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M22" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M22" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N22" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="e" vm="54">
         <v>#VALUE!</v>
       </c>
@@ -9280,20 +9527,20 @@
         <f t="array" ref="K23">_FV(A23,"Change (%)",TRUE)</f>
         <v>-2.65E-3</v>
       </c>
-      <c r="L23" s="2" cm="1">
-        <f t="array" ref="L23">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>45.24</v>
-      </c>
-      <c r="M23" s="2" cm="1">
-        <f t="array" ref="M23">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>14.52</v>
-      </c>
-      <c r="N23" s="3">
-        <f>(L23-J23)/L23</f>
-        <v>0.50088417329796642</v>
+      <c r="L23" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L23" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M23" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M23" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N23" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="e" vm="55">
         <v>#VALUE!</v>
       </c>
@@ -9334,20 +9581,20 @@
         <f t="array" ref="K24">_FV(A24,"Change (%)",TRUE)</f>
         <v>-3.0919999999999997E-3</v>
       </c>
-      <c r="L24" s="2" cm="1">
-        <f t="array" ref="L24">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>99.72</v>
-      </c>
-      <c r="M24" s="2" cm="1">
-        <f t="array" ref="M24">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>50.02</v>
-      </c>
-      <c r="N24" s="3">
-        <f>(L24-J24)/L24</f>
-        <v>0.25631768953068595</v>
+      <c r="L24" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L24" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M24" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M24" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N24" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="e" vm="56">
         <v>#VALUE!</v>
       </c>
@@ -9388,17 +9635,62 @@
         <f t="array" ref="K25">_FV(A25,"Change (%)",TRUE)</f>
         <v>1.1489000000000001E-2</v>
       </c>
-      <c r="L25" s="2" cm="1">
-        <f t="array" ref="L25">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
-        <v>144.94</v>
-      </c>
-      <c r="M25" s="2" cm="1">
-        <f t="array" ref="M25">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
-        <v>60</v>
-      </c>
-      <c r="N25" s="3">
-        <f>(L25-J25)/L25</f>
-        <v>3.7946736580654851E-3</v>
+      <c r="L25" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="L25" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M25" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="M25" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N25" s="3" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="e" vm="57">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B26" s="4" t="e">
+        <f t="array" aca="1" ref="B26" ca="1">_FV(A26,"Ticker symbol",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F26" s="3" t="e">
+        <f t="array" aca="1" ref="F26" ca="1">_FV(A26,"Industry")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G26" s="2" t="e">
+        <f t="array" aca="1" ref="G26" ca="1">_FV(A26,"Open")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H26" s="2" t="e">
+        <f t="array" aca="1" ref="H26" ca="1">_FV(A26,"High")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="I26" s="2" t="e">
+        <f t="array" aca="1" ref="I26" ca="1">_FV(A26,"Low")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="J26" s="2" t="e">
+        <f t="array" aca="1" ref="J26" ca="1">_FV(A26,"Price")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K26" s="3" t="e">
+        <f t="array" aca="1" ref="K26" ca="1">_FV(A26,"Change (%)",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L26" s="2" t="e">
+        <f t="array" aca="1" ref="L26" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M26" s="2" t="e">
+        <f t="array" aca="1" ref="M26" ca="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N26" s="3" t="e">
+        <f ca="1">(L26-J26)/L26</f>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
@@ -9424,24 +9716,24 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" style="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="17.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="67.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="61.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" style="1" customWidth="1"/>
+    <col min="7" max="9" width="9.109375" style="1"/>
+    <col min="10" max="10" width="17.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="67.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
@@ -9464,7 +9756,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -9489,7 +9781,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -9514,7 +9806,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -9544,7 +9836,7 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -9574,7 +9866,7 @@
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -9599,7 +9891,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -9624,7 +9916,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -9649,7 +9941,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -9674,7 +9966,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -9699,7 +9991,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -9724,7 +10016,7 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>56</v>
       </c>
@@ -9746,7 +10038,7 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>2</v>
       </c>
@@ -9766,7 +10058,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -9788,7 +10080,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -9810,7 +10102,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -9832,7 +10124,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -9854,7 +10146,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
@@ -9876,7 +10168,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -9898,7 +10190,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
@@ -9920,7 +10212,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>56</v>
       </c>
@@ -9949,12 +10241,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D95AC4467A64E54FAB628610D0FE135F" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="79e84842eaddaeb917644b39e1597e3c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e8f9595b-0d5a-46b2-8488-c972c1ea4246" xmlns:ns4="6bcbbac3-d60f-4c54-b2b4-d245c065548d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb8f6ae9099bbec0b468ebfdbf5b501b" ns3:_="" ns4:_="">
     <xsd:import namespace="e8f9595b-0d5a-46b2-8488-c972c1ea4246"/>
@@ -10177,6 +10463,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -10187,13 +10479,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401ADED5-CC5A-4072-B36A-6DA217C5A368}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11321DBA-FDAB-45E8-A045-E3E44A7AE235}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e8f9595b-0d5a-46b2-8488-c972c1ea4246"/>
+    <ds:schemaRef ds:uri="6bcbbac3-d60f-4c54-b2b4-d245c065548d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11321DBA-FDAB-45E8-A045-E3E44A7AE235}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401ADED5-CC5A-4072-B36A-6DA217C5A368}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DB5870C-189D-475E-8E58-449C30115ACA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DB5870C-189D-475E-8E58-449C30115ACA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added international etf to watchlist
</commit_message>
<xml_diff>
--- a/input/Watchlist.xlsx
+++ b/input/Watchlist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssoma\OneDrive - Bayer\Personal Data\Analytics\us-stocks-analysis\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bayergroup-my.sharepoint.com/personal/sivacharan_chandrasekar_ext_bayer_com/Documents/Personal Data/Analytics/us-stocks-analysis/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A259AFBD-2F1F-43A4-8040-58927886A03B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{A259AFBD-2F1F-43A4-8040-58927886A03B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{9270F764-42D1-4F89-B58A-37580100E994}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fund List" sheetId="1" r:id="rId1"/>
@@ -763,7 +763,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1563" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="427">
   <si>
     <t>Funds</t>
   </si>
@@ -1926,12 +1926,6 @@
     <t>Bond</t>
   </si>
   <si>
-    <t>AGG</t>
-  </si>
-  <si>
-    <t>BND</t>
-  </si>
-  <si>
     <t>FNBGX</t>
   </si>
   <si>
@@ -2016,9 +2010,6 @@
     <t>Retirement</t>
   </si>
   <si>
-    <t>QQQ</t>
-  </si>
-  <si>
     <t>ARKK, ARKW</t>
   </si>
   <si>
@@ -2032,6 +2023,27 @@
   </si>
   <si>
     <t>FUAMX</t>
+  </si>
+  <si>
+    <t>EFG</t>
+  </si>
+  <si>
+    <t>SPEM</t>
+  </si>
+  <si>
+    <t>SCHE</t>
+  </si>
+  <si>
+    <t>ACWX</t>
+  </si>
+  <si>
+    <t>IMTM, EFG</t>
+  </si>
+  <si>
+    <t>FLTW, FLSW</t>
+  </si>
+  <si>
+    <t>https://money.usnews.com/funds/etfs/international-stock</t>
   </si>
 </sst>
 </file>
@@ -2133,7 +2145,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2191,6 +2203,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2275,7 +2293,7 @@
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2427,6 +2445,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -8401,7 +8420,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>3</v>
@@ -8422,7 +8441,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="81" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="L1" s="19" t="s">
         <v>9</v>
@@ -8449,7 +8468,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>14</v>
@@ -8507,7 +8526,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
@@ -8565,7 +8584,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -8623,7 +8642,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -8681,7 +8700,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>14</v>
@@ -8739,7 +8758,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>15</v>
@@ -8797,7 +8816,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>15</v>
@@ -8855,7 +8874,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>15</v>
@@ -8913,7 +8932,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>15</v>
@@ -8971,7 +8990,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>16</v>
@@ -9029,7 +9048,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>16</v>
@@ -9087,7 +9106,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>16</v>
@@ -9145,7 +9164,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>16</v>
@@ -9203,7 +9222,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
@@ -9261,7 +9280,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>16</v>
@@ -9319,10 +9338,10 @@
         <v>13</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -9377,10 +9396,10 @@
         <v>13</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="0"/>
@@ -9435,10 +9454,10 @@
         <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="0"/>
@@ -9493,10 +9512,10 @@
         <v>13</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="0"/>
@@ -9551,10 +9570,10 @@
         <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="0"/>
@@ -9609,10 +9628,10 @@
         <v>13</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="0"/>
@@ -9667,10 +9686,10 @@
         <v>13</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F23" s="3" t="str">
         <f t="shared" si="0"/>
@@ -9725,10 +9744,10 @@
         <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="0"/>
@@ -9783,10 +9802,10 @@
         <v>13</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="0"/>
@@ -9841,10 +9860,10 @@
         <v>13</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="0"/>
@@ -9899,7 +9918,7 @@
         <v>13</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>17</v>
@@ -9957,7 +9976,7 @@
         <v>13</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>17</v>
@@ -10015,7 +10034,7 @@
         <v>13</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>18</v>
@@ -10073,7 +10092,7 @@
         <v>13</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>18</v>
@@ -10131,7 +10150,7 @@
         <v>13</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>18</v>
@@ -10189,7 +10208,7 @@
         <v>13</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>19</v>
@@ -10247,7 +10266,7 @@
         <v>13</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>19</v>
@@ -10305,7 +10324,7 @@
         <v>13</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>20</v>
@@ -10363,7 +10382,7 @@
         <v>13</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>20</v>
@@ -10421,7 +10440,7 @@
         <v>13</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>20</v>
@@ -10479,7 +10498,7 @@
         <v>13</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>20</v>
@@ -10537,7 +10556,7 @@
         <v>13</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>20</v>
@@ -10595,7 +10614,7 @@
         <v>13</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>20</v>
@@ -10653,7 +10672,7 @@
         <v>13</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>20</v>
@@ -10711,7 +10730,7 @@
         <v>13</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>20</v>
@@ -10769,7 +10788,7 @@
         <v>13</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>21</v>
@@ -10827,7 +10846,7 @@
         <v>13</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>21</v>
@@ -10885,7 +10904,7 @@
         <v>13</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>386</v>
@@ -10943,7 +10962,7 @@
         <v>13</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>386</v>
@@ -11001,7 +11020,7 @@
         <v>13</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>386</v>
@@ -17323,7 +17342,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D2" s="3">
         <v>0.09</v>
@@ -17345,7 +17364,7 @@
         <v>321</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D3" s="3">
         <v>0.09</v>
@@ -17367,7 +17386,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D4" s="3">
         <v>0.18</v>
@@ -17389,7 +17408,7 @@
         <v>322</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D5" s="3">
         <v>0.12</v>
@@ -17411,7 +17430,7 @@
         <v>323</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D6" s="3">
         <v>8.4000000000000005E-2</v>
@@ -17455,7 +17474,7 @@
         <v>326</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D8" s="3">
         <v>0.09</v>
@@ -17477,7 +17496,7 @@
         <v>327</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D9" s="3">
         <v>0.18</v>
@@ -17499,7 +17518,7 @@
         <v>328</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D10" s="3">
         <v>0.08</v>
@@ -17521,7 +17540,7 @@
         <v>329</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D11" s="3">
         <v>0.05</v>
@@ -17576,7 +17595,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>21</v>
@@ -17598,7 +17617,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>321</v>
@@ -17620,7 +17639,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>20</v>
@@ -17642,7 +17661,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>322</v>
@@ -17664,7 +17683,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>323</v>
@@ -17686,7 +17705,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>336</v>
@@ -17708,7 +17727,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>338</v>
@@ -17871,11 +17890,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9442434-AE3F-49F6-94ED-A6D1C7BB92DA}">
-  <dimension ref="A1:AK27"/>
+  <dimension ref="A1:AK36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="12.75" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -18149,7 +18168,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C3" s="48">
         <v>1.4999999999999999E-4</v>
@@ -18216,68 +18235,68 @@
         <v>21</v>
       </c>
       <c r="U3" s="47" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="V3" s="48">
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="W3" s="48">
-        <v>0.11409999999999999</v>
+        <v>0.1368</v>
       </c>
       <c r="X3" s="49">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="Y3" s="50">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="Z3" s="50">
         <f t="shared" ref="Z3:Z23" si="8">Y3*12</f>
-        <v>600</v>
+        <v>540</v>
       </c>
       <c r="AA3" s="51">
         <f t="shared" ref="AA3:AJ3" si="9">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y3*12*(1+$W3)) - ($Y3*12*(1+$W3))*$V3, (Z3+($Y3*12))*(1+$W3) - (Z3+($Y3*12))*(1+$W3)*$V3)</f>
-        <v>668.35973100000001</v>
+        <v>613.77991920000011</v>
       </c>
       <c r="AB3" s="51">
         <f t="shared" si="9"/>
-        <v>1412.8676143706541</v>
+        <v>1311.4202695947383</v>
       </c>
       <c r="AC3" s="51">
         <f t="shared" si="9"/>
-        <v>2242.1994287989705</v>
+        <v>2104.3788582909269</v>
       </c>
       <c r="AD3" s="51">
         <f t="shared" si="9"/>
-        <v>3166.0194094673893</v>
+        <v>3005.6789666222103</v>
       </c>
       <c r="AE3" s="51">
         <f t="shared" si="9"/>
-        <v>4195.0928657540062</v>
+        <v>4030.1232400787403</v>
       </c>
       <c r="AF3" s="51">
         <f t="shared" si="9"/>
-        <v>5341.4116297922783</v>
+        <v>5194.5368019066145</v>
       </c>
       <c r="AG3" s="51">
         <f t="shared" si="9"/>
-        <v>6618.3337977470646</v>
+        <v>6518.0435831919785</v>
       </c>
       <c r="AH3" s="51">
         <f t="shared" si="9"/>
-        <v>8040.7393922173942</v>
+        <v>8022.3804077808354</v>
       </c>
       <c r="AI3" s="51">
         <f t="shared" si="9"/>
-        <v>9625.2037597058679</v>
+        <v>9732.2539904581172</v>
       </c>
       <c r="AJ3" s="51">
         <f t="shared" si="9"/>
-        <v>11390.190723762005</v>
+        <v>11675.746711602334</v>
       </c>
       <c r="AK3" s="51">
         <f t="shared" ref="AK3:AK23" si="10">Z3*10</f>
-        <v>6000</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.2">
@@ -18358,62 +18377,62 @@
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="W4" s="35">
-        <v>0.1113</v>
+        <v>0.13550000000000001</v>
       </c>
       <c r="X4" s="36">
-        <v>2.5000000000000001E-2</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="Y4" s="37">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>22.5</v>
       </c>
       <c r="Z4" s="37">
         <f t="shared" si="8"/>
-        <v>300</v>
+        <v>270</v>
       </c>
       <c r="AA4" s="38">
         <f t="shared" ref="AA4:AJ4" si="12">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y4*12*(1+$W4)) - ($Y4*12*(1+$W4))*$V4, (Z4+($Y4*12))*(1+$W4) - (Z4+($Y4*12))*(1+$W4)*$V4)</f>
-        <v>333.28998300000001</v>
+        <v>306.49302449999999</v>
       </c>
       <c r="AB4" s="38">
         <f t="shared" si="12"/>
-        <v>703.5640255604676</v>
+        <v>654.4114469709541</v>
       </c>
       <c r="AC4" s="38">
         <f t="shared" si="12"/>
-        <v>1114.926123394866</v>
+        <v>1049.3542972761077</v>
       </c>
       <c r="AD4" s="38">
         <f t="shared" si="12"/>
-        <v>1571.9356787084357</v>
+        <v>1497.6773665156531</v>
       </c>
       <c r="AE4" s="38">
         <f t="shared" si="12"/>
-        <v>2079.65803511276</v>
+        <v>2006.5954903836207</v>
       </c>
       <c r="AF4" s="38">
         <f t="shared" si="12"/>
-        <v>2643.7206202284838</v>
+        <v>2584.2986570768026</v>
       </c>
       <c r="AG4" s="38">
         <f t="shared" si="12"/>
-        <v>3270.3753182423357</v>
+        <v>3240.0838082731761</v>
       </c>
       <c r="AH4" s="38">
         <f t="shared" si="12"/>
-        <v>3966.5677637353588</v>
+        <v>3984.5044542449032</v>
       </c>
       <c r="AI4" s="38">
         <f t="shared" si="12"/>
-        <v>4740.0143248123513</v>
+        <v>4829.5405108527493</v>
       </c>
       <c r="AJ4" s="38">
         <f t="shared" si="12"/>
-        <v>5599.2876287882173</v>
+        <v>5788.7910915982748</v>
       </c>
       <c r="AK4" s="38">
         <f t="shared" si="10"/>
-        <v>3000</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.2">
@@ -18494,62 +18513,62 @@
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="W5" s="35">
-        <v>0.113</v>
+        <v>0.13</v>
       </c>
       <c r="X5" s="36">
-        <v>2.5000000000000001E-2</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="Y5" s="37">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>22.5</v>
       </c>
       <c r="Z5" s="37">
         <f t="shared" si="8"/>
-        <v>300</v>
+        <v>270</v>
       </c>
       <c r="AA5" s="38">
         <f t="shared" ref="AA5:AJ5" si="14">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y5*12*(1+$W5)) - ($Y5*12*(1+$W5))*$V5, (Z5+($Y5*12))*(1+$W5) - (Z5+($Y5*12))*(1+$W5)*$V5)</f>
-        <v>333.79982999999999</v>
+        <v>305.00846999999999</v>
       </c>
       <c r="AB5" s="38">
         <f t="shared" si="14"/>
-        <v>705.20758502676301</v>
+        <v>649.56464322866987</v>
       </c>
       <c r="AC5" s="38">
         <f t="shared" si="14"/>
-        <v>1118.4604033221469</v>
+        <v>1038.7963144343423</v>
       </c>
       <c r="AD5" s="38">
         <f t="shared" si="14"/>
-        <v>1578.2728049688803</v>
+        <v>1478.4961533602136</v>
       </c>
       <c r="AE5" s="38">
         <f t="shared" si="14"/>
-        <v>2089.8904766407845</v>
+        <v>1975.2079131010521</v>
       </c>
       <c r="AF5" s="38">
         <f t="shared" si="14"/>
-        <v>2659.1501160710427</v>
+        <v>2536.3238163216479</v>
       </c>
       <c r="AG5" s="38">
         <f t="shared" si="14"/>
-        <v>3292.5460189633141</v>
+        <v>3170.1945686697286</v>
       </c>
       <c r="AH5" s="38">
         <f t="shared" si="14"/>
-        <v>3997.3041679904363</v>
+        <v>3886.2536366380136</v>
       </c>
       <c r="AI5" s="38">
         <f t="shared" si="14"/>
-        <v>4781.4646691116632</v>
+        <v>4695.1576394181347</v>
       </c>
       <c r="AJ5" s="38">
         <f t="shared" si="14"/>
-        <v>5653.9734756682647</v>
+        <v>5608.9449441027291</v>
       </c>
       <c r="AK5" s="38">
         <f t="shared" si="10"/>
-        <v>3000</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
@@ -18557,7 +18576,7 @@
         <v>321</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C6" s="35">
         <v>1.4999999999999999E-4</v>
@@ -18624,68 +18643,68 @@
         <v>321</v>
       </c>
       <c r="U6" s="23" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="V6" s="35">
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="W6" s="35">
-        <v>0.1164</v>
+        <v>0.13969999999999999</v>
       </c>
       <c r="X6" s="36">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="Y6" s="37">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="Z6" s="37">
         <f t="shared" si="8"/>
-        <v>600</v>
+        <v>540</v>
       </c>
       <c r="AA6" s="38">
         <f t="shared" ref="AA6:AJ6" si="16">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y6*12*(1+$W6)) - ($Y6*12*(1+$W6))*$V6, (Z6+($Y6*12))*(1+$W6) - (Z6+($Y6*12))*(1+$W6)*$V6)</f>
-        <v>669.73952400000007</v>
+        <v>615.34568430000002</v>
       </c>
       <c r="AB6" s="38">
         <f t="shared" si="16"/>
-        <v>1417.3245740129112</v>
+        <v>1316.5499642752502</v>
       </c>
       <c r="AC6" s="38">
         <f t="shared" si="16"/>
-        <v>2251.8033332548498</v>
+        <v>2115.5926077853596</v>
       </c>
       <c r="AD6" s="38">
         <f t="shared" si="16"/>
-        <v>3183.2756782595275</v>
+        <v>3026.1249082587101</v>
       </c>
       <c r="AE6" s="38">
         <f t="shared" si="16"/>
-        <v>4223.0154198638547</v>
+        <v>4063.7029110587605</v>
       </c>
       <c r="AF6" s="38">
         <f t="shared" si="16"/>
-        <v>5383.6067525737972</v>
+        <v>5246.0531817025094</v>
       </c>
       <c r="AG6" s="38">
         <f t="shared" si="16"/>
-        <v>6679.0965637866011</v>
+        <v>6593.3756564646719</v>
       </c>
       <c r="AH6" s="38">
         <f t="shared" si="16"/>
-        <v>8125.1644463007906</v>
+        <v>8128.688749437435</v>
       </c>
       <c r="AI6" s="38">
         <f t="shared" si="16"/>
-        <v>9739.3124718120253</v>
+        <v>9878.2226120486848</v>
       </c>
       <c r="AJ6" s="38">
         <f t="shared" si="16"/>
-        <v>11541.077022264415</v>
+        <v>11871.867263705242</v>
       </c>
       <c r="AK6" s="38">
         <f t="shared" si="10"/>
-        <v>6000</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.2">
@@ -18766,62 +18785,62 @@
         <v>1E-3</v>
       </c>
       <c r="W7" s="48">
-        <v>0.1716</v>
+        <v>0.193</v>
       </c>
       <c r="X7" s="49">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="Y7" s="50">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="Z7" s="50">
         <f t="shared" si="8"/>
-        <v>1200</v>
+        <v>1080</v>
       </c>
       <c r="AA7" s="51">
         <f t="shared" ref="AA7:AJ7" si="18">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y7*12*(1+$W7)) - ($Y7*12*(1+$W7))*$V7, (Z7+($Y7*12))*(1+$W7) - (Z7+($Y7*12))*(1+$W7)*$V7)</f>
-        <v>1404.5140800000001</v>
+        <v>1287.15156</v>
       </c>
       <c r="AB7" s="51">
         <f t="shared" si="18"/>
-        <v>3048.3972474318721</v>
+        <v>2821.1877992689206</v>
       </c>
       <c r="AC7" s="51">
         <f t="shared" si="18"/>
-        <v>4972.444792876091</v>
+        <v>4649.4629274832942</v>
       </c>
       <c r="AD7" s="51">
         <f t="shared" si="18"/>
-        <v>7224.4046830142943</v>
+        <v>6828.4140232150821</v>
       </c>
       <c r="AE7" s="51">
         <f t="shared" si="18"/>
-        <v>9860.1624940929269</v>
+        <v>9425.3031917658973</v>
       </c>
       <c r="AF7" s="51">
         <f t="shared" si="18"/>
-        <v>12945.128291701194</v>
+        <v>12520.293881068939</v>
       </c>
       <c r="AG7" s="51">
         <f t="shared" si="18"/>
-        <v>16555.85987425056</v>
+        <v>16208.925449515129</v>
       </c>
       <c r="AH7" s="51">
         <f t="shared" si="18"/>
-        <v>20781.962663243285</v>
+        <v>20605.062373210279</v>
       </c>
       <c r="AI7" s="51">
         <f t="shared" si="18"/>
-        <v>25728.313388799575</v>
+        <v>25844.409131828626</v>
       </c>
       <c r="AJ7" s="51">
         <f t="shared" si="18"/>
-        <v>31517.662754351266</v>
+        <v>32088.699274177281</v>
       </c>
       <c r="AK7" s="51">
         <f t="shared" si="10"/>
-        <v>12000</v>
+        <v>10800</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.2">
@@ -18902,62 +18921,62 @@
         <v>8.4000000000000003E-4</v>
       </c>
       <c r="W8" s="48">
-        <v>0.16980000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="X8" s="49">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="Y8" s="50">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="Z8" s="50">
         <f t="shared" si="8"/>
-        <v>1200</v>
+        <v>1080</v>
       </c>
       <c r="AA8" s="51">
         <f t="shared" ref="AA8:AJ8" si="20">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y8*12*(1+$W8)) - ($Y8*12*(1+$W8))*$V8, (Z8+($Y8*12))*(1+$W8) - (Z8+($Y8*12))*(1+$W8)*$V8)</f>
-        <v>1402.5808416</v>
+        <v>1294.9113600000001</v>
       </c>
       <c r="AB8" s="51">
         <f t="shared" si="20"/>
-        <v>3041.9416892861368</v>
+        <v>2847.4997213491197</v>
       </c>
       <c r="AC8" s="51">
         <f t="shared" si="20"/>
-        <v>4958.0551204808962</v>
+        <v>4709.0407458998234</v>
       </c>
       <c r="AD8" s="51">
         <f t="shared" si="20"/>
-        <v>7197.6417779194044</v>
+        <v>6941.0135420079214</v>
       </c>
       <c r="AE8" s="51">
         <f t="shared" si="20"/>
-        <v>9815.3095602745998</v>
+        <v>9617.1310687591613</v>
       </c>
       <c r="AF8" s="51">
         <f t="shared" si="20"/>
-        <v>12874.885127945394</v>
+        <v>12825.774574393685</v>
       </c>
       <c r="AG8" s="51">
         <f t="shared" si="20"/>
-        <v>16450.97019014748</v>
+        <v>16672.912468501432</v>
       </c>
       <c r="AH8" s="51">
         <f t="shared" si="20"/>
-        <v>20630.760520294636</v>
+        <v>21285.600026433469</v>
       </c>
       <c r="AI8" s="51">
         <f t="shared" si="20"/>
-        <v>25516.172052769089</v>
+        <v>26816.175506893516</v>
       </c>
       <c r="AJ8" s="51">
         <f t="shared" si="20"/>
-        <v>31226.325901752723</v>
+        <v>33447.291263361272</v>
       </c>
       <c r="AK8" s="51">
         <f t="shared" si="10"/>
-        <v>12000</v>
+        <v>10800</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.2">
@@ -19038,7 +19057,7 @@
         <v>1E-3</v>
       </c>
       <c r="W9" s="35">
-        <v>0.13320000000000001</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="X9" s="36">
         <v>4.2000000000000003E-2</v>
@@ -19053,43 +19072,43 @@
       </c>
       <c r="AA9" s="38">
         <f t="shared" ref="AA9:AJ9" si="22">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y9*12*(1+$W9)) - ($Y9*12*(1+$W9))*$V9, (Z9+($Y9*12))*(1+$W9) - (Z9+($Y9*12))*(1+$W9)*$V9)</f>
-        <v>570.56166719999999</v>
+        <v>587.07633599999997</v>
       </c>
       <c r="AB9" s="38">
         <f t="shared" si="22"/>
-        <v>1216.4755879897691</v>
+        <v>1270.922812768224</v>
       </c>
       <c r="AC9" s="38">
         <f t="shared" si="22"/>
-        <v>1947.6932933736962</v>
+        <v>2067.4904396880611</v>
       </c>
       <c r="AD9" s="38">
         <f t="shared" si="22"/>
-        <v>2775.4805812110217</v>
+        <v>2995.3594948236027</v>
       </c>
       <c r="AE9" s="38">
         <f t="shared" si="22"/>
-        <v>3712.5910872337013</v>
+        <v>4076.1729177933562</v>
       </c>
       <c r="AF9" s="38">
         <f t="shared" si="22"/>
-        <v>4773.462779033176</v>
+        <v>5335.1411405249055</v>
       </c>
       <c r="AG9" s="38">
         <f t="shared" si="22"/>
-        <v>5974.4404003791942</v>
+        <v>6801.630131282187</v>
       </c>
       <c r="AH9" s="38">
         <f t="shared" si="22"/>
-        <v>7334.0272930479932</v>
+        <v>8509.8463683419559</v>
       </c>
       <c r="AI9" s="38">
         <f t="shared" si="22"/>
-        <v>8873.1704759535023</v>
+        <v>10499.634720621234</v>
       </c>
       <c r="AJ9" s="38">
         <f t="shared" si="22"/>
-        <v>10615.583373767158</v>
+        <v>12817.407846160113</v>
       </c>
       <c r="AK9" s="38">
         <f t="shared" si="10"/>
@@ -19174,7 +19193,7 @@
         <v>8.4000000000000003E-4</v>
       </c>
       <c r="W10" s="35">
-        <v>0.13827</v>
+        <v>0.16</v>
       </c>
       <c r="X10" s="36">
         <v>4.2000000000000003E-2</v>
@@ -19189,43 +19208,43 @@
       </c>
       <c r="AA10" s="38">
         <f t="shared" ref="AA10:AJ10" si="24">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y10*12*(1+$W10)) - ($Y10*12*(1+$W10))*$V10, (Z10+($Y10*12))*(1+$W10) - (Z10+($Y10*12))*(1+$W10)*$V10)</f>
-        <v>573.2061820127999</v>
+        <v>584.1489024</v>
       </c>
       <c r="AB10" s="38">
         <f t="shared" si="24"/>
-        <v>1225.1215135558377</v>
+        <v>1261.1924344935012</v>
       </c>
       <c r="AC10" s="38">
         <f t="shared" si="24"/>
-        <v>1966.5538512332055</v>
+        <v>2045.9032205042906</v>
       </c>
       <c r="AD10" s="38">
         <f t="shared" si="24"/>
-        <v>2809.7951200841362</v>
+        <v>2955.403110086917</v>
       </c>
       <c r="AE10" s="38">
         <f t="shared" si="24"/>
-        <v>3768.8250967382451</v>
+        <v>4009.5367653103549</v>
       </c>
       <c r="AF10" s="38">
         <f t="shared" si="24"/>
-        <v>4859.5431748210349</v>
+        <v>5231.3046575358931</v>
       </c>
       <c r="AG10" s="38">
         <f t="shared" si="24"/>
-        <v>6100.0319549602718</v>
+        <v>6647.3649218833325</v>
       </c>
       <c r="AH10" s="38">
         <f t="shared" si="24"/>
-        <v>7510.8570293517951</v>
+        <v>8288.6150194047823</v>
       </c>
       <c r="AI10" s="38">
         <f t="shared" si="24"/>
-        <v>9115.407930899195</v>
+        <v>10190.865898434638</v>
       </c>
       <c r="AJ10" s="38">
         <f t="shared" si="24"/>
-        <v>10940.285899393601</v>
+        <v>12395.623364852745</v>
       </c>
       <c r="AK10" s="38">
         <f t="shared" si="10"/>
@@ -19310,7 +19329,7 @@
         <v>4.3E-3</v>
       </c>
       <c r="W11" s="48">
-        <v>0.15260000000000001</v>
+        <v>0.18970000000000001</v>
       </c>
       <c r="X11" s="49">
         <v>3.5999999999999997E-2</v>
@@ -19325,43 +19344,43 @@
       </c>
       <c r="AA11" s="51">
         <f t="shared" ref="AA11:AJ11" si="26">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y11*12*(1+$W11)) - ($Y11*12*(1+$W11))*$V11, (Z11+($Y11*12))*(1+$W11) - (Z11+($Y11*12))*(1+$W11)*$V11)</f>
-        <v>495.78213024000001</v>
+        <v>511.74041327999993</v>
       </c>
       <c r="AB11" s="51">
         <f t="shared" si="26"/>
-        <v>1064.7634280763712</v>
+        <v>1117.9400674095953</v>
       </c>
       <c r="AC11" s="51">
         <f t="shared" si="26"/>
-        <v>1717.7512982338619</v>
+        <v>1836.0346542949476</v>
       </c>
       <c r="AD11" s="51">
         <f t="shared" si="26"/>
-        <v>2467.1487919550691</v>
+        <v>2686.6782206533758</v>
       </c>
       <c r="AE11" s="51">
         <f t="shared" si="26"/>
-        <v>3327.190194347701</v>
+        <v>3694.3372257511423</v>
       </c>
       <c r="AF11" s="51">
         <f t="shared" si="26"/>
-        <v>4314.2113947477383</v>
+        <v>4887.9942528669853</v>
       </c>
       <c r="AG11" s="51">
         <f t="shared" si="26"/>
-        <v>5446.9601755958229</v>
+        <v>6301.9816148365189</v>
       </c>
       <c r="AH11" s="51">
         <f t="shared" si="26"/>
-        <v>6746.9523135486616</v>
+        <v>7976.9688300841708</v>
       </c>
       <c r="AI11" s="51">
         <f t="shared" si="26"/>
-        <v>8238.880256718825</v>
+        <v>9961.1323712173871</v>
       </c>
       <c r="AJ11" s="51">
         <f t="shared" si="26"/>
-        <v>9951.082140583374</v>
+        <v>12311.541330834565</v>
       </c>
       <c r="AK11" s="51">
         <f t="shared" si="10"/>
@@ -19446,62 +19465,62 @@
         <v>3.5000000000000001E-3</v>
       </c>
       <c r="W12" s="35">
-        <v>0.1893</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="X12" s="36">
-        <v>5.5E-2</v>
+        <v>0.06</v>
       </c>
       <c r="Y12" s="37">
         <f t="shared" si="2"/>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="Z12" s="37">
         <f t="shared" si="8"/>
-        <v>660</v>
+        <v>720</v>
       </c>
       <c r="AA12" s="38">
         <f t="shared" ref="AA12:AJ12" si="28">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y12*12*(1+$W12)) - ($Y12*12*(1+$W12))*$V12, (Z12+($Y12*12))*(1+$W12) - (Z12+($Y12*12))*(1+$W12)*$V12)</f>
-        <v>782.19071699999995</v>
+        <v>857.38860000000011</v>
       </c>
       <c r="AB12" s="38">
         <f t="shared" si="28"/>
-        <v>1709.1942287590516</v>
+        <v>1878.3819491805004</v>
       </c>
       <c r="AC12" s="38">
         <f t="shared" si="28"/>
-        <v>2807.8208068262193</v>
+        <v>3094.198696768251</v>
       </c>
       <c r="AD12" s="38">
         <f t="shared" si="28"/>
-        <v>4109.8443080589686</v>
+        <v>4542.014556588827</v>
       </c>
       <c r="AE12" s="38">
         <f t="shared" si="28"/>
-        <v>5652.9211201500211</v>
+        <v>6266.0990192407162</v>
       </c>
       <c r="AF12" s="38">
         <f t="shared" si="28"/>
-        <v>7481.6792383857392</v>
+        <v>8319.1689688446822</v>
       </c>
       <c r="AG12" s="38">
         <f t="shared" si="28"/>
-        <v>9649.0089712984172</v>
+        <v>10764.000593557203</v>
       </c>
       <c r="AH12" s="38">
         <f t="shared" si="28"/>
-        <v>12217.592604271729</v>
+        <v>13675.348876818305</v>
       </c>
       <c r="AI12" s="38">
         <f t="shared" si="28"/>
-        <v>15261.717261165455</v>
+        <v>17142.233361120583</v>
       </c>
       <c r="AJ12" s="38">
         <f t="shared" si="28"/>
-        <v>18869.42339451861</v>
+        <v>21270.66007550621</v>
       </c>
       <c r="AK12" s="38">
         <f t="shared" si="10"/>
-        <v>6600</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.2">
@@ -19582,62 +19601,62 @@
         <v>3.5000000000000001E-3</v>
       </c>
       <c r="W13" s="35">
-        <v>0.16209999999999999</v>
+        <v>0.18540000000000001</v>
       </c>
       <c r="X13" s="36">
-        <v>5.5E-2</v>
+        <v>0.06</v>
       </c>
       <c r="Y13" s="37">
         <f t="shared" si="2"/>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="Z13" s="37">
         <f t="shared" si="8"/>
-        <v>660</v>
+        <v>720</v>
       </c>
       <c r="AA13" s="38">
         <f t="shared" ref="AA13:AJ13" si="30">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y13*12*(1+$W13)) - ($Y13*12*(1+$W13))*$V13, (Z13+($Y13*12))*(1+$W13) - (Z13+($Y13*12))*(1+$W13)*$V13)</f>
-        <v>764.30154900000002</v>
+        <v>850.50079200000005</v>
       </c>
       <c r="AB13" s="38">
         <f t="shared" si="30"/>
-        <v>1649.3876971875748</v>
+        <v>1855.1557881008712</v>
       </c>
       <c r="AC13" s="38">
         <f t="shared" si="30"/>
-        <v>2674.3463548515247</v>
+        <v>3041.9056073655211</v>
       </c>
       <c r="AD13" s="38">
         <f t="shared" si="30"/>
-        <v>3861.2819453265511</v>
+        <v>4443.7551367966898</v>
       </c>
       <c r="AE13" s="38">
         <f t="shared" si="30"/>
-        <v>5235.7921125436606</v>
+        <v>6099.6914354717401</v>
       </c>
       <c r="AF13" s="38">
         <f t="shared" si="30"/>
-        <v>6827.5197639380331</v>
+        <v>8055.7680098115716</v>
       </c>
       <c r="AG13" s="38">
         <f t="shared" si="30"/>
-        <v>8670.7923541605342</v>
+        <v>10366.385614934728</v>
       </c>
       <c r="AH13" s="38">
         <f t="shared" si="30"/>
-        <v>10805.36219648826</v>
+        <v>13095.805202665824</v>
       </c>
       <c r="AI13" s="38">
         <f t="shared" si="30"/>
-        <v>13277.26376760912</v>
+        <v>16319.935093034728</v>
       </c>
       <c r="AJ13" s="38">
         <f t="shared" si="30"/>
-        <v>16139.806494553373</v>
+        <v>20128.442072575875</v>
       </c>
       <c r="AK13" s="38">
         <f t="shared" si="10"/>
-        <v>6600</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.2">
@@ -19718,7 +19737,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="W14" s="48">
-        <v>9.0499999999999997E-2</v>
+        <v>0.1142</v>
       </c>
       <c r="X14" s="49">
         <v>4.4999999999999998E-2</v>
@@ -19733,43 +19752,43 @@
       </c>
       <c r="AA14" s="51">
         <f t="shared" ref="AA14:AJ14" si="32">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y14*12*(1+$W14)) - ($Y14*12*(1+$W14))*$V14, (Z14+($Y14*12))*(1+$W14) - (Z14+($Y14*12))*(1+$W14)*$V14)</f>
-        <v>588.51667799999996</v>
+        <v>601.30699919999995</v>
       </c>
       <c r="AB14" s="51">
         <f t="shared" si="32"/>
-        <v>1229.9090488965846</v>
+        <v>1270.8812719535349</v>
       </c>
       <c r="AC14" s="51">
         <f t="shared" si="32"/>
-        <v>1928.9277663310327</v>
+        <v>2016.4733028627024</v>
       </c>
       <c r="AD14" s="51">
         <f t="shared" si="32"/>
-        <v>2690.750309746481</v>
+        <v>2846.7135005171936</v>
       </c>
       <c r="AE14" s="51">
         <f t="shared" si="32"/>
-        <v>3521.0193328508703</v>
+        <v>3771.2120965668919</v>
       </c>
       <c r="AF14" s="51">
         <f t="shared" si="32"/>
-        <v>4425.8844575243893</v>
+        <v>4800.6703864840338</v>
       </c>
       <c r="AG14" s="51">
         <f t="shared" si="32"/>
-        <v>5412.0478227297881</v>
+        <v>5947.0045996537383</v>
       </c>
       <c r="AH14" s="51">
         <f t="shared" si="32"/>
-        <v>6486.8137257964227</v>
+        <v>7223.4838326192348</v>
       </c>
       <c r="AI14" s="51">
         <f t="shared" si="32"/>
-        <v>7658.1427237602111</v>
+        <v>8644.8836420925691</v>
       </c>
       <c r="AJ14" s="51">
         <f t="shared" si="32"/>
-        <v>8934.7105954763538</v>
+        <v>10227.657075607131</v>
       </c>
       <c r="AK14" s="51">
         <f t="shared" si="10"/>
@@ -19854,7 +19873,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="W15" s="53">
-        <v>0.11899999999999999</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="X15" s="54">
         <v>4.4999999999999998E-2</v>
@@ -19869,43 +19888,43 @@
       </c>
       <c r="AA15" s="51">
         <f t="shared" ref="AA15:AJ15" si="34">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y15*12*(1+$W15)) - ($Y15*12*(1+$W15))*$V15, (Z15+($Y15*12))*(1+$W15) - (Z15+($Y15*12))*(1+$W15)*$V15)</f>
-        <v>603.89744399999995</v>
+        <v>612.53225999999995</v>
       </c>
       <c r="AB15" s="51">
         <f t="shared" si="34"/>
-        <v>1279.2532270920983</v>
+        <v>1307.3392406309399</v>
       </c>
       <c r="AC15" s="51">
         <f t="shared" si="34"/>
-        <v>2034.5229144993882</v>
+        <v>2095.4720000932471</v>
       </c>
       <c r="AD15" s="51">
         <f t="shared" si="34"/>
-        <v>2879.1626066400204</v>
+        <v>2989.465963673772</v>
       </c>
       <c r="AE15" s="51">
         <f t="shared" si="34"/>
-        <v>3823.7473310560849</v>
+        <v>4003.5403024484694</v>
       </c>
       <c r="AF15" s="51">
         <f t="shared" si="34"/>
-        <v>4880.1034434936892</v>
+        <v>5153.8240923330459</v>
       </c>
       <c r="AG15" s="51">
         <f t="shared" si="34"/>
-        <v>6061.4566958174764</v>
+        <v>6458.6128505911283</v>
       </c>
       <c r="AH15" s="51">
         <f t="shared" si="34"/>
-        <v>7382.5978245941842</v>
+        <v>7938.6595300696781</v>
       </c>
       <c r="AI15" s="51">
         <f t="shared" si="34"/>
-        <v>8860.0677335414603</v>
+        <v>9617.5045994891079</v>
       </c>
       <c r="AJ15" s="51">
         <f t="shared" si="34"/>
-        <v>10512.364588356593</v>
+        <v>11521.850459787885</v>
       </c>
       <c r="AK15" s="51">
         <f t="shared" si="10"/>
@@ -19917,7 +19936,7 @@
         <v>385</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C16" s="35">
         <v>7.4999999999999997E-3</v>
@@ -19984,68 +20003,68 @@
         <v>385</v>
       </c>
       <c r="U16" s="23" t="s">
-        <v>68</v>
+        <v>415</v>
       </c>
       <c r="V16" s="35">
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="W16" s="35">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="X16" s="36">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="Y16" s="37">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="Z16" s="37">
         <f t="shared" si="8"/>
-        <v>1200</v>
+        <v>1080</v>
       </c>
       <c r="AA16" s="38">
         <f t="shared" ref="AA16:AJ16" si="36">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y16*12*(1+$W16)) - ($Y16*12*(1+$W16))*$V16, (Z16+($Y16*12))*(1+$W16) - (Z16+($Y16*12))*(1+$W16)*$V16)</f>
-        <v>1488.75</v>
+        <v>1350.5940000000001</v>
       </c>
       <c r="AB16" s="38">
         <f t="shared" si="36"/>
-        <v>3335.73046875</v>
+        <v>3039.5793266999999</v>
       </c>
       <c r="AC16" s="38">
         <f t="shared" si="36"/>
-        <v>5627.1406127929686</v>
+        <v>5151.7399270046853</v>
       </c>
       <c r="AD16" s="38">
         <f t="shared" si="36"/>
-        <v>8469.9213227462769</v>
+        <v>7793.1023657157093</v>
       </c>
       <c r="AE16" s="38">
         <f t="shared" si="36"/>
-        <v>11996.746141032099</v>
+        <v>11096.25816344578</v>
       </c>
       <c r="AF16" s="38">
         <f t="shared" si="36"/>
-        <v>16372.21318121795</v>
+        <v>15227.01964629712</v>
       </c>
       <c r="AG16" s="38">
         <f t="shared" si="36"/>
-        <v>21800.526977948521</v>
+        <v>20392.743418676862</v>
       </c>
       <c r="AH16" s="38">
         <f t="shared" si="36"/>
-        <v>28535.028782017383</v>
+        <v>26852.73928222635</v>
       </c>
       <c r="AI16" s="38">
         <f t="shared" si="36"/>
-        <v>36890.020082690316</v>
+        <v>34931.287109388162</v>
       </c>
       <c r="AJ16" s="38">
         <f t="shared" si="36"/>
-        <v>47255.431165087677</v>
+        <v>45033.915094645366</v>
       </c>
       <c r="AK16" s="38">
         <f t="shared" si="10"/>
-        <v>12000</v>
+        <v>10800</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.2">
@@ -20053,7 +20072,7 @@
         <v>385</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C17" s="35">
         <v>7.6E-3</v>
@@ -20120,68 +20139,68 @@
         <v>385</v>
       </c>
       <c r="U17" s="23" t="s">
-        <v>37</v>
+        <v>416</v>
       </c>
       <c r="V17" s="35">
         <v>7.6E-3</v>
       </c>
       <c r="W17" s="35">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="X17" s="36">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="Y17" s="37">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="Z17" s="37">
         <f t="shared" si="8"/>
-        <v>1200</v>
+        <v>1080</v>
       </c>
       <c r="AA17" s="38">
         <f t="shared" ref="AA17:AJ17" si="38">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y17*12*(1+$W17)) - ($Y17*12*(1+$W17))*$V17, (Z17+($Y17*12))*(1+$W17) - (Z17+($Y17*12))*(1+$W17)*$V17)</f>
-        <v>1488.6</v>
+        <v>1318.3041600000001</v>
       </c>
       <c r="AB17" s="38">
         <f t="shared" si="38"/>
-        <v>3335.2082999999998</v>
+        <v>2927.4947695123201</v>
       </c>
       <c r="AC17" s="38">
         <f t="shared" si="38"/>
-        <v>5625.92589615</v>
+        <v>4891.7565053947519</v>
       </c>
       <c r="AD17" s="38">
         <f t="shared" si="38"/>
-        <v>8467.5610741740747</v>
+        <v>7289.4365218231142</v>
       </c>
       <c r="AE17" s="38">
         <f t="shared" si="38"/>
-        <v>11992.60951251294</v>
+        <v>10216.169429236428</v>
       </c>
       <c r="AF17" s="38">
         <f t="shared" si="38"/>
-        <v>16365.432100272301</v>
+        <v>13788.691806136305</v>
       </c>
       <c r="AG17" s="38">
         <f t="shared" si="38"/>
-        <v>21789.91852038779</v>
+        <v>18149.498390543893</v>
       </c>
       <c r="AH17" s="38">
         <f t="shared" si="38"/>
-        <v>28518.993924541053</v>
+        <v>23472.525669414183</v>
       </c>
       <c r="AI17" s="38">
         <f t="shared" si="38"/>
-        <v>36866.411963393177</v>
+        <v>29970.089563421763</v>
       </c>
       <c r="AJ17" s="38">
         <f t="shared" si="38"/>
-        <v>47221.384040589241</v>
+        <v>37901.353925769901</v>
       </c>
       <c r="AK17" s="38">
         <f t="shared" si="10"/>
-        <v>12000</v>
+        <v>10800</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.2">
@@ -20189,7 +20208,7 @@
         <v>386</v>
       </c>
       <c r="B18" s="47" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C18" s="48">
         <v>3.5E-4</v>
@@ -20256,13 +20275,13 @@
         <v>386</v>
       </c>
       <c r="U18" s="47" t="s">
-        <v>387</v>
+        <v>418</v>
       </c>
       <c r="V18" s="48">
         <v>3.5E-4</v>
       </c>
       <c r="W18" s="48">
-        <v>2.3599999999999999E-2</v>
+        <v>3.7900000000000003E-2</v>
       </c>
       <c r="X18" s="49">
         <v>0.01</v>
@@ -20277,43 +20296,43 @@
       </c>
       <c r="AA18" s="51">
         <f t="shared" ref="AA18:AJ18" si="40">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y18*12*(1+$W18)) - ($Y18*12*(1+$W18))*$V18, (Z18+($Y18*12))*(1+$W18) - (Z18+($Y18*12))*(1+$W18)*$V18)</f>
-        <v>122.7890088</v>
+        <v>124.5044082</v>
       </c>
       <c r="AB18" s="51">
         <f t="shared" si="40"/>
-        <v>248.43184781738734</v>
+        <v>253.68230537693523</v>
       </c>
       <c r="AC18" s="51">
         <f t="shared" si="40"/>
-        <v>376.99484503207862</v>
+        <v>387.70911904805837</v>
       </c>
       <c r="AD18" s="51">
         <f t="shared" si="40"/>
-        <v>508.54587000165452</v>
+        <v>526.76686170684877</v>
       </c>
       <c r="AE18" s="51">
         <f t="shared" si="40"/>
-        <v>643.15436969030679</v>
+        <v>671.04437800152039</v>
       </c>
       <c r="AF18" s="51">
         <f t="shared" si="40"/>
-        <v>780.89140513051279</v>
+        <v>820.73760119180326</v>
       </c>
       <c r="AG18" s="51">
         <f t="shared" si="40"/>
-        <v>921.82968893679083</v>
+        <v>976.04981923227569</v>
       </c>
       <c r="AH18" s="51">
         <f t="shared" si="40"/>
-        <v>1066.0436236913406</v>
+        <v>1137.1919508435956</v>
       </c>
       <c r="AI18" s="51">
         <f t="shared" si="40"/>
-        <v>1213.6093412218327</v>
+        <v>1304.3828319465449</v>
       </c>
       <c r="AJ18" s="51">
         <f t="shared" si="40"/>
-        <v>1364.6047427920819</v>
+        <v>1477.8495128478719</v>
       </c>
       <c r="AK18" s="51">
         <f t="shared" si="10"/>
@@ -20325,7 +20344,7 @@
         <v>386</v>
       </c>
       <c r="B19" s="47" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C19" s="48">
         <v>3.5E-4</v>
@@ -20392,13 +20411,13 @@
         <v>386</v>
       </c>
       <c r="U19" s="47" t="s">
-        <v>388</v>
+        <v>419</v>
       </c>
       <c r="V19" s="48">
         <v>3.5E-4</v>
       </c>
       <c r="W19" s="48">
-        <v>2.4E-2</v>
+        <v>4.0399999999999998E-2</v>
       </c>
       <c r="X19" s="49">
         <v>0.01</v>
@@ -20413,43 +20432,43 @@
       </c>
       <c r="AA19" s="51">
         <f t="shared" ref="AA19:AJ19" si="42">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y19*12*(1+$W19)) - ($Y19*12*(1+$W19))*$V19, (Z19+($Y19*12))*(1+$W19) - (Z19+($Y19*12))*(1+$W19)*$V19)</f>
-        <v>122.836992</v>
+        <v>124.80430319999999</v>
       </c>
       <c r="AB19" s="51">
         <f t="shared" si="42"/>
-        <v>248.57804703006721</v>
+        <v>254.60525401031273</v>
       </c>
       <c r="AC19" s="51">
         <f t="shared" si="42"/>
-        <v>377.29182178673324</v>
+        <v>389.60289751513398</v>
       </c>
       <c r="AD19" s="51">
         <f t="shared" si="42"/>
-        <v>509.04859612068651</v>
+        <v>530.00528777564421</v>
       </c>
       <c r="AE19" s="51">
         <f t="shared" si="42"/>
-        <v>643.92031141073335</v>
+        <v>676.02880847628956</v>
       </c>
       <c r="AF19" s="51">
         <f t="shared" si="42"/>
-        <v>781.98060984498136</v>
+        <v>827.89850640841303</v>
       </c>
       <c r="AG19" s="51">
         <f t="shared" si="42"/>
-        <v>923.30487463069255</v>
+        <v>985.84843830518935</v>
       </c>
       <c r="AH19" s="51">
         <f t="shared" si="42"/>
-        <v>1067.9702711547618</v>
+        <v>1150.1220315623946</v>
       </c>
       <c r="AI19" s="51">
         <f t="shared" si="42"/>
-        <v>1216.0557891172941</v>
+        <v>1320.9724594009422</v>
       </c>
       <c r="AJ19" s="51">
         <f t="shared" si="42"/>
-        <v>1367.6422856612896</v>
+        <v>1498.663031049374</v>
       </c>
       <c r="AK19" s="51">
         <f t="shared" si="10"/>
@@ -20461,7 +20480,7 @@
         <v>386</v>
       </c>
       <c r="B20" s="47" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C20" s="48">
         <v>2.9999999999999997E-4</v>
@@ -20528,16 +20547,15 @@
         <v>386</v>
       </c>
       <c r="U20" s="47" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="V20" s="48">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="W20" s="48">
-        <v>0.1076</v>
+        <v>7.6300000000000007E-2</v>
       </c>
       <c r="X20" s="49">
-        <f>0.1*0.6</f>
         <v>0.06</v>
       </c>
       <c r="Y20" s="50">
@@ -20550,43 +20568,43 @@
       </c>
       <c r="AA20" s="51">
         <f t="shared" ref="AA20:AJ20" si="44">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y20*12*(1+$W20)) - ($Y20*12*(1+$W20))*$V20, (Z20+($Y20*12))*(1+$W20) - (Z20+($Y20*12))*(1+$W20)*$V20)</f>
-        <v>797.23275839999997</v>
+        <v>774.70351920000007</v>
       </c>
       <c r="AB20" s="51">
         <f t="shared" si="44"/>
-        <v>1679.9828571028786</v>
+        <v>1608.2667728956458</v>
       </c>
       <c r="AC20" s="51">
         <f t="shared" si="44"/>
-        <v>2657.4235462233901</v>
+        <v>2505.1617536092836</v>
       </c>
       <c r="AD20" s="51">
         <f t="shared" si="44"/>
-        <v>3739.7120695010876</v>
+        <v>3470.2002229310488</v>
       </c>
       <c r="AE20" s="51">
         <f t="shared" si="44"/>
-        <v>4938.0952150529502</v>
+        <v>4508.5595261907065</v>
       </c>
       <c r="AF20" s="51">
         <f t="shared" si="44"/>
-        <v>6265.0261883145895</v>
+        <v>5625.8103684536463</v>
       </c>
       <c r="AG20" s="51">
         <f t="shared" si="44"/>
-        <v>7734.2940216753859</v>
+        <v>6827.9467008567899</v>
       </c>
       <c r="AH20" s="51">
         <f t="shared" si="44"/>
-        <v>9361.166865590134</v>
+        <v>8121.4178776219242</v>
       </c>
       <c r="AI20" s="51">
         <f t="shared" si="44"/>
-        <v>11162.550650201532</v>
+        <v>9513.1632562659706</v>
       </c>
       <c r="AJ20" s="51">
         <f t="shared" si="44"/>
-        <v>13157.164766233167</v>
+        <v>11010.649426635247</v>
       </c>
       <c r="AK20" s="51">
         <f t="shared" si="10"/>
@@ -20598,7 +20616,7 @@
         <v>329</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C21" s="35">
         <v>1.8E-3</v>
@@ -20665,68 +20683,68 @@
         <v>329</v>
       </c>
       <c r="U21" s="23" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="V21" s="35">
         <v>1.8E-3</v>
       </c>
       <c r="W21" s="35">
-        <v>2.5499999999999998E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="X21" s="36">
-        <v>0</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="Y21" s="37">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="Z21" s="37">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="AA21" s="38">
         <f t="shared" ref="AA21:AJ21" si="46">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y21*12*(1+$W21)) - ($Y21*12*(1+$W21))*$V21, (Z21+($Y21*12))*(1+$W21) - (Z21+($Y21*12))*(1+$W21)*$V21)</f>
-        <v>0</v>
+        <v>312.63623999999999</v>
       </c>
       <c r="AB21" s="38">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>638.44096853779206</v>
       </c>
       <c r="AC21" s="38">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>977.96885288537862</v>
       </c>
       <c r="AD21" s="38">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>1331.7979233439928</v>
       </c>
       <c r="AE21" s="38">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>1700.5305573135804</v>
       </c>
       <c r="AF21" s="38">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>2084.7945048120741</v>
       </c>
       <c r="AG21" s="38">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>2485.2439571903624</v>
       </c>
       <c r="AH21" s="38">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>2902.5606608623866</v>
       </c>
       <c r="AI21" s="38">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>3337.4550779464394</v>
       </c>
       <c r="AJ21" s="38">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>3790.6675957936059</v>
       </c>
       <c r="AK21" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.2">
@@ -20734,7 +20752,7 @@
         <v>329</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C22" s="39">
         <v>5.0000000000000001E-3</v>
@@ -20801,76 +20819,76 @@
         <v>329</v>
       </c>
       <c r="U22" s="25" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="V22" s="39">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="W22" s="39">
-        <v>1.2500000000000001E-2</v>
+        <v>1.8100000000000002E-2</v>
       </c>
       <c r="X22" s="40">
-        <v>0</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="Y22" s="37">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="Z22" s="37">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="AA22" s="38">
         <f t="shared" ref="AA22:AJ23" si="48">IF(MID(Z$1,1,2) &lt;&gt; "CY",($Y22*12*(1+$W22)) - ($Y22*12*(1+$W22))*$V22, (Z22+($Y22*12))*(1+$W22) - (Z22+($Y22*12))*(1+$W22)*$V22)</f>
-        <v>0</v>
+        <v>303.90285</v>
       </c>
       <c r="AB22" s="38">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>611.75932412707493</v>
       </c>
       <c r="AC22" s="38">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>923.62085705430604</v>
       </c>
       <c r="AD22" s="38">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>1239.539552594154</v>
       </c>
       <c r="AE22" s="38">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>1559.5681924036276</v>
       </c>
       <c r="AF22" s="38">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>1883.7602448027026</v>
       </c>
       <c r="AG22" s="38">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>2212.1698737074635</v>
       </c>
       <c r="AH22" s="38">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>2544.8519476794609</v>
       </c>
       <c r="AI22" s="38">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>2881.862049092797</v>
       </c>
       <c r="AJ22" s="38">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>3223.25648342047</v>
       </c>
       <c r="AK22" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C23" s="35"/>
       <c r="D23" s="35"/>
@@ -20888,80 +20906,64 @@
       <c r="P23" s="38"/>
       <c r="Q23" s="38"/>
       <c r="R23" s="38"/>
-      <c r="T23" s="23" t="s">
-        <v>385</v>
-      </c>
-      <c r="U23" s="23" t="s">
-        <v>417</v>
-      </c>
-      <c r="V23" s="35">
-        <v>2E-3</v>
-      </c>
-      <c r="W23" s="35">
-        <v>0.19900000000000001</v>
-      </c>
-      <c r="X23" s="36">
-        <v>0.1</v>
-      </c>
-      <c r="Y23" s="37">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="Z23" s="37">
-        <f t="shared" si="8"/>
-        <v>1200</v>
-      </c>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="35"/>
+      <c r="W23" s="35"/>
+      <c r="X23" s="36"/>
+      <c r="Y23" s="37"/>
+      <c r="Z23" s="37"/>
       <c r="AA23" s="38">
         <f t="shared" si="48"/>
-        <v>1435.9224000000002</v>
+        <v>0</v>
       </c>
       <c r="AB23" s="38">
         <f t="shared" si="48"/>
-        <v>3154.1500156848006</v>
+        <v>0</v>
       </c>
       <c r="AC23" s="38">
         <f t="shared" si="48"/>
-        <v>5210.1846170684639</v>
+        <v>0</v>
       </c>
       <c r="AD23" s="38">
         <f t="shared" si="48"/>
-        <v>7670.4397331533582</v>
+        <v>0</v>
       </c>
       <c r="AE23" s="38">
         <f t="shared" si="48"/>
-        <v>10614.385925570776</v>
+        <v>0</v>
       </c>
       <c r="AF23" s="38">
         <f t="shared" si="48"/>
-        <v>14137.117827309841</v>
+        <v>0</v>
       </c>
       <c r="AG23" s="38">
         <f t="shared" si="48"/>
-        <v>18352.425866394609</v>
+        <v>0</v>
       </c>
       <c r="AH23" s="38">
         <f t="shared" si="48"/>
-        <v>23396.471896579522</v>
+        <v>0</v>
       </c>
       <c r="AI23" s="38">
         <f t="shared" si="48"/>
-        <v>29432.187464390849</v>
+        <v>0</v>
       </c>
       <c r="AJ23" s="38">
         <f t="shared" si="48"/>
-        <v>36654.536784265023</v>
+        <v>0</v>
       </c>
       <c r="AK23" s="38">
         <f t="shared" si="10"/>
-        <v>12000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C24" s="35"/>
       <c r="D24" s="35"/>
@@ -20980,10 +20982,10 @@
       <c r="Q24" s="38"/>
       <c r="R24" s="38"/>
       <c r="T24" s="23" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="U24" s="23" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="V24" s="35"/>
       <c r="W24" s="35"/>
@@ -21004,10 +21006,10 @@
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C25" s="35"/>
       <c r="D25" s="35"/>
@@ -21026,10 +21028,10 @@
       <c r="Q25" s="38"/>
       <c r="R25" s="38"/>
       <c r="T25" s="23" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="U25" s="23" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="V25" s="35"/>
       <c r="W25" s="35"/>
@@ -21095,17 +21097,52 @@
       <c r="AI26" s="41"/>
       <c r="AJ26" s="41">
         <f>SUM(AJ2:AJ25)</f>
-        <v>341034.56977015134</v>
+        <v>316212.90983632038</v>
       </c>
       <c r="AK26" s="41">
         <f>SUM(AK2:AK25)</f>
-        <v>132000</v>
+        <v>120600</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Q27" s="83">
         <f>Q26-R26</f>
         <v>196556.03502084804</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A30" s="21" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A31" s="21" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A32" s="21" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="85" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="85" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="21" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="21" t="s">
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -21121,7 +21158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A42C0D-8FE3-45A5-B249-37C5FF5CEED1}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
@@ -21135,16 +21172,16 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="29"/>
       <c r="B1" s="29" t="s">
+        <v>391</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>392</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>393</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="E1" s="29" t="s">
         <v>394</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>395</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>396</v>
       </c>
       <c r="F1" s="29" t="s">
         <v>359</v>
@@ -21225,7 +21262,7 @@
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="55" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -21241,9 +21278,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21470,27 +21510,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401ADED5-CC5A-4072-B36A-6DA217C5A368}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DB5870C-189D-475E-8E58-449C30115ACA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e8f9595b-0d5a-46b2-8488-c972c1ea4246"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6bcbbac3-d60f-4c54-b2b4-d245c065548d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -21515,9 +21543,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DB5870C-189D-475E-8E58-449C30115ACA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401ADED5-CC5A-4072-B36A-6DA217C5A368}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e8f9595b-0d5a-46b2-8488-c972c1ea4246"/>
+    <ds:schemaRef ds:uri="6bcbbac3-d60f-4c54-b2b4-d245c065548d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated watchlist with some additional stocks to watch
</commit_message>
<xml_diff>
--- a/input/Watchlist.xlsx
+++ b/input/Watchlist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23120"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bayergroup-my.sharepoint.com/personal/sivacharan_chandrasekar_ext_bayer_com/Documents/Personal Data/Analytics/us-stocks-analysis/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssoma\OneDrive - Bayer\Personal Data\Analytics\us-stocks-analysis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{A259AFBD-2F1F-43A4-8040-58927886A03B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BC115BD5-D20C-4716-B016-6379ACDD3F90}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{A259AFBD-2F1F-43A4-8040-58927886A03B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{0DA8173F-C062-4081-948D-20278E95ACEC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fund List" sheetId="1" r:id="rId1"/>
@@ -23,14 +23,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ARK Comparison'!$A$1:$M$132</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
@@ -46,7 +44,7 @@
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -765,7 +763,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="437">
   <si>
     <t>Funds</t>
   </si>
@@ -2055,6 +2053,27 @@
   </si>
   <si>
     <t>https://www.begintoinvest.com/expense-ratio-calculator/</t>
+  </si>
+  <si>
+    <t>IBB - Biotech</t>
+  </si>
+  <si>
+    <t>XBI</t>
+  </si>
+  <si>
+    <t>Biotech</t>
+  </si>
+  <si>
+    <t>FBT</t>
+  </si>
+  <si>
+    <t>QTUM</t>
+  </si>
+  <si>
+    <t>Tech &amp; Semiconductor</t>
+  </si>
+  <si>
+    <t>This has 40% international mix with just 1 year of performance data</t>
   </si>
 </sst>
 </file>
@@ -2062,14 +2081,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="170" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2301,7 +2320,7 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="86">
@@ -2352,7 +2371,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2448,10 +2467,10 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="12" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2879,7 +2898,7 @@
         <name val="Source Sans Pro"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -3387,6 +3406,9 @@
   <types>
     <type name="_imageurl">
       <keyFlags>
+        <key name="Attribution Size">
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
         <key name="Blip Identifier">
           <flag name="ShowInCardView" value="0"/>
         </key>
@@ -3434,12 +3456,12 @@
           <flag name="ShowInDotNotation" value="0"/>
           <flag name="ShowInAutoComplete" value="0"/>
         </key>
-        <key name="%DataProviderExternalLinkLogo">
+        <key name="%DataProviderExternalLink">
           <flag name="ShowInCardView" value="0"/>
           <flag name="ShowInDotNotation" value="0"/>
           <flag name="ShowInAutoComplete" value="0"/>
         </key>
-        <key name="%DataProviderExternalLink">
+        <key name="%DataProviderExternalLinkLogo">
           <flag name="ShowInCardView" value="0"/>
           <flag name="ShowInDotNotation" value="0"/>
           <flag name="ShowInAutoComplete" value="0"/>
@@ -5444,9 +5466,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_65638ce82d623bac8d564989d24bda28&amp;qlt=95</v>
     <v>140</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=honda</v>
     <v>Image of HONDA MOTOR CO., LTD.</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1uqyc&amp;q=XNYS%3aHMC&amp;form=skydnc</v>
@@ -5515,9 +5537,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_97bd8dad8c0360a49d8c3a8c9f408be5&amp;qlt=95</v>
     <v>147</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=wells+fargo</v>
     <v>Image of WELLS FARGO &amp; COMPANY</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a25tgh&amp;q=XNYS%3aWFC&amp;form=skydnc</v>
@@ -5582,9 +5604,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_0720042c42661f705c810fedd777349a&amp;qlt=95</v>
     <v>153</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=bank+of+america</v>
     <v>Image of BANK OF AMERICA CORPORATION</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1o4sm&amp;q=XNYS%3aBAC&amp;form=skydnc</v>
@@ -5649,9 +5671,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_06392bb84e5fdc62d2356a2306f4ae1e&amp;qlt=95</v>
     <v>159</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=jpmorgan+chase</v>
     <v>Image of JPMORGAN CHASE &amp; CO.</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1waa2&amp;q=XNYS%3aJPM&amp;form=skydnc</v>
@@ -5716,9 +5738,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_c244bad2af0aa117b9f67bcd11fd44e9&amp;qlt=95</v>
     <v>165</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=the+coca-cola+company</v>
     <v>Image of THE COCA-COLA COMPANY</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1wljc&amp;q=XNYS%3aKO&amp;form=skydnc</v>
@@ -5783,9 +5805,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_90a82bf7d9bf620ad2bd5ec79a4882af&amp;qlt=95</v>
     <v>171</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=costco</v>
     <v>Image of COSTCO WHOLESALE CORPORATION</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1q6k2&amp;q=XNAS%3aCOST&amp;form=skydnc</v>
@@ -5890,9 +5912,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_f277632c13de4db2ca85eddfe0a297c9&amp;qlt=95</v>
     <v>180</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=six+flags</v>
     <v>Image of SIX FLAGS ENTERTAINMENT CORPORATION</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a22zu2&amp;q=XNYS%3aSIX&amp;form=skydnc</v>
@@ -5957,9 +5979,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_b7e2eab1a0465d4acb936b45513ab111&amp;qlt=95</v>
     <v>186</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=the+cheesecake+factory</v>
     <v>Image of THE CHEESECAKE FACTORY INCORPORATED</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1p5h7&amp;q=XNAS%3aCAKE&amp;form=skydnc</v>
@@ -6024,9 +6046,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_5a814ff30fd1ffac245379798a819c9e&amp;qlt=95</v>
     <v>192</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=wyndham+worldwide</v>
     <v>Image of WYNDHAM DESTINATIONS, INC.</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=b16nh7&amp;q=XNYS%3aWYND&amp;form=skydnc</v>
@@ -6095,9 +6117,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_0906c9459990b0fab2037038e2dfe1bd&amp;qlt=95</v>
     <v>199</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=las+vegas+sands</v>
     <v>Image of LAS VEGAS SANDS CORP.</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1x7im&amp;q=XNYS%3aLVS&amp;form=skydnc</v>
@@ -6162,9 +6184,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_e27b6f4d10a663f3cbffe838112b48be&amp;qlt=95</v>
     <v>205</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=starbucks</v>
     <v>Image of STARBUCKS CORPORATION</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a22k9c&amp;q=XNAS%3aSBUX&amp;form=skydnc</v>
@@ -6284,9 +6306,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_982b67ee8686548274ef55ed627e1e1f&amp;qlt=95</v>
     <v>215</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=royal+dutch+shell</v>
     <v>Image of ROYAL DUTCH SHELL PLC</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a21t52&amp;q=XNYS%3aRDS.A&amp;form=skydnc</v>
@@ -6402,9 +6424,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_a92fdfeb8644bf85ee9299accf15739c&amp;qlt=95</v>
     <v>224</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=exxon+mobil</v>
     <v>Image of EXXON MOBIL CORPORATION</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a269ec&amp;q=XNYS%3aXOM&amp;form=skydnc</v>
@@ -6469,9 +6491,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_328c42228a7a7c01496b8aa73b7a09ba&amp;qlt=95</v>
     <v>230</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=conocophillips</v>
     <v>Image of CONOCOPHILLIPS</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1q5nm&amp;q=XNYS%3aCOP&amp;form=skydnc</v>
@@ -6576,9 +6598,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_2d49dc55c1faf81186e7649c0d153e02&amp;qlt=95</v>
     <v>239</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=chevron+corporation</v>
     <v>Image of CHEVRON CORPORATION</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1qlz2&amp;q=XNYS%3aCVX&amp;form=skydnc</v>
@@ -6643,9 +6665,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_d132f0c8d3455e1bb112e94f5d892d58&amp;qlt=95</v>
     <v>245</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=h%26r+block</v>
     <v>Image of H &amp; R BLOCK, INC.</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1uuvh&amp;q=XNYS%3aHRB&amp;form=skydnc</v>
@@ -6812,9 +6834,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_4afbc0a090454dfb219470553edb70e4&amp;qlt=95</v>
     <v>257</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=lowe%27s</v>
     <v>Image of LOWE`S COMPANIES, INC.</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1x2ur&amp;q=XNYS%3aLOW&amp;form=skydnc</v>
@@ -6879,9 +6901,9 @@
   <rv s="8">
     <v>https://www.bing.com/th?id=AMMS_25dbea32b4516ce1661da911a36f7ad2&amp;qlt=95</v>
     <v>263</v>
+    <v/>
     <v>https://www.bing.com/images/search?form=xlimg&amp;q=at%26t</v>
     <v>Image of AT&amp;T INC.</v>
-    <v/>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a23www&amp;q=XNYS%3aT&amp;form=skydnc</v>
@@ -7139,9 +7161,9 @@
   <s t="_imageurl">
     <k n="Address" t="s"/>
     <k n="Attribution" t="r"/>
+    <k n="Blip Identifier" t="s"/>
     <k n="More Images Address" t="s"/>
     <k n="Text" t="s"/>
-    <k n="Blip Identifier" t="s"/>
   </s>
   <s t="_linkedentitycore">
     <k n="%EntityCulture" t="s"/>
@@ -7964,13 +7986,13 @@
       <x:numFmt numFmtId="165" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;_);_(@_)"/>
     </x:dxf>
     <x:dxf>
-      <x:numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <x:numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </x:dxf>
     <x:dxf>
       <x:numFmt numFmtId="2" formatCode="0.00"/>
     </x:dxf>
     <x:dxf>
-      <x:numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <x:numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </x:dxf>
     <x:dxf>
       <x:numFmt numFmtId="1" formatCode="0"/>
@@ -8112,8 +8134,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{66674435-6956-4569-B586-8504E039F3C5}" name="Table4" displayName="Table4" ref="A29:C38" totalsRowShown="0">
-  <autoFilter ref="A29:C38" xr:uid="{76A2AC23-EA1A-42A9-A4A0-BA4126640B6B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{66674435-6956-4569-B586-8504E039F3C5}" name="Table4" displayName="Table4" ref="A29:C41" totalsRowShown="0">
+  <autoFilter ref="A29:C41" xr:uid="{76A2AC23-EA1A-42A9-A4A0-BA4126640B6B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C5A951EA-02C9-4EEA-B580-3EE51E7FDF81}" name="Fund"/>
     <tableColumn id="2" xr3:uid="{EDFF81EE-5847-4637-99DE-F7A607DAE56F}" name="Category" dataDxfId="1"/>
@@ -8426,7 +8448,7 @@
       <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -8442,7 +8464,7 @@
     <col min="16" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="17" customFormat="1" ht="44.25" customHeight="1">
+    <row r="1" spans="1:15" s="17" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -8489,7 +8511,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" hidden="1">
+    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -8547,7 +8569,7 @@
         <v>0.25420205752006669</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1">
+    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
@@ -8605,7 +8627,7 @@
         <v>1.2657342657342641E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
@@ -8663,7 +8685,7 @@
         <v>4.3300984763585942E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1">
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
@@ -8721,7 +8743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1">
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
@@ -8779,7 +8801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1">
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
@@ -8837,7 +8859,7 @@
         <v>0.39543197360595578</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1">
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
@@ -8895,7 +8917,7 @@
         <v>0.12977124183006541</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
@@ -8953,7 +8975,7 @@
         <v>0.11538461538461535</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1">
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
@@ -9011,7 +9033,7 @@
         <v>8.9994963062458064E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1">
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
@@ -9069,7 +9091,7 @@
         <v>2.8327529797328291E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1">
+    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
@@ -9127,7 +9149,7 @@
         <v>3.4513531091734205E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1">
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
@@ -9185,7 +9207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1">
+    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
@@ -9243,7 +9265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1">
+    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
@@ -9301,7 +9323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1">
+    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
@@ -9359,7 +9381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="e" vm="16">
         <v>#VALUE!</v>
       </c>
@@ -9417,7 +9439,7 @@
         <v>4.4306757072714587E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:15" hidden="1">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
@@ -9475,7 +9497,7 @@
         <v>2.4148339801638732E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
@@ -9533,7 +9555,7 @@
         <v>1.9918905220476468E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="e" vm="19">
         <v>#VALUE!</v>
       </c>
@@ -9591,7 +9613,7 @@
         <v>4.1428571428571488E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="e" vm="20">
         <v>#VALUE!</v>
       </c>
@@ -9649,7 +9671,7 @@
         <v>3.0125854722029454E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="e" vm="21">
         <v>#VALUE!</v>
       </c>
@@ -9707,7 +9729,7 @@
         <v>2.7251324308416688E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:15" hidden="1">
+    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="e" vm="22">
         <v>#VALUE!</v>
       </c>
@@ -9765,7 +9787,7 @@
         <v>2.3583589171085651E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" hidden="1">
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="e" vm="23">
         <v>#VALUE!</v>
       </c>
@@ -9823,7 +9845,7 @@
         <v>8.9334548769371379E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="e" vm="24">
         <v>#VALUE!</v>
       </c>
@@ -9881,7 +9903,7 @@
         <v>4.2860365441010091E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="e" vm="25">
         <v>#VALUE!</v>
       </c>
@@ -9939,7 +9961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="e" vm="26">
         <v>#VALUE!</v>
       </c>
@@ -9997,7 +10019,7 @@
         <v>0.20768150822302442</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="e" vm="27">
         <v>#VALUE!</v>
       </c>
@@ -10055,7 +10077,7 @@
         <v>2.1440875468639602E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:15" hidden="1">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="e" vm="28">
         <v>#VALUE!</v>
       </c>
@@ -10113,7 +10135,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:15" hidden="1">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="e" vm="29">
         <v>#VALUE!</v>
       </c>
@@ -10171,7 +10193,7 @@
         <v>3.9797293964851106E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
@@ -10229,7 +10251,7 @@
         <v>3.9763792162777971E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:15" hidden="1">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="e" vm="31">
         <v>#VALUE!</v>
       </c>
@@ -10287,7 +10309,7 @@
         <v>1.4131677830419898E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="e" vm="32">
         <v>#VALUE!</v>
       </c>
@@ -10345,7 +10367,7 @@
         <v>9.8080765272142417E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:15" hidden="1">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="e" vm="33">
         <v>#VALUE!</v>
       </c>
@@ -10403,7 +10425,7 @@
         <v>2.6178236397748616E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:15" hidden="1">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
@@ -10461,7 +10483,7 @@
         <v>1.9206377967022924E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:15" hidden="1">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="e" vm="35">
         <v>#VALUE!</v>
       </c>
@@ -10519,7 +10541,7 @@
         <v>1.8207092968061316E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:15" hidden="1">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="e" vm="36">
         <v>#VALUE!</v>
       </c>
@@ -10577,7 +10599,7 @@
         <v>1.7680826636050428E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:15" hidden="1">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="e" vm="37">
         <v>#VALUE!</v>
       </c>
@@ -10635,7 +10657,7 @@
         <v>4.584442472641264E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:15" hidden="1">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="e" vm="38">
         <v>#VALUE!</v>
       </c>
@@ -10693,7 +10715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15" hidden="1">
+    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="e" vm="39">
         <v>#VALUE!</v>
       </c>
@@ -10751,7 +10773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15" hidden="1">
+    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="e" vm="40">
         <v>#VALUE!</v>
       </c>
@@ -10809,7 +10831,7 @@
         <v>3.89855376231383E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:15" hidden="1">
+    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="e" vm="41">
         <v>#VALUE!</v>
       </c>
@@ -10867,7 +10889,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:15" hidden="1">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="e" vm="42">
         <v>#VALUE!</v>
       </c>
@@ -10925,7 +10947,7 @@
         <v>4.1010867732171608E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:15" hidden="1">
+    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="e" vm="43">
         <v>#VALUE!</v>
       </c>
@@ -10983,7 +11005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" hidden="1">
+    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="e" vm="44">
         <v>#VALUE!</v>
       </c>
@@ -11041,7 +11063,7 @@
         <v>1.6793551276308943E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:15" hidden="1">
+    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="e" vm="45">
         <v>#VALUE!</v>
       </c>
@@ -11126,7 +11148,7 @@
       <selection pane="bottomLeft" activeCell="J1" sqref="J1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="56" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" style="56" customWidth="1"/>
@@ -11153,7 +11175,7 @@
     <col min="23" max="16384" width="9.140625" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
         <v>31</v>
       </c>
@@ -11197,7 +11219,7 @@
       <c r="U1" s="57"/>
       <c r="V1" s="57"/>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
         <v>44</v>
       </c>
@@ -11256,7 +11278,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
         <v>54</v>
       </c>
@@ -11296,7 +11318,7 @@
       <c r="U3" s="57"/>
       <c r="V3" s="57"/>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
         <v>56</v>
       </c>
@@ -11336,7 +11358,7 @@
       <c r="U4" s="57"/>
       <c r="V4" s="57"/>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
         <v>58</v>
       </c>
@@ -11380,7 +11402,7 @@
       <c r="U5" s="57"/>
       <c r="V5" s="57"/>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="56" t="s">
         <v>60</v>
       </c>
@@ -11420,7 +11442,7 @@
       <c r="U6" s="57"/>
       <c r="V6" s="57"/>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="56" t="s">
         <v>62</v>
       </c>
@@ -11460,7 +11482,7 @@
       <c r="U7" s="57"/>
       <c r="V7" s="57"/>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
         <v>64</v>
       </c>
@@ -11500,7 +11522,7 @@
       <c r="U8" s="57"/>
       <c r="V8" s="57"/>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="56" t="s">
         <v>66</v>
       </c>
@@ -11540,7 +11562,7 @@
       <c r="U9" s="57"/>
       <c r="V9" s="57"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="s">
         <v>69</v>
       </c>
@@ -11584,7 +11606,7 @@
       <c r="U10" s="57"/>
       <c r="V10" s="57"/>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
         <v>71</v>
       </c>
@@ -11628,7 +11650,7 @@
       <c r="U11" s="57"/>
       <c r="V11" s="57"/>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
         <v>73</v>
       </c>
@@ -11668,7 +11690,7 @@
       <c r="U12" s="57"/>
       <c r="V12" s="57"/>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="56" t="s">
         <v>75</v>
       </c>
@@ -11727,7 +11749,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
         <v>81</v>
       </c>
@@ -11767,7 +11789,7 @@
       <c r="U14" s="57"/>
       <c r="V14" s="57"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="56" t="s">
         <v>83</v>
       </c>
@@ -11807,7 +11829,7 @@
       <c r="U15" s="57"/>
       <c r="V15" s="57"/>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="56" t="s">
         <v>85</v>
       </c>
@@ -11847,7 +11869,7 @@
       <c r="U16" s="57"/>
       <c r="V16" s="57"/>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="56" t="s">
         <v>87</v>
       </c>
@@ -11887,7 +11909,7 @@
       <c r="U17" s="57"/>
       <c r="V17" s="57"/>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="56" t="s">
         <v>89</v>
       </c>
@@ -11931,7 +11953,7 @@
       <c r="U18" s="57"/>
       <c r="V18" s="57"/>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
         <v>91</v>
       </c>
@@ -11971,7 +11993,7 @@
       <c r="U19" s="57"/>
       <c r="V19" s="57"/>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="56" t="s">
         <v>93</v>
       </c>
@@ -12011,7 +12033,7 @@
       <c r="U20" s="57"/>
       <c r="V20" s="57"/>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
         <v>95</v>
       </c>
@@ -12051,7 +12073,7 @@
       <c r="U21" s="57"/>
       <c r="V21" s="57"/>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="56" t="s">
         <v>97</v>
       </c>
@@ -12091,7 +12113,7 @@
       <c r="U22" s="57"/>
       <c r="V22" s="57"/>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="56" t="s">
         <v>99</v>
       </c>
@@ -12131,7 +12153,7 @@
       <c r="U23" s="57"/>
       <c r="V23" s="57"/>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="56" t="s">
         <v>101</v>
       </c>
@@ -12171,7 +12193,7 @@
       <c r="U24" s="57"/>
       <c r="V24" s="57"/>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="56" t="s">
         <v>103</v>
       </c>
@@ -12211,7 +12233,7 @@
       <c r="U25" s="57"/>
       <c r="V25" s="57"/>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="56" t="s">
         <v>105</v>
       </c>
@@ -12264,7 +12286,7 @@
       <c r="U26" s="57"/>
       <c r="V26" s="57"/>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="56" t="s">
         <v>109</v>
       </c>
@@ -12304,7 +12326,7 @@
       <c r="U27" s="57"/>
       <c r="V27" s="57"/>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="56" t="s">
         <v>111</v>
       </c>
@@ -12345,7 +12367,7 @@
       <c r="U28" s="57"/>
       <c r="V28" s="57"/>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="56" t="s">
         <v>113</v>
       </c>
@@ -12386,7 +12408,7 @@
       <c r="U29" s="57"/>
       <c r="V29" s="57"/>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="56" t="s">
         <v>115</v>
       </c>
@@ -12427,7 +12449,7 @@
       <c r="U30" s="57"/>
       <c r="V30" s="57"/>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="56" t="s">
         <v>117</v>
       </c>
@@ -12468,7 +12490,7 @@
       <c r="U31" s="57"/>
       <c r="V31" s="57"/>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="56" t="s">
         <v>119</v>
       </c>
@@ -12509,7 +12531,7 @@
       <c r="U32" s="57"/>
       <c r="V32" s="57"/>
     </row>
-    <row r="33" spans="1:22">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="56" t="s">
         <v>121</v>
       </c>
@@ -12550,7 +12572,7 @@
       <c r="U33" s="57"/>
       <c r="V33" s="57"/>
     </row>
-    <row r="34" spans="1:22">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="56" t="s">
         <v>123</v>
       </c>
@@ -12591,7 +12613,7 @@
       <c r="U34" s="57"/>
       <c r="V34" s="57"/>
     </row>
-    <row r="35" spans="1:22">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="56" t="s">
         <v>125</v>
       </c>
@@ -12635,7 +12657,7 @@
       <c r="U35" s="57"/>
       <c r="V35" s="57"/>
     </row>
-    <row r="36" spans="1:22">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="56" t="s">
         <v>127</v>
       </c>
@@ -12675,7 +12697,7 @@
       <c r="U36" s="57"/>
       <c r="V36" s="57"/>
     </row>
-    <row r="37" spans="1:22">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="56" t="s">
         <v>129</v>
       </c>
@@ -12715,7 +12737,7 @@
       <c r="U37" s="57"/>
       <c r="V37" s="57"/>
     </row>
-    <row r="38" spans="1:22">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="56" t="s">
         <v>131</v>
       </c>
@@ -12755,7 +12777,7 @@
       <c r="U38" s="57"/>
       <c r="V38" s="57"/>
     </row>
-    <row r="39" spans="1:22">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="56" t="s">
         <v>133</v>
       </c>
@@ -12796,7 +12818,7 @@
       <c r="U39" s="57"/>
       <c r="V39" s="57"/>
     </row>
-    <row r="40" spans="1:22">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="56" t="s">
         <v>135</v>
       </c>
@@ -12837,7 +12859,7 @@
       <c r="U40" s="57"/>
       <c r="V40" s="57"/>
     </row>
-    <row r="41" spans="1:22">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="56" t="s">
         <v>137</v>
       </c>
@@ -12878,7 +12900,7 @@
       <c r="U41" s="57"/>
       <c r="V41" s="57"/>
     </row>
-    <row r="42" spans="1:22">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="56" t="s">
         <v>139</v>
       </c>
@@ -12920,7 +12942,7 @@
       </c>
       <c r="V42" s="57"/>
     </row>
-    <row r="43" spans="1:22">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="56" t="s">
         <v>141</v>
       </c>
@@ -12958,7 +12980,7 @@
       </c>
       <c r="V43" s="57"/>
     </row>
-    <row r="44" spans="1:22">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="56" t="s">
         <v>143</v>
       </c>
@@ -12996,7 +13018,7 @@
       </c>
       <c r="V44" s="57"/>
     </row>
-    <row r="45" spans="1:22">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="56" t="s">
         <v>145</v>
       </c>
@@ -13033,7 +13055,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:22">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="56" t="s">
         <v>147</v>
       </c>
@@ -13070,7 +13092,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:22">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="56" t="s">
         <v>149</v>
       </c>
@@ -13111,7 +13133,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:22">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="56" t="s">
         <v>151</v>
       </c>
@@ -13148,7 +13170,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="56" t="s">
         <v>153</v>
       </c>
@@ -13185,7 +13207,7 @@
         <v>2.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="56" t="s">
         <v>155</v>
       </c>
@@ -13222,7 +13244,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="56" t="s">
         <v>157</v>
       </c>
@@ -13259,7 +13281,7 @@
         <v>1.06E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="56" t="s">
         <v>159</v>
       </c>
@@ -13296,7 +13318,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="56" t="s">
         <v>161</v>
       </c>
@@ -13333,7 +13355,7 @@
         <v>1.9199999999999998E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="56" t="s">
         <v>163</v>
       </c>
@@ -13370,7 +13392,7 @@
         <v>1.9800000000000002E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="56" t="s">
         <v>165</v>
       </c>
@@ -13407,7 +13429,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="56" t="s">
         <v>167</v>
       </c>
@@ -13444,7 +13466,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="56" t="s">
         <v>169</v>
       </c>
@@ -13481,7 +13503,7 @@
         <v>3.8699999999999998E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="56" t="s">
         <v>171</v>
       </c>
@@ -13518,7 +13540,7 @@
         <v>2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="56" t="s">
         <v>173</v>
       </c>
@@ -13555,7 +13577,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="56" t="s">
         <v>175</v>
       </c>
@@ -13592,7 +13614,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="56" t="s">
         <v>177</v>
       </c>
@@ -13629,7 +13651,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="56" t="s">
         <v>179</v>
       </c>
@@ -13666,7 +13688,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="56" t="s">
         <v>181</v>
       </c>
@@ -13703,7 +13725,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="56" t="s">
         <v>183</v>
       </c>
@@ -13740,7 +13762,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="56" t="s">
         <v>185</v>
       </c>
@@ -13777,7 +13799,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="56" t="s">
         <v>187</v>
       </c>
@@ -13814,7 +13836,7 @@
         <v>1.15E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="56" t="s">
         <v>189</v>
       </c>
@@ -13851,7 +13873,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="56" t="s">
         <v>191</v>
       </c>
@@ -13888,7 +13910,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="56" t="s">
         <v>193</v>
       </c>
@@ -13925,7 +13947,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="56" t="s">
         <v>195</v>
       </c>
@@ -13962,7 +13984,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="56" t="s">
         <v>197</v>
       </c>
@@ -13999,7 +14021,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="56" t="s">
         <v>199</v>
       </c>
@@ -14036,7 +14058,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="56" t="s">
         <v>201</v>
       </c>
@@ -14073,7 +14095,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="56" t="s">
         <v>203</v>
       </c>
@@ -14110,7 +14132,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="56" t="s">
         <v>205</v>
       </c>
@@ -14147,7 +14169,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="56" t="s">
         <v>207</v>
       </c>
@@ -14184,7 +14206,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="56" t="s">
         <v>209</v>
       </c>
@@ -14217,7 +14239,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="56" t="s">
         <v>210</v>
       </c>
@@ -14250,7 +14272,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="56" t="s">
         <v>212</v>
       </c>
@@ -14283,7 +14305,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="56" t="s">
         <v>214</v>
       </c>
@@ -14316,7 +14338,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="56" t="s">
         <v>216</v>
       </c>
@@ -14349,7 +14371,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="56" t="s">
         <v>218</v>
       </c>
@@ -14382,7 +14404,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="56" t="s">
         <v>220</v>
       </c>
@@ -14415,7 +14437,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="56" t="s">
         <v>222</v>
       </c>
@@ -14448,7 +14470,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="56" t="s">
         <v>224</v>
       </c>
@@ -14481,7 +14503,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="56" t="s">
         <v>226</v>
       </c>
@@ -14514,7 +14536,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="56" t="s">
         <v>228</v>
       </c>
@@ -14547,7 +14569,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="56" t="s">
         <v>230</v>
       </c>
@@ -14580,7 +14602,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="56" t="s">
         <v>232</v>
       </c>
@@ -14613,7 +14635,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="56" t="s">
         <v>234</v>
       </c>
@@ -14646,7 +14668,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="56" t="s">
         <v>236</v>
       </c>
@@ -14679,7 +14701,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="56" t="s">
         <v>238</v>
       </c>
@@ -14712,7 +14734,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="56" t="s">
         <v>240</v>
       </c>
@@ -14745,7 +14767,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="56" t="s">
         <v>242</v>
       </c>
@@ -14778,7 +14800,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="56" t="s">
         <v>244</v>
       </c>
@@ -14811,7 +14833,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="56" t="s">
         <v>246</v>
       </c>
@@ -14844,7 +14866,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="97" spans="1:13">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="56" t="s">
         <v>248</v>
       </c>
@@ -14873,7 +14895,7 @@
         <v>6.2799999999999995E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="56" t="s">
         <v>250</v>
       </c>
@@ -14902,7 +14924,7 @@
         <v>7.9200000000000007E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="56" t="s">
         <v>252</v>
       </c>
@@ -14931,7 +14953,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="56" t="s">
         <v>254</v>
       </c>
@@ -14960,7 +14982,7 @@
         <v>3.6600000000000001E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="56" t="s">
         <v>256</v>
       </c>
@@ -14989,7 +15011,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="56" t="s">
         <v>258</v>
       </c>
@@ -15018,7 +15040,7 @@
         <v>9.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="56" t="s">
         <v>260</v>
       </c>
@@ -15047,7 +15069,7 @@
         <v>1.5800000000000002E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="56" t="s">
         <v>262</v>
       </c>
@@ -15076,7 +15098,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="56" t="s">
         <v>264</v>
       </c>
@@ -15105,7 +15127,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="56" t="s">
         <v>266</v>
       </c>
@@ -15134,7 +15156,7 @@
         <v>2.6100000000000002E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:13">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="56" t="s">
         <v>268</v>
       </c>
@@ -15163,7 +15185,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="108" spans="1:13">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="56" t="s">
         <v>270</v>
       </c>
@@ -15192,7 +15214,7 @@
         <v>1.66E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:13">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="56" t="s">
         <v>272</v>
       </c>
@@ -15221,7 +15243,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="110" spans="1:13">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="56" t="s">
         <v>274</v>
       </c>
@@ -15250,7 +15272,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="111" spans="1:13">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" s="56" t="s">
         <v>276</v>
       </c>
@@ -15279,7 +15301,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="112" spans="1:13">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" s="56" t="s">
         <v>278</v>
       </c>
@@ -15308,7 +15330,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="113" spans="1:13">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" s="56" t="s">
         <v>280</v>
       </c>
@@ -15337,7 +15359,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="114" spans="1:13">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="56" t="s">
         <v>282</v>
       </c>
@@ -15366,7 +15388,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:13">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="56" t="s">
         <v>284</v>
       </c>
@@ -15395,7 +15417,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="116" spans="1:13">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="56" t="s">
         <v>286</v>
       </c>
@@ -15424,7 +15446,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="117" spans="1:13">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="56" t="s">
         <v>288</v>
       </c>
@@ -15453,7 +15475,7 @@
         <v>1.6400000000000001E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:13">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="56" t="s">
         <v>290</v>
       </c>
@@ -15482,7 +15504,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="119" spans="1:13">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="56" t="s">
         <v>292</v>
       </c>
@@ -15511,7 +15533,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="120" spans="1:13">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="56" t="s">
         <v>294</v>
       </c>
@@ -15540,7 +15562,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="121" spans="1:13">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" s="56" t="s">
         <v>296</v>
       </c>
@@ -15569,7 +15591,7 @@
         <v>6.3E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:13">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" s="56" t="s">
         <v>298</v>
       </c>
@@ -15598,7 +15620,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="123" spans="1:13">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" s="56" t="s">
         <v>300</v>
       </c>
@@ -15627,7 +15649,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" s="57" t="s">
         <v>302</v>
       </c>
@@ -15656,7 +15678,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="125" spans="1:13">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" s="57" t="s">
         <v>304</v>
       </c>
@@ -15685,7 +15707,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="126" spans="1:13">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" s="57" t="s">
         <v>306</v>
       </c>
@@ -15714,7 +15736,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="127" spans="1:13">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" s="57" t="s">
         <v>308</v>
       </c>
@@ -15743,7 +15765,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="128" spans="1:13">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" s="57" t="s">
         <v>310</v>
       </c>
@@ -15772,7 +15794,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="129" spans="1:13">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="57" t="s">
         <v>312</v>
       </c>
@@ -15801,7 +15823,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="130" spans="1:13">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="57" t="s">
         <v>314</v>
       </c>
@@ -15830,7 +15852,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="131" spans="1:13">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="56" t="s">
         <v>316</v>
       </c>
@@ -15859,7 +15881,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="132" spans="1:13">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="56" t="s">
         <v>318</v>
       </c>
@@ -15910,7 +15932,7 @@
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -15925,7 +15947,7 @@
     <col min="15" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15969,7 +15991,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="e" vm="46">
         <v>#VALUE!</v>
       </c>
@@ -16023,7 +16045,7 @@
         <v>0.17977528089887637</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="e" vm="47">
         <v>#VALUE!</v>
       </c>
@@ -16077,7 +16099,7 @@
         <v>0.11481317934782616</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="e" vm="48">
         <v>#VALUE!</v>
       </c>
@@ -16131,7 +16153,7 @@
         <v>0.52456621004566206</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="e" vm="49">
         <v>#VALUE!</v>
       </c>
@@ -16185,7 +16207,7 @@
         <v>0.31760918253079506</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="e" vm="50">
         <v>#VALUE!</v>
       </c>
@@ -16239,7 +16261,7 @@
         <v>0.30226789510985114</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="e" vm="51">
         <v>#VALUE!</v>
       </c>
@@ -16290,7 +16312,7 @@
         <v>0.19640778313653753</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="e" vm="52">
         <v>#VALUE!</v>
       </c>
@@ -16341,7 +16363,7 @@
         <v>1.0860056110289971E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="e" vm="53">
         <v>#VALUE!</v>
       </c>
@@ -16394,7 +16416,7 @@
         <v>0.30081541582150101</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="e" vm="54">
         <v>#VALUE!</v>
       </c>
@@ -16448,7 +16470,7 @@
         <v>0.65314180107526876</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="e" vm="55">
         <v>#VALUE!</v>
       </c>
@@ -16502,7 +16524,7 @@
         <v>0.47424845269672861</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="e" vm="56">
         <v>#VALUE!</v>
       </c>
@@ -16556,7 +16578,7 @@
         <v>0.43308865047995482</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="e" vm="57">
         <v>#VALUE!</v>
       </c>
@@ -16610,7 +16632,7 @@
         <v>0.39534257638982367</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="e" vm="58">
         <v>#VALUE!</v>
       </c>
@@ -16664,7 +16686,7 @@
         <v>0.23565984757320499</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="e" vm="59">
         <v>#VALUE!</v>
       </c>
@@ -16718,7 +16740,7 @@
         <v>0.68897317298797411</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="e" vm="60">
         <v>#VALUE!</v>
       </c>
@@ -16772,7 +16794,7 @@
         <v>0.49615575936577022</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="e" vm="61">
         <v>#VALUE!</v>
       </c>
@@ -16826,7 +16848,7 @@
         <v>0.4397489949995097</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="e" vm="62">
         <v>#VALUE!</v>
       </c>
@@ -16880,7 +16902,7 @@
         <v>0.429585798816568</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="e" vm="63">
         <v>#VALUE!</v>
       </c>
@@ -16934,7 +16956,7 @@
         <v>0.39594816028601221</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="e" vm="64">
         <v>#VALUE!</v>
       </c>
@@ -16987,7 +17009,7 @@
         <v>0.37653136531365311</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="e" vm="65">
         <v>#VALUE!</v>
       </c>
@@ -17041,7 +17063,7 @@
         <v>0.28739763779527555</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="e" vm="66">
         <v>#VALUE!</v>
       </c>
@@ -17095,7 +17117,7 @@
         <v>0.48044096728307256</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="e" vm="67">
         <v>#VALUE!</v>
       </c>
@@ -17149,7 +17171,7 @@
         <v>0.10314068017097201</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="e" vm="68">
         <v>#VALUE!</v>
       </c>
@@ -17203,7 +17225,7 @@
         <v>8.6445783132530124E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="e" vm="69">
         <v>#VALUE!</v>
       </c>
@@ -17257,7 +17279,7 @@
         <v>7.1739859202145035E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="e" vm="70">
         <v>#VALUE!</v>
       </c>
@@ -17325,13 +17347,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13513A75-7FB1-4B44-A9EF-B1F8874E7B1E}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
@@ -17347,7 +17369,7 @@
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -17367,7 +17389,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -17389,7 +17411,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -17411,7 +17433,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -17433,7 +17455,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -17455,7 +17477,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -17477,7 +17499,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -17499,7 +17521,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -17521,7 +17543,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -17543,7 +17565,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -17565,7 +17587,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -17587,7 +17609,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>348</v>
       </c>
@@ -17606,7 +17628,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>2</v>
       </c>
@@ -17626,7 +17648,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>349</v>
       </c>
@@ -17648,7 +17670,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>349</v>
       </c>
@@ -17670,7 +17692,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>349</v>
       </c>
@@ -17692,7 +17714,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>349</v>
       </c>
@@ -17714,7 +17736,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>349</v>
       </c>
@@ -17736,7 +17758,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>349</v>
       </c>
@@ -17758,7 +17780,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>349</v>
       </c>
@@ -17780,7 +17802,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>348</v>
       </c>
@@ -17799,14 +17821,14 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="18.75">
+    <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="85" t="s">
         <v>359</v>
       </c>
       <c r="B28" s="85"/>
       <c r="C28" s="85"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>360</v>
       </c>
@@ -17817,7 +17839,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>363</v>
       </c>
@@ -17826,7 +17848,7 @@
       </c>
       <c r="C30" s="12"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>365</v>
       </c>
@@ -17835,7 +17857,7 @@
       </c>
       <c r="C31" s="12"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>366</v>
       </c>
@@ -17844,7 +17866,7 @@
       </c>
       <c r="C32" s="12"/>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>367</v>
       </c>
@@ -17853,7 +17875,7 @@
       </c>
       <c r="C33" s="12"/>
     </row>
-    <row r="34" spans="1:3" ht="60">
+    <row r="34" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>368</v>
       </c>
@@ -17864,7 +17886,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="60">
+    <row r="35" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>371</v>
       </c>
@@ -17875,7 +17897,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>80</v>
       </c>
@@ -17886,7 +17908,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
@@ -17897,7 +17919,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>376</v>
       </c>
@@ -17905,6 +17927,35 @@
         <v>377</v>
       </c>
       <c r="C38" s="12"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C39" s="12"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C40" s="12"/>
+    </row>
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>436</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -17923,14 +17974,14 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9442434-AE3F-49F6-94ED-A6D1C7BB92DA}">
-  <dimension ref="A1:AK40"/>
+  <dimension ref="A1:AK41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="12.75" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="12.75" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.140625" style="21" customWidth="1"/>
     <col min="2" max="2" width="15.140625" style="21" bestFit="1" customWidth="1"/>
@@ -17950,7 +18001,7 @@
     <col min="37" max="16384" width="10.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="46" customFormat="1" ht="29.25" customHeight="1">
+    <row r="1" spans="1:37" s="46" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>4</v>
       </c>
@@ -18060,7 +18111,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" s="47" t="s">
         <v>29</v>
       </c>
@@ -18144,7 +18195,7 @@
         <v>0.05</v>
       </c>
       <c r="Y2" s="50">
-        <f t="shared" ref="Y2:Y23" si="2">X2*1000</f>
+        <f t="shared" ref="Y2:Y22" si="2">X2*1000</f>
         <v>50</v>
       </c>
       <c r="Z2" s="50">
@@ -18196,7 +18247,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" s="47" t="s">
         <v>29</v>
       </c>
@@ -18284,7 +18335,7 @@
         <v>45</v>
       </c>
       <c r="Z3" s="50">
-        <f t="shared" ref="Z3:Z23" si="8">Y3*12</f>
+        <f t="shared" ref="Z3:Z22" si="8">Y3*12</f>
         <v>540</v>
       </c>
       <c r="AA3" s="51">
@@ -18332,7 +18383,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>331</v>
       </c>
@@ -18468,7 +18519,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>331</v>
       </c>
@@ -18604,7 +18655,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>331</v>
       </c>
@@ -18740,7 +18791,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7" s="47" t="s">
         <v>28</v>
       </c>
@@ -18876,7 +18927,7 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8" s="47" t="s">
         <v>28</v>
       </c>
@@ -19012,7 +19063,7 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>20</v>
       </c>
@@ -19148,7 +19199,7 @@
         <v>5040</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>20</v>
       </c>
@@ -19284,7 +19335,7 @@
         <v>5040</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11" s="47" t="s">
         <v>401</v>
       </c>
@@ -19420,7 +19471,7 @@
         <v>4320</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>334</v>
       </c>
@@ -19556,7 +19607,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>334</v>
       </c>
@@ -19692,7 +19743,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A14" s="47" t="s">
         <v>18</v>
       </c>
@@ -19828,7 +19879,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A15" s="52" t="s">
         <v>18</v>
       </c>
@@ -19964,7 +20015,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>406</v>
       </c>
@@ -20100,7 +20151,7 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>406</v>
       </c>
@@ -20236,7 +20287,7 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A18" s="47" t="s">
         <v>30</v>
       </c>
@@ -20372,7 +20423,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A19" s="47" t="s">
         <v>30</v>
       </c>
@@ -20508,7 +20559,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A20" s="47" t="s">
         <v>30</v>
       </c>
@@ -20644,7 +20695,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>346</v>
       </c>
@@ -20780,7 +20831,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
         <v>346</v>
       </c>
@@ -20916,7 +20967,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
         <v>414</v>
       </c>
@@ -20991,7 +21042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
         <v>414</v>
       </c>
@@ -21037,7 +21088,7 @@
       <c r="AJ24" s="38"/>
       <c r="AK24" s="38"/>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
         <v>414</v>
       </c>
@@ -21083,7 +21134,7 @@
       <c r="AJ25" s="38"/>
       <c r="AK25" s="38"/>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A26" s="24" t="s">
         <v>348</v>
       </c>
@@ -21137,65 +21188,70 @@
         <v>120600</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Q27" s="83">
         <f>Q26-R26</f>
         <v>196556.03502084804</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A31" s="21" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="84" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="84" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="21" t="s">
         <v>421</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="21" t="s">
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -21215,14 +21271,14 @@
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="5" width="9.140625" style="28"/>
     <col min="6" max="6" width="10.7109375" style="28" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="29"/>
       <c r="B1" s="29" t="s">
         <v>425</v>
@@ -21240,7 +21296,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="27"/>
       <c r="B2" s="30">
         <v>78.319999999999993</v>
@@ -21257,7 +21313,7 @@
         <v>0.37198333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="27"/>
       <c r="B3" s="30">
         <v>84.28</v>
@@ -21274,7 +21330,7 @@
         <v>0.47854999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="27"/>
       <c r="B4" s="30">
         <v>74.39</v>
@@ -21291,7 +21347,7 @@
         <v>0.43246666666666672</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="27"/>
       <c r="B5" s="30"/>
       <c r="C5" s="30"/>
@@ -21302,7 +21358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -21313,7 +21369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="55" t="s">
         <v>429</v>
       </c>
@@ -21331,18 +21387,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21569,13 +21625,45 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401ADED5-CC5A-4072-B36A-6DA217C5A368}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DB5870C-189D-475E-8E58-449C30115ACA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DB5870C-189D-475E-8E58-449C30115ACA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401ADED5-CC5A-4072-B36A-6DA217C5A368}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e8f9595b-0d5a-46b2-8488-c972c1ea4246"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6bcbbac3-d60f-4c54-b2b4-d245c065548d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11321DBA-FDAB-45E8-A045-E3E44A7AE235}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11321DBA-FDAB-45E8-A045-E3E44A7AE235}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e8f9595b-0d5a-46b2-8488-c972c1ea4246"/>
+    <ds:schemaRef ds:uri="6bcbbac3-d60f-4c54-b2b4-d245c065548d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated ira strategy in watchlist
</commit_message>
<xml_diff>
--- a/input/Watchlist.xlsx
+++ b/input/Watchlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssoma\OneDrive - Bayer\Personal Data-R90PQ30R\Analytics\us-stocks-analysis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="722" documentId="13_ncr:1_{A259AFBD-2F1F-43A4-8040-58927886A03B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{376AC5B9-1E05-4AE5-9879-C994D2D2AA88}"/>
+  <xr:revisionPtr revIDLastSave="724" documentId="13_ncr:1_{A259AFBD-2F1F-43A4-8040-58927886A03B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{485B905D-B7D0-4474-ADD9-EE244A370B1C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fund List" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="21" r:id="rId9"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -789,7 +789,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="536">
   <si>
     <t>Funds</t>
   </si>
@@ -2391,6 +2391,12 @@
   </si>
   <si>
     <t>ISHARES MSCI EMERGING MARKETS ASIA ETF</t>
+  </si>
+  <si>
+    <t>FSKAX (10%), FZROX (6%)</t>
+  </si>
+  <si>
+    <t>FXAIX (10%), FNILX (6%)</t>
   </si>
 </sst>
 </file>
@@ -2405,7 +2411,7 @@
     <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="170" formatCode="0.0%"/>
-    <numFmt numFmtId="173" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -2865,14 +2871,11 @@
     <xf numFmtId="167" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2881,7 +2884,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="4" fillId="13" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="4" fillId="13" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="4" fillId="13" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="13" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="14" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2894,7 +2897,7 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="13" fillId="13" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="13" fillId="13" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="13" fillId="13" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="13" fillId="13" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="13" fillId="14" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2916,6 +2919,9 @@
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -2923,60 +2929,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="39">
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
@@ -3299,6 +3252,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -3596,6 +3559,26 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -4077,7 +4060,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{03CB7FE0-41D1-435D-B030-06F23C6C3345}" name="PivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{03CB7FE0-41D1-435D-B030-06F23C6C3345}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="P3:Q12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="3">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -4184,7 +4167,7 @@
     <dataField name="Sum of Percent" fld="1" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="6">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -9350,48 +9333,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{69112644-6D4F-4AA0-8CCC-1CEE1E0148D7}" name="Table1" displayName="Table1" ref="A1:O48" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{69112644-6D4F-4AA0-8CCC-1CEE1E0148D7}" name="Table1" displayName="Table1" ref="A1:O48" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="A1:O48" xr:uid="{95189E96-064D-425D-BE39-47B18B49F5F0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O46">
     <sortCondition ref="E2:E46"/>
     <sortCondition descending="1" ref="O2:O46"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{BB2FF6EB-53FD-4E78-BD0B-C24026A8DB98}" name="Funds" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{B45FB7AC-F148-421D-9B37-4E7E7D8C8E6A}" name="Ticker" dataDxfId="38">
+    <tableColumn id="1" xr3:uid="{BB2FF6EB-53FD-4E78-BD0B-C24026A8DB98}" name="Funds" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{B45FB7AC-F148-421D-9B37-4E7E7D8C8E6A}" name="Ticker" dataDxfId="33">
       <calculatedColumnFormula array="1">_FV(A2,"Ticker symbol",TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0E04398C-EA9A-4618-BD02-DA8ABAA2CF7C}" name="Account" dataDxfId="37"/>
-    <tableColumn id="10" xr3:uid="{07652F3D-BD92-4EA5-B3CD-C8CA26C51045}" name="Portfolio" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{84FCDA56-42CA-4155-A371-09849AF21EE5}" name="Bucket" dataDxfId="35"/>
-    <tableColumn id="14" xr3:uid="{4B646908-1DAD-4E96-87A0-816CCAEC36A5}" name="Expense Ratio" dataDxfId="34">
+    <tableColumn id="3" xr3:uid="{0E04398C-EA9A-4618-BD02-DA8ABAA2CF7C}" name="Account" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{07652F3D-BD92-4EA5-B3CD-C8CA26C51045}" name="Portfolio" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{84FCDA56-42CA-4155-A371-09849AF21EE5}" name="Bucket" dataDxfId="30"/>
+    <tableColumn id="14" xr3:uid="{4B646908-1DAD-4E96-87A0-816CCAEC36A5}" name="Expense Ratio" dataDxfId="29">
       <calculatedColumnFormula>IFERROR(_FV(A2,"Expense ratio",TRUE),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{315E67EE-D83C-47DE-877C-398E379B6F15}" name="Open" dataDxfId="33" dataCellStyle="Currency">
+    <tableColumn id="5" xr3:uid="{315E67EE-D83C-47DE-877C-398E379B6F15}" name="Open" dataDxfId="28" dataCellStyle="Currency">
       <calculatedColumnFormula array="1">IFERROR(_FV(A2,"Open"),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{94216B5A-94A5-40EA-8CFA-BB6BCBAE0B5C}" name="High" dataDxfId="32" dataCellStyle="Currency">
+    <tableColumn id="6" xr3:uid="{94216B5A-94A5-40EA-8CFA-BB6BCBAE0B5C}" name="High" dataDxfId="27" dataCellStyle="Currency">
       <calculatedColumnFormula array="1">IFERROR(_FV(A2,"High"),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0995BD2E-CC80-4453-962B-4B371F66AD96}" name="Low" dataDxfId="31" dataCellStyle="Currency">
+    <tableColumn id="7" xr3:uid="{0995BD2E-CC80-4453-962B-4B371F66AD96}" name="Low" dataDxfId="26" dataCellStyle="Currency">
       <calculatedColumnFormula array="1">IFERROR(_FV(A2,"Low"),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{59B32FD1-E741-455C-AB3F-CC8305A4082D}" name="Close" dataDxfId="30" dataCellStyle="Currency">
+    <tableColumn id="8" xr3:uid="{59B32FD1-E741-455C-AB3F-CC8305A4082D}" name="Close" dataDxfId="25" dataCellStyle="Currency">
       <calculatedColumnFormula array="1">IFERROR(_FV(A2,"Price"),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{B7EF52F1-C3EC-4E9C-9810-4A9443FB6AC8}" name="Bid Price" dataDxfId="29" dataCellStyle="Currency">
+    <tableColumn id="15" xr3:uid="{B7EF52F1-C3EC-4E9C-9810-4A9443FB6AC8}" name="Bid Price" dataDxfId="24" dataCellStyle="Currency">
       <calculatedColumnFormula>IFERROR((Table1[[#This Row],[Close]]+Table1[[#This Row],[Low]])/2,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{BFFB38B1-DFB9-43B1-881D-A7371E276BF4}" name="Change (%)" dataDxfId="28">
+    <tableColumn id="9" xr3:uid="{BFFB38B1-DFB9-43B1-881D-A7371E276BF4}" name="Change (%)" dataDxfId="23">
       <calculatedColumnFormula array="1">IFERROR(_FV(A2,"Change (%)",TRUE),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{FBDD8949-4F7E-41F5-AC1F-CA98CC4626EE}" name="52 week high" dataDxfId="27" dataCellStyle="Currency">
+    <tableColumn id="11" xr3:uid="{FBDD8949-4F7E-41F5-AC1F-CA98CC4626EE}" name="52 week high" dataDxfId="22" dataCellStyle="Currency">
       <calculatedColumnFormula>IFERROR(_FV(Table1[[#This Row],[Funds]],"52 week high",TRUE),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{CD345540-5848-4748-B639-D5DB23BDEE94}" name="52 week low" dataDxfId="26" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{CD345540-5848-4748-B639-D5DB23BDEE94}" name="52 week low" dataDxfId="21" dataCellStyle="Currency">
       <calculatedColumnFormula>IFERROR(_FV(Table1[[#This Row],[Funds]],"52 week low",TRUE),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D10DB507-EF50-48A6-9A07-64B0D17CC79B}" name="Deviation from 52 Week High" dataDxfId="25" dataCellStyle="Percent">
+    <tableColumn id="13" xr3:uid="{D10DB507-EF50-48A6-9A07-64B0D17CC79B}" name="Deviation from 52 Week High" dataDxfId="20" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR((M2-J2)/M2,"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9400,45 +9383,45 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D0CAA086-D84C-4EA4-B5F1-7030749A7F3E}" name="Table13" displayName="Table13" ref="A1:N26" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D0CAA086-D84C-4EA4-B5F1-7030749A7F3E}" name="Table13" displayName="Table13" ref="A1:N26" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A1:N26" xr:uid="{7148AA24-1D57-4322-B6E6-30CB6857B1C8}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N26">
     <sortCondition ref="F2:F26"/>
     <sortCondition descending="1" ref="N2:N26"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{57268FAB-0DAA-4F5F-B46D-3806B1FBF806}" name="Funds" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{A08DC65A-57D6-483A-BC4A-A7473C7F025B}" name="Ticker" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{57268FAB-0DAA-4F5F-B46D-3806B1FBF806}" name="Funds" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{A08DC65A-57D6-483A-BC4A-A7473C7F025B}" name="Ticker" dataDxfId="15">
       <calculatedColumnFormula array="1">_FV(A2,"Ticker symbol",TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B68D1E78-2858-40F0-938D-30A7BD84787D}" name="Account" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{15A75516-1C6A-4B58-B9D6-851E503B9FB8}" name="Bucket" dataDxfId="19"/>
-    <tableColumn id="15" xr3:uid="{47D0498E-EC1F-4FEA-A214-7DB4FEA6AF04}" name="Sector" dataDxfId="18"/>
-    <tableColumn id="14" xr3:uid="{B112A09B-C1DB-49F3-8BB2-F1FCBE93700E}" name="Industry" dataDxfId="17">
+    <tableColumn id="3" xr3:uid="{B68D1E78-2858-40F0-938D-30A7BD84787D}" name="Account" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{15A75516-1C6A-4B58-B9D6-851E503B9FB8}" name="Bucket" dataDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{47D0498E-EC1F-4FEA-A214-7DB4FEA6AF04}" name="Sector" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{B112A09B-C1DB-49F3-8BB2-F1FCBE93700E}" name="Industry" dataDxfId="11">
       <calculatedColumnFormula array="1">_FV(A2,"Industry")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{0FA6A548-B1BE-4B6C-B4B8-163F5654ABD5}" name="Open" dataDxfId="16">
+    <tableColumn id="5" xr3:uid="{0FA6A548-B1BE-4B6C-B4B8-163F5654ABD5}" name="Open" dataDxfId="10">
       <calculatedColumnFormula array="1">_FV(A2,"Open")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B8CB571D-5B2B-453B-82BA-5EA66AB797D7}" name="High" dataDxfId="15">
+    <tableColumn id="6" xr3:uid="{B8CB571D-5B2B-453B-82BA-5EA66AB797D7}" name="High" dataDxfId="9">
       <calculatedColumnFormula array="1">_FV(A2,"High")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F44149AE-6680-4B2A-93F2-98C9F6507E5A}" name="Low" dataDxfId="14">
+    <tableColumn id="7" xr3:uid="{F44149AE-6680-4B2A-93F2-98C9F6507E5A}" name="Low" dataDxfId="8">
       <calculatedColumnFormula array="1">_FV(A2,"Low")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{EE5B9F16-BFFA-4732-8F70-E2D37CF19600}" name="Close" dataDxfId="13">
+    <tableColumn id="8" xr3:uid="{EE5B9F16-BFFA-4732-8F70-E2D37CF19600}" name="Close" dataDxfId="7">
       <calculatedColumnFormula array="1">_FV(A2,"Price")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{2DE1F60D-5DEF-405B-808F-FEA1CD488B45}" name="Change (%)" dataDxfId="12">
+    <tableColumn id="9" xr3:uid="{2DE1F60D-5DEF-405B-808F-FEA1CD488B45}" name="Change (%)" dataDxfId="6">
       <calculatedColumnFormula array="1">_FV(A2,"Change (%)",TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{AF24AD6C-48A4-4E24-9504-7E6E23ABFAFF}" name="52 week high" dataDxfId="11">
+    <tableColumn id="11" xr3:uid="{AF24AD6C-48A4-4E24-9504-7E6E23ABFAFF}" name="52 week high" dataDxfId="5">
       <calculatedColumnFormula array="1">_FV(Table13[[#This Row],[Funds]],"52 week high",TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{C74C9A6D-67EB-491D-A6D1-55C66BF936BE}" name="52 week low" dataDxfId="10">
+    <tableColumn id="12" xr3:uid="{C74C9A6D-67EB-491D-A6D1-55C66BF936BE}" name="52 week low" dataDxfId="4">
       <calculatedColumnFormula array="1">_FV(Table13[[#This Row],[Funds]],"52 week low",TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{79973E41-98D9-4950-8B9A-E0B263B075E3}" name="Deviation from 52 Week High" dataDxfId="9">
+    <tableColumn id="13" xr3:uid="{79973E41-98D9-4950-8B9A-E0B263B075E3}" name="Deviation from 52 Week High" dataDxfId="3">
       <calculatedColumnFormula>(L2-J2)/L2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9451,8 +9434,8 @@
   <autoFilter ref="A29:C39" xr:uid="{76A2AC23-EA1A-42A9-A4A0-BA4126640B6B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C5A951EA-02C9-4EEA-B580-3EE51E7FDF81}" name="Fund"/>
-    <tableColumn id="2" xr3:uid="{EDFF81EE-5847-4637-99DE-F7A607DAE56F}" name="Category" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{FE5FE4F2-8EE0-4222-A1A6-C6369FAE2A5F}" name="Notes" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{EDFF81EE-5847-4637-99DE-F7A607DAE56F}" name="Category" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{FE5FE4F2-8EE0-4222-A1A6-C6369FAE2A5F}" name="Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9757,8 +9740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12438,7 +12421,7 @@
       <c r="A47" s="14" t="e" vm="46">
         <v>#VALUE!</v>
       </c>
-      <c r="B47" s="116" t="str">
+      <c r="B47" s="115" t="str">
         <f t="array" ref="B47">_FV(A47,"Ticker symbol",TRUE)</f>
         <v>FPBFX</v>
       </c>
@@ -12451,52 +12434,52 @@
       <c r="E47" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="F47" s="91">
+      <c r="F47" s="90">
         <f>IFERROR(_FV(A47,"Expense ratio",TRUE),"")</f>
         <v>1.11E-2</v>
       </c>
-      <c r="G47" s="117" t="str">
+      <c r="G47" s="116" t="str">
         <f t="array" ref="G47">IFERROR(_FV(A47,"Open"),"")</f>
         <v/>
       </c>
-      <c r="H47" s="117" t="str">
+      <c r="H47" s="116" t="str">
         <f t="array" ref="H47">IFERROR(_FV(A47,"High"),"")</f>
         <v/>
       </c>
-      <c r="I47" s="117" t="str">
+      <c r="I47" s="116" t="str">
         <f t="array" ref="I47">IFERROR(_FV(A47,"Low"),"")</f>
         <v/>
       </c>
-      <c r="J47" s="117">
+      <c r="J47" s="116">
         <f t="array" ref="J47">IFERROR(_FV(A47,"Price"),"")</f>
         <v>38.18</v>
       </c>
-      <c r="K47" s="118" t="str">
+      <c r="K47" s="117" t="str">
         <f>IFERROR((Table1[[#This Row],[Close]]+Table1[[#This Row],[Low]])/2,"")</f>
         <v/>
       </c>
-      <c r="L47" s="91">
+      <c r="L47" s="90">
         <f t="array" ref="L47">IFERROR(_FV(A47,"Change (%)",TRUE),"")</f>
         <v>3.1530000000000004E-3</v>
       </c>
-      <c r="M47" s="117" t="str">
+      <c r="M47" s="116" t="str">
         <f>IFERROR(_FV(Table1[[#This Row],[Funds]],"52 week high",TRUE),"")</f>
         <v/>
       </c>
-      <c r="N47" s="117" t="str">
+      <c r="N47" s="116" t="str">
         <f>IFERROR(_FV(Table1[[#This Row],[Funds]],"52 week low",TRUE),"")</f>
         <v/>
       </c>
-      <c r="O47" s="92" t="str">
+      <c r="O47" s="91" t="str">
         <f>IFERROR((M47-J47)/M47,"")</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="119" t="e" vm="47">
+      <c r="A48" s="118" t="e" vm="47">
         <v>#VALUE!</v>
       </c>
-      <c r="B48" s="120" t="str">
+      <c r="B48" s="119" t="str">
         <f t="array" ref="B48">_FV(A48,"Ticker symbol",TRUE)</f>
         <v>FIGFX</v>
       </c>
@@ -12509,53 +12492,53 @@
       <c r="E48" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="F48" s="121">
+      <c r="F48" s="120">
         <f>IFERROR(_FV(A48,"Expense ratio",TRUE),"")</f>
         <v>1.03E-2</v>
       </c>
-      <c r="G48" s="122" t="str">
+      <c r="G48" s="121" t="str">
         <f t="array" ref="G48">IFERROR(_FV(A48,"Open"),"")</f>
         <v/>
       </c>
-      <c r="H48" s="122" t="str">
+      <c r="H48" s="121" t="str">
         <f t="array" ref="H48">IFERROR(_FV(A48,"High"),"")</f>
         <v/>
       </c>
-      <c r="I48" s="122" t="str">
+      <c r="I48" s="121" t="str">
         <f t="array" ref="I48">IFERROR(_FV(A48,"Low"),"")</f>
         <v/>
       </c>
-      <c r="J48" s="122">
+      <c r="J48" s="121">
         <f t="array" ref="J48">IFERROR(_FV(A48,"Price"),"")</f>
         <v>16.579999999999998</v>
       </c>
-      <c r="K48" s="123" t="str">
+      <c r="K48" s="122" t="str">
         <f>IFERROR((Table1[[#This Row],[Close]]+Table1[[#This Row],[Low]])/2,"")</f>
         <v/>
       </c>
-      <c r="L48" s="121">
+      <c r="L48" s="120">
         <f t="array" ref="L48">IFERROR(_FV(A48,"Change (%)",TRUE),"")</f>
         <v>7.9030000000000003E-3</v>
       </c>
-      <c r="M48" s="122" t="str">
+      <c r="M48" s="121" t="str">
         <f>IFERROR(_FV(Table1[[#This Row],[Funds]],"52 week high",TRUE),"")</f>
         <v/>
       </c>
-      <c r="N48" s="122" t="str">
+      <c r="N48" s="121" t="str">
         <f>IFERROR(_FV(Table1[[#This Row],[Funds]],"52 week low",TRUE),"")</f>
         <v/>
       </c>
-      <c r="O48" s="124" t="str">
+      <c r="O48" s="123" t="str">
         <f>IFERROR((M48-J48)/M48,"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A48">
-    <cfRule type="duplicateValues" dxfId="4" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="14"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -18761,7 +18744,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -18778,8 +18761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13513A75-7FB1-4B44-A9EF-B1F8874E7B1E}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19085,7 +19068,7 @@
         <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>350</v>
+        <v>534</v>
       </c>
       <c r="D17" s="3">
         <v>0.16</v>
@@ -19107,7 +19090,7 @@
         <v>331</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>351</v>
+        <v>535</v>
       </c>
       <c r="D18" s="3">
         <v>0.16</v>
@@ -19251,11 +19234,11 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="90" t="s">
+      <c r="A28" s="124" t="s">
         <v>359</v>
       </c>
-      <c r="B28" s="90"/>
-      <c r="C28" s="90"/>
+      <c r="B28" s="124"/>
+      <c r="C28" s="124"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -19388,7 +19371,7 @@
   <dimension ref="A1:AK43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -22603,7 +22586,7 @@
         <v>0</v>
       </c>
       <c r="Z25" s="32">
-        <f t="shared" ref="Z25:Z26" si="63">Y25*12</f>
+        <f t="shared" ref="Z25" si="63">Y25*12</f>
         <v>0</v>
       </c>
       <c r="AA25" s="33">
@@ -23457,1069 +23440,1069 @@
   <cols>
     <col min="1" max="1" width="9.140625" style="14"/>
     <col min="2" max="2" width="48.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="93" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="95" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="94" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="93" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" style="95" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="92" customWidth="1"/>
-    <col min="9" max="20" width="9.140625" style="92"/>
-    <col min="21" max="21" width="10.42578125" style="92" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" style="92"/>
-    <col min="23" max="23" width="7.7109375" style="92" customWidth="1"/>
-    <col min="24" max="24" width="9.7109375" style="92" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.7109375" style="92" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.28515625" style="92" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.28515625" style="92" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.140625" style="92" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.7109375" style="92" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.5703125" style="92" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.85546875" style="92" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.5703125" style="92" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.28515625" style="92" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="92" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="94" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="93" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="92" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="94" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="91" customWidth="1"/>
+    <col min="9" max="20" width="9.140625" style="91"/>
+    <col min="21" max="21" width="10.42578125" style="91" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" style="91"/>
+    <col min="23" max="23" width="7.7109375" style="91" customWidth="1"/>
+    <col min="24" max="24" width="9.7109375" style="91" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" style="91" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.28515625" style="91" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.28515625" style="91" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.140625" style="91" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.7109375" style="91" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.5703125" style="91" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.85546875" style="91" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.5703125" style="91" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.28515625" style="91" bestFit="1" customWidth="1"/>
     <col min="34" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="114" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+    <row r="1" spans="1:33" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="106" t="s">
         <v>360</v>
       </c>
-      <c r="B1" s="107" t="s">
+      <c r="B1" s="106" t="s">
         <v>454</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="107" t="s">
         <v>446</v>
       </c>
-      <c r="D1" s="109" t="s">
+      <c r="D1" s="108" t="s">
         <v>520</v>
       </c>
-      <c r="E1" s="110" t="s">
+      <c r="E1" s="109" t="s">
         <v>464</v>
       </c>
-      <c r="F1" s="108" t="s">
+      <c r="F1" s="107" t="s">
         <v>462</v>
       </c>
-      <c r="G1" s="109" t="s">
+      <c r="G1" s="108" t="s">
         <v>465</v>
       </c>
-      <c r="H1" s="111" t="s">
+      <c r="H1" s="110" t="s">
         <v>457</v>
       </c>
-      <c r="I1" s="111" t="s">
+      <c r="I1" s="110" t="s">
         <v>447</v>
       </c>
-      <c r="J1" s="111" t="s">
+      <c r="J1" s="110" t="s">
         <v>448</v>
       </c>
-      <c r="K1" s="111" t="s">
+      <c r="K1" s="110" t="s">
         <v>449</v>
       </c>
-      <c r="L1" s="112" t="s">
+      <c r="L1" s="111" t="s">
         <v>507</v>
       </c>
-      <c r="M1" s="112" t="s">
+      <c r="M1" s="111" t="s">
         <v>505</v>
       </c>
-      <c r="N1" s="112" t="s">
+      <c r="N1" s="111" t="s">
         <v>484</v>
       </c>
-      <c r="O1" s="112" t="s">
+      <c r="O1" s="111" t="s">
         <v>452</v>
       </c>
-      <c r="P1" s="112" t="s">
+      <c r="P1" s="111" t="s">
         <v>451</v>
       </c>
-      <c r="Q1" s="112" t="s">
+      <c r="Q1" s="111" t="s">
         <v>458</v>
       </c>
-      <c r="R1" s="112" t="s">
+      <c r="R1" s="111" t="s">
         <v>453</v>
       </c>
-      <c r="S1" s="112" t="s">
+      <c r="S1" s="111" t="s">
         <v>515</v>
       </c>
-      <c r="T1" s="112" t="s">
+      <c r="T1" s="111" t="s">
         <v>459</v>
       </c>
-      <c r="U1" s="112" t="s">
+      <c r="U1" s="111" t="s">
         <v>528</v>
       </c>
-      <c r="V1" s="112" t="s">
+      <c r="V1" s="111" t="s">
         <v>450</v>
       </c>
-      <c r="W1" s="113" t="s">
+      <c r="W1" s="112" t="s">
         <v>466</v>
       </c>
-      <c r="X1" s="113" t="s">
+      <c r="X1" s="112" t="s">
         <v>467</v>
       </c>
-      <c r="Y1" s="113" t="s">
+      <c r="Y1" s="112" t="s">
         <v>468</v>
       </c>
-      <c r="Z1" s="113" t="s">
+      <c r="Z1" s="112" t="s">
         <v>469</v>
       </c>
-      <c r="AA1" s="113" t="s">
+      <c r="AA1" s="112" t="s">
         <v>470</v>
       </c>
-      <c r="AB1" s="113" t="s">
+      <c r="AB1" s="112" t="s">
         <v>471</v>
       </c>
-      <c r="AC1" s="113" t="s">
+      <c r="AC1" s="112" t="s">
         <v>324</v>
       </c>
-      <c r="AD1" s="113" t="s">
+      <c r="AD1" s="112" t="s">
         <v>472</v>
       </c>
-      <c r="AE1" s="113" t="s">
+      <c r="AE1" s="112" t="s">
         <v>473</v>
       </c>
-      <c r="AF1" s="113" t="s">
+      <c r="AF1" s="112" t="s">
         <v>474</v>
       </c>
-      <c r="AG1" s="113" t="s">
+      <c r="AG1" s="112" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="99" t="s">
         <v>478</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="99" t="s">
         <v>477</v>
       </c>
-      <c r="C2" s="101">
+      <c r="C2" s="100">
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="D2" s="102">
+      <c r="D2" s="101">
         <v>50</v>
       </c>
-      <c r="E2" s="103">
+      <c r="E2" s="102">
         <v>1.5986</v>
       </c>
-      <c r="F2" s="101" t="s">
+      <c r="F2" s="100" t="s">
         <v>463</v>
       </c>
-      <c r="G2" s="102">
+      <c r="G2" s="101">
         <v>5</v>
       </c>
-      <c r="H2" s="104">
+      <c r="H2" s="103">
         <v>0.3755</v>
       </c>
-      <c r="I2" s="104">
+      <c r="I2" s="103">
         <v>0.18959999999999999</v>
       </c>
-      <c r="J2" s="104">
+      <c r="J2" s="103">
         <v>0.1489</v>
       </c>
-      <c r="K2" s="104">
+      <c r="K2" s="103">
         <v>0.1497</v>
       </c>
-      <c r="L2" s="105">
+      <c r="L2" s="104">
         <v>0</v>
       </c>
-      <c r="M2" s="105">
+      <c r="M2" s="104">
         <v>0.08</v>
       </c>
-      <c r="N2" s="105">
+      <c r="N2" s="104">
         <v>0</v>
       </c>
-      <c r="O2" s="105">
+      <c r="O2" s="104">
         <v>0.36709999999999998</v>
       </c>
-      <c r="P2" s="105">
+      <c r="P2" s="104">
         <v>0.12</v>
       </c>
-      <c r="Q2" s="105">
+      <c r="Q2" s="104">
         <v>4.5900000000000003E-2</v>
       </c>
-      <c r="R2" s="105">
+      <c r="R2" s="104">
         <v>0</v>
       </c>
-      <c r="S2" s="105">
+      <c r="S2" s="104">
         <v>0</v>
       </c>
-      <c r="T2" s="105">
+      <c r="T2" s="104">
         <v>2.1499999999999998E-2</v>
       </c>
-      <c r="U2" s="105">
+      <c r="U2" s="104">
         <v>0</v>
       </c>
-      <c r="V2" s="105">
+      <c r="V2" s="104">
         <v>0.28000000000000003</v>
       </c>
-      <c r="W2" s="106">
+      <c r="W2" s="105">
         <v>0.19670000000000001</v>
       </c>
-      <c r="X2" s="106">
+      <c r="X2" s="105">
         <v>0.22969999999999999</v>
       </c>
-      <c r="Y2" s="106">
+      <c r="Y2" s="105">
         <v>0.14149999999999999</v>
       </c>
-      <c r="Z2" s="106">
+      <c r="Z2" s="105">
         <v>0.15049999999999999</v>
       </c>
-      <c r="AA2" s="106">
+      <c r="AA2" s="105">
         <v>0.14630000000000001</v>
       </c>
-      <c r="AB2" s="106">
+      <c r="AB2" s="105">
         <v>0.1353</v>
       </c>
-      <c r="AC2" s="106">
+      <c r="AC2" s="105">
         <v>0</v>
       </c>
-      <c r="AD2" s="106">
+      <c r="AD2" s="105">
         <v>0</v>
       </c>
-      <c r="AE2" s="106">
+      <c r="AE2" s="105">
         <v>0</v>
       </c>
-      <c r="AF2" s="106">
+      <c r="AF2" s="105">
         <v>0</v>
       </c>
-      <c r="AG2" s="106">
+      <c r="AG2" s="105">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" s="115" t="s">
+      <c r="A3" s="114" t="s">
         <v>419</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="99" t="s">
         <v>476</v>
       </c>
-      <c r="C3" s="101">
+      <c r="C3" s="100">
         <v>9.7000000000000003E-3</v>
       </c>
-      <c r="D3" s="102">
+      <c r="D3" s="101">
         <v>110</v>
       </c>
-      <c r="E3" s="103">
+      <c r="E3" s="102">
         <v>0.24</v>
       </c>
-      <c r="F3" s="101" t="s">
+      <c r="F3" s="100" t="s">
         <v>463</v>
       </c>
-      <c r="G3" s="102">
+      <c r="G3" s="101">
         <v>5</v>
       </c>
-      <c r="H3" s="104">
+      <c r="H3" s="103">
         <v>0.2135</v>
       </c>
-      <c r="I3" s="104">
+      <c r="I3" s="103">
         <v>9.8799999999999999E-2</v>
       </c>
-      <c r="J3" s="104">
+      <c r="J3" s="103">
         <v>0.1051</v>
       </c>
-      <c r="K3" s="104">
+      <c r="K3" s="103">
         <v>0.1099</v>
       </c>
-      <c r="L3" s="105">
+      <c r="L3" s="104">
         <v>0</v>
       </c>
-      <c r="M3" s="105">
+      <c r="M3" s="104">
         <v>0.32500000000000001</v>
       </c>
-      <c r="N3" s="105">
+      <c r="N3" s="104">
         <v>0</v>
       </c>
-      <c r="O3" s="105">
+      <c r="O3" s="104">
         <v>0.27400000000000002</v>
       </c>
-      <c r="P3" s="105">
+      <c r="P3" s="104">
         <v>0.02</v>
       </c>
-      <c r="Q3" s="105">
+      <c r="Q3" s="104">
         <v>5.7200000000000001E-2</v>
       </c>
-      <c r="R3" s="105">
+      <c r="R3" s="104">
         <v>0.29289999999999999</v>
       </c>
-      <c r="S3" s="105">
+      <c r="S3" s="104">
         <v>0</v>
       </c>
-      <c r="T3" s="105">
+      <c r="T3" s="104">
         <v>0</v>
       </c>
-      <c r="U3" s="105">
+      <c r="U3" s="104">
         <v>0</v>
       </c>
-      <c r="V3" s="105">
+      <c r="V3" s="104">
         <v>0.01</v>
       </c>
-      <c r="W3" s="106">
+      <c r="W3" s="105">
         <v>0.16819999999999999</v>
       </c>
-      <c r="X3" s="106">
+      <c r="X3" s="105">
         <v>0.1457</v>
       </c>
-      <c r="Y3" s="106">
+      <c r="Y3" s="105">
         <v>0.12939999999999999</v>
       </c>
-      <c r="Z3" s="106">
+      <c r="Z3" s="105">
         <v>0.1011</v>
       </c>
-      <c r="AA3" s="106">
+      <c r="AA3" s="105">
         <v>0.1492</v>
       </c>
-      <c r="AB3" s="106">
+      <c r="AB3" s="105">
         <v>9.0399999999999994E-2</v>
       </c>
-      <c r="AC3" s="106">
+      <c r="AC3" s="105">
         <v>2.0400000000000001E-2</v>
       </c>
-      <c r="AD3" s="106">
+      <c r="AD3" s="105">
         <v>0.1242</v>
       </c>
-      <c r="AE3" s="106">
+      <c r="AE3" s="105">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="AF3" s="106">
+      <c r="AF3" s="105">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="AG3" s="106">
+      <c r="AG3" s="105">
         <v>4.24E-2</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="99" t="s">
         <v>430</v>
       </c>
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="99" t="s">
         <v>460</v>
       </c>
-      <c r="C4" s="101">
+      <c r="C4" s="100">
         <v>1.01E-2</v>
       </c>
-      <c r="D4" s="102">
+      <c r="D4" s="101">
         <v>95</v>
       </c>
-      <c r="E4" s="103">
+      <c r="E4" s="102">
         <v>1.37</v>
       </c>
-      <c r="F4" s="101" t="s">
+      <c r="F4" s="100" t="s">
         <v>463</v>
       </c>
-      <c r="G4" s="102">
+      <c r="G4" s="101">
         <v>5</v>
       </c>
-      <c r="H4" s="104">
+      <c r="H4" s="103">
         <v>0.14554</v>
       </c>
-      <c r="I4" s="104">
+      <c r="I4" s="103">
         <v>0.1027</v>
       </c>
-      <c r="J4" s="104">
+      <c r="J4" s="103">
         <v>9.2100000000000001E-2</v>
       </c>
-      <c r="K4" s="104">
+      <c r="K4" s="103">
         <v>0.1052</v>
       </c>
-      <c r="L4" s="105">
+      <c r="L4" s="104">
         <v>0</v>
       </c>
-      <c r="M4" s="105">
+      <c r="M4" s="104">
         <v>0.05</v>
       </c>
-      <c r="N4" s="105">
+      <c r="N4" s="104">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="O4" s="105">
+      <c r="O4" s="104">
         <v>0.10879999999999999</v>
       </c>
-      <c r="P4" s="105">
+      <c r="P4" s="104">
         <v>0.49</v>
       </c>
-      <c r="Q4" s="105">
+      <c r="Q4" s="104">
         <v>2.24E-2</v>
       </c>
-      <c r="R4" s="105">
+      <c r="R4" s="104">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="S4" s="105">
+      <c r="S4" s="104">
         <v>0</v>
       </c>
-      <c r="T4" s="105">
+      <c r="T4" s="104">
         <v>0.01</v>
       </c>
-      <c r="U4" s="105">
+      <c r="U4" s="104">
         <v>0</v>
       </c>
-      <c r="V4" s="105">
+      <c r="V4" s="104">
         <v>0.16</v>
       </c>
-      <c r="W4" s="106">
+      <c r="W4" s="105">
         <v>0.1714</v>
       </c>
-      <c r="X4" s="106">
+      <c r="X4" s="105">
         <v>0.1206</v>
       </c>
-      <c r="Y4" s="106">
+      <c r="Y4" s="105">
         <v>0.12659999999999999</v>
       </c>
-      <c r="Z4" s="106">
+      <c r="Z4" s="105">
         <v>7.1900000000000006E-2</v>
       </c>
-      <c r="AA4" s="106">
+      <c r="AA4" s="105">
         <v>0.11940000000000001</v>
       </c>
-      <c r="AB4" s="106">
+      <c r="AB4" s="105">
         <v>0.1193</v>
       </c>
-      <c r="AC4" s="106">
+      <c r="AC4" s="105">
         <v>1.2699999999999999E-2</v>
       </c>
-      <c r="AD4" s="106">
+      <c r="AD4" s="105">
         <v>0.13120000000000001</v>
       </c>
-      <c r="AE4" s="106">
+      <c r="AE4" s="105">
         <v>5.04E-2</v>
       </c>
-      <c r="AF4" s="106">
+      <c r="AF4" s="105">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="AG4" s="106">
+      <c r="AG4" s="105">
         <v>1.8800000000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" s="115" t="s">
+      <c r="A5" s="114" t="s">
         <v>418</v>
       </c>
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="99" t="s">
         <v>461</v>
       </c>
-      <c r="C5" s="101">
+      <c r="C5" s="100">
         <v>9.9000000000000008E-3</v>
       </c>
-      <c r="D5" s="102">
+      <c r="D5" s="101">
         <v>84</v>
       </c>
-      <c r="E5" s="103">
+      <c r="E5" s="102">
         <v>0.24</v>
       </c>
-      <c r="F5" s="101" t="s">
+      <c r="F5" s="100" t="s">
         <v>463</v>
       </c>
-      <c r="G5" s="102">
+      <c r="G5" s="101">
         <v>4</v>
       </c>
-      <c r="H5" s="104">
+      <c r="H5" s="103">
         <v>0.13370000000000001</v>
       </c>
-      <c r="I5" s="104">
+      <c r="I5" s="103">
         <v>8.7400000000000005E-2</v>
       </c>
-      <c r="J5" s="104">
+      <c r="J5" s="103">
         <v>7.4399999999999994E-2</v>
       </c>
-      <c r="K5" s="104">
+      <c r="K5" s="103">
         <v>9.2100000000000001E-2</v>
       </c>
-      <c r="L5" s="105">
+      <c r="L5" s="104">
         <v>0</v>
       </c>
-      <c r="M5" s="105">
+      <c r="M5" s="104">
         <v>0.05</v>
       </c>
-      <c r="N5" s="105">
+      <c r="N5" s="104">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="O5" s="105">
+      <c r="O5" s="104">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="P5" s="105">
+      <c r="P5" s="104">
         <v>0.45900000000000002</v>
       </c>
-      <c r="Q5" s="105">
+      <c r="Q5" s="104">
         <v>1.04E-2</v>
       </c>
-      <c r="R5" s="105">
+      <c r="R5" s="104">
         <v>0.12590000000000001</v>
       </c>
-      <c r="S5" s="105">
+      <c r="S5" s="104">
         <v>0</v>
       </c>
-      <c r="T5" s="105">
+      <c r="T5" s="104">
         <v>0</v>
       </c>
-      <c r="U5" s="105">
+      <c r="U5" s="104">
         <v>0</v>
       </c>
-      <c r="V5" s="105">
+      <c r="V5" s="104">
         <v>0.18</v>
       </c>
-      <c r="W5" s="106">
+      <c r="W5" s="105">
         <v>0.2487</v>
       </c>
-      <c r="X5" s="106">
+      <c r="X5" s="105">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="Y5" s="106">
+      <c r="Y5" s="105">
         <v>0.1643</v>
       </c>
-      <c r="Z5" s="106">
+      <c r="Z5" s="105">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="AA5" s="106">
+      <c r="AA5" s="105">
         <v>0.13500000000000001</v>
       </c>
-      <c r="AB5" s="106">
+      <c r="AB5" s="105">
         <v>7.1499999999999994E-2</v>
       </c>
-      <c r="AC5" s="106">
+      <c r="AC5" s="105">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="AD5" s="106">
+      <c r="AD5" s="105">
         <v>0.1835</v>
       </c>
-      <c r="AE5" s="106">
+      <c r="AE5" s="105">
         <v>6.3700000000000007E-2</v>
       </c>
-      <c r="AF5" s="106">
+      <c r="AF5" s="105">
         <v>0</v>
       </c>
-      <c r="AG5" s="106">
+      <c r="AG5" s="105">
         <v>1.18E-2</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="99" t="s">
         <v>421</v>
       </c>
-      <c r="B6" s="100" t="s">
+      <c r="B6" s="99" t="s">
         <v>516</v>
       </c>
-      <c r="C6" s="101">
+      <c r="C6" s="100">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D6" s="102">
+      <c r="D6" s="101">
         <v>448</v>
       </c>
-      <c r="E6" s="103">
+      <c r="E6" s="102">
         <v>0.22</v>
       </c>
-      <c r="F6" s="101" t="s">
+      <c r="F6" s="100" t="s">
         <v>463</v>
       </c>
-      <c r="G6" s="102">
+      <c r="G6" s="101">
         <v>3</v>
       </c>
-      <c r="H6" s="104">
+      <c r="H6" s="103">
         <v>3.8399999999999997E-2</v>
       </c>
-      <c r="I6" s="104">
+      <c r="I6" s="103">
         <v>5.6399999999999999E-2</v>
       </c>
-      <c r="J6" s="104">
+      <c r="J6" s="103">
         <v>5.2299999999999999E-2</v>
       </c>
-      <c r="K6" s="104">
+      <c r="K6" s="103">
         <v>7.4800000000000005E-2</v>
       </c>
-      <c r="L6" s="105">
+      <c r="L6" s="104">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="M6" s="105">
+      <c r="M6" s="104">
         <v>0.1105</v>
       </c>
-      <c r="N6" s="105">
+      <c r="N6" s="104">
         <v>0</v>
       </c>
-      <c r="O6" s="105">
+      <c r="O6" s="104">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="P6" s="105">
+      <c r="P6" s="104">
         <v>0.59960000000000002</v>
       </c>
-      <c r="Q6" s="105">
+      <c r="Q6" s="104">
         <v>0</v>
       </c>
-      <c r="R6" s="105">
+      <c r="R6" s="104">
         <v>0.24709999999999999</v>
       </c>
-      <c r="S6" s="105">
+      <c r="S6" s="104">
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="T6" s="105">
+      <c r="T6" s="104">
         <v>0</v>
       </c>
-      <c r="U6" s="105">
+      <c r="U6" s="104">
         <v>0</v>
       </c>
-      <c r="V6" s="105">
+      <c r="V6" s="104">
         <v>1.21E-2</v>
       </c>
-      <c r="W6" s="106">
+      <c r="W6" s="105">
         <v>0.14230000000000001</v>
       </c>
-      <c r="X6" s="106">
+      <c r="X6" s="105">
         <v>0.1182</v>
       </c>
-      <c r="Y6" s="106">
+      <c r="Y6" s="105">
         <v>6.9699999999999998E-2</v>
       </c>
-      <c r="Z6" s="106">
+      <c r="Z6" s="105">
         <v>4.1300000000000003E-2</v>
       </c>
-      <c r="AA6" s="106">
+      <c r="AA6" s="105">
         <v>0.19819999999999999</v>
       </c>
-      <c r="AB6" s="106">
+      <c r="AB6" s="105">
         <v>0.1673</v>
       </c>
-      <c r="AC6" s="106">
+      <c r="AC6" s="105">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="AD6" s="106">
+      <c r="AD6" s="105">
         <v>0.15079999999999999</v>
       </c>
-      <c r="AE6" s="106">
+      <c r="AE6" s="105">
         <v>5.6399999999999999E-2</v>
       </c>
-      <c r="AF6" s="106">
+      <c r="AF6" s="105">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="AG6" s="106">
+      <c r="AG6" s="105">
         <v>1.9599999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="99" t="s">
         <v>455</v>
       </c>
-      <c r="B7" s="100" t="s">
+      <c r="B7" s="99" t="s">
         <v>456</v>
       </c>
-      <c r="C7" s="101">
+      <c r="C7" s="100">
         <v>9.4000000000000004E-3</v>
       </c>
-      <c r="D7" s="102">
+      <c r="D7" s="101">
         <v>86</v>
       </c>
-      <c r="E7" s="103">
+      <c r="E7" s="102">
         <v>0.43</v>
       </c>
-      <c r="F7" s="101" t="s">
+      <c r="F7" s="100" t="s">
         <v>463</v>
       </c>
-      <c r="G7" s="102">
+      <c r="G7" s="101">
         <v>5</v>
       </c>
-      <c r="H7" s="104">
+      <c r="H7" s="103">
         <v>0.218</v>
       </c>
-      <c r="I7" s="104">
+      <c r="I7" s="103">
         <v>0.1055</v>
       </c>
-      <c r="J7" s="104">
+      <c r="J7" s="103">
         <v>0.11219999999999999</v>
       </c>
-      <c r="K7" s="104">
+      <c r="K7" s="103">
         <v>6.3799999999999996E-2</v>
       </c>
-      <c r="L7" s="105">
+      <c r="L7" s="104">
         <v>0</v>
       </c>
-      <c r="M7" s="105">
+      <c r="M7" s="104">
         <v>0.17</v>
       </c>
-      <c r="N7" s="105">
+      <c r="N7" s="104">
         <v>0</v>
       </c>
-      <c r="O7" s="105">
+      <c r="O7" s="104">
         <v>0.35199999999999998</v>
       </c>
-      <c r="P7" s="105">
+      <c r="P7" s="104">
         <v>0.06</v>
       </c>
-      <c r="Q7" s="105">
+      <c r="Q7" s="104">
         <v>0.1116</v>
       </c>
-      <c r="R7" s="105">
+      <c r="R7" s="104">
         <v>0</v>
       </c>
-      <c r="S7" s="105">
+      <c r="S7" s="104">
         <v>0</v>
       </c>
-      <c r="T7" s="105">
+      <c r="T7" s="104">
         <v>0.05</v>
       </c>
-      <c r="U7" s="105">
+      <c r="U7" s="104">
         <v>0</v>
       </c>
-      <c r="V7" s="105">
+      <c r="V7" s="104">
         <v>0.08</v>
       </c>
-      <c r="W7" s="106">
+      <c r="W7" s="105">
         <v>0.2185</v>
       </c>
-      <c r="X7" s="106">
+      <c r="X7" s="105">
         <v>0.1825</v>
       </c>
-      <c r="Y7" s="106">
+      <c r="Y7" s="105">
         <v>0.15820000000000001</v>
       </c>
-      <c r="Z7" s="106">
+      <c r="Z7" s="105">
         <v>0.13300000000000001</v>
       </c>
-      <c r="AA7" s="106">
+      <c r="AA7" s="105">
         <v>6.9800000000000001E-2</v>
       </c>
-      <c r="AB7" s="106">
+      <c r="AB7" s="105">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="AC7" s="106">
+      <c r="AC7" s="105">
         <v>6.7900000000000002E-2</v>
       </c>
-      <c r="AD7" s="106">
+      <c r="AD7" s="105">
         <v>4.48E-2</v>
       </c>
-      <c r="AE7" s="106">
+      <c r="AE7" s="105">
         <v>1.9199999999999998E-2</v>
       </c>
-      <c r="AF7" s="106">
+      <c r="AF7" s="105">
         <v>1.0500000000000001E-2</v>
       </c>
-      <c r="AG7" s="106">
+      <c r="AG7" s="105">
         <v>0.01</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A8" s="100" t="s">
+      <c r="A8" s="99" t="s">
         <v>429</v>
       </c>
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="99" t="s">
         <v>530</v>
       </c>
-      <c r="C8" s="101">
+      <c r="C8" s="100">
         <v>4.8999999999999998E-3</v>
       </c>
-      <c r="D8" s="102">
+      <c r="D8" s="101">
         <v>1236</v>
       </c>
-      <c r="E8" s="103">
+      <c r="E8" s="102">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F8" s="101" t="s">
+      <c r="F8" s="100" t="s">
         <v>531</v>
       </c>
-      <c r="G8" s="102">
+      <c r="G8" s="101">
         <v>3</v>
       </c>
-      <c r="H8" s="104">
+      <c r="H8" s="103">
         <v>4.19E-2</v>
       </c>
-      <c r="I8" s="104">
+      <c r="I8" s="103">
         <v>5.0500000000000003E-2</v>
       </c>
-      <c r="J8" s="104">
+      <c r="J8" s="103">
         <v>4.87E-2</v>
       </c>
-      <c r="K8" s="104">
+      <c r="K8" s="103">
         <v>6.1699999999999998E-2</v>
       </c>
-      <c r="L8" s="105">
+      <c r="L8" s="104">
         <v>0</v>
       </c>
-      <c r="M8" s="105">
+      <c r="M8" s="104">
         <v>0.2908</v>
       </c>
-      <c r="N8" s="105">
+      <c r="N8" s="104">
         <v>0</v>
       </c>
-      <c r="O8" s="105">
+      <c r="O8" s="104">
         <v>0.53300000000000003</v>
       </c>
-      <c r="P8" s="105">
+      <c r="P8" s="104">
         <v>2.7099999999999999E-2</v>
       </c>
-      <c r="Q8" s="105">
+      <c r="Q8" s="104">
         <v>0.14149999999999999</v>
       </c>
-      <c r="R8" s="105">
+      <c r="R8" s="104">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="S8" s="105">
+      <c r="S8" s="104">
         <v>0</v>
       </c>
-      <c r="T8" s="105">
+      <c r="T8" s="104">
         <v>0</v>
       </c>
-      <c r="U8" s="105">
+      <c r="U8" s="104">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="V8" s="105">
+      <c r="V8" s="104">
         <v>1.8E-3</v>
       </c>
-      <c r="W8" s="106">
+      <c r="W8" s="105">
         <v>0.18310000000000001</v>
       </c>
-      <c r="X8" s="106">
+      <c r="X8" s="105">
         <v>0.18970000000000001</v>
       </c>
-      <c r="Y8" s="106">
+      <c r="Y8" s="105">
         <v>0.17460000000000001</v>
       </c>
-      <c r="Z8" s="106">
+      <c r="Z8" s="105">
         <v>0.13489999999999999</v>
       </c>
-      <c r="AA8" s="106">
+      <c r="AA8" s="105">
         <v>5.0500000000000003E-2</v>
       </c>
-      <c r="AB8" s="106">
+      <c r="AB8" s="105">
         <v>5.96E-2</v>
       </c>
-      <c r="AC8" s="106">
+      <c r="AC8" s="105">
         <v>4.3400000000000001E-2</v>
       </c>
-      <c r="AD8" s="106">
+      <c r="AD8" s="105">
         <v>5.62E-2</v>
       </c>
-      <c r="AE8" s="106">
+      <c r="AE8" s="105">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="AF8" s="106">
+      <c r="AF8" s="105">
         <v>1.77E-2</v>
       </c>
-      <c r="AG8" s="106">
+      <c r="AG8" s="105">
         <v>3.1199999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="99" t="s">
         <v>420</v>
       </c>
-      <c r="B9" s="100" t="s">
+      <c r="B9" s="99" t="s">
         <v>479</v>
       </c>
-      <c r="C9" s="101">
+      <c r="C9" s="100">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D9" s="102">
+      <c r="D9" s="101">
         <v>293</v>
       </c>
-      <c r="E9" s="103">
+      <c r="E9" s="102">
         <v>1.05</v>
       </c>
-      <c r="F9" s="101" t="s">
+      <c r="F9" s="100" t="s">
         <v>463</v>
       </c>
-      <c r="G9" s="102">
+      <c r="G9" s="101">
         <v>3</v>
       </c>
-      <c r="H9" s="104">
+      <c r="H9" s="103">
         <v>6.8500000000000005E-2</v>
       </c>
-      <c r="I9" s="104">
+      <c r="I9" s="103">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="J9" s="104">
+      <c r="J9" s="103">
         <v>5.2699999999999997E-2</v>
       </c>
-      <c r="K9" s="104"/>
-      <c r="L9" s="105">
+      <c r="K9" s="103"/>
+      <c r="L9" s="104">
         <v>8.6999999999999994E-3</v>
       </c>
-      <c r="M9" s="105">
+      <c r="M9" s="104">
         <v>6.0600000000000001E-2</v>
       </c>
-      <c r="N9" s="105">
+      <c r="N9" s="104">
         <v>8.09E-2</v>
       </c>
-      <c r="O9" s="105">
+      <c r="O9" s="104">
         <v>7.9000000000000008E-3</v>
       </c>
-      <c r="P9" s="105">
+      <c r="P9" s="104">
         <v>0.54800000000000004</v>
       </c>
-      <c r="Q9" s="105">
+      <c r="Q9" s="104">
         <v>0</v>
       </c>
-      <c r="R9" s="105">
+      <c r="R9" s="104">
         <v>0.22969999999999999</v>
       </c>
-      <c r="S9" s="105">
+      <c r="S9" s="104">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="T9" s="105">
+      <c r="T9" s="104">
         <v>0</v>
       </c>
-      <c r="U9" s="105">
+      <c r="U9" s="104">
         <v>0</v>
       </c>
-      <c r="V9" s="105">
+      <c r="V9" s="104">
         <v>4.1599999999999998E-2</v>
       </c>
-      <c r="W9" s="106">
+      <c r="W9" s="105">
         <v>0.18329999999999999</v>
       </c>
-      <c r="X9" s="106">
+      <c r="X9" s="105">
         <v>7.8799999999999995E-2</v>
       </c>
-      <c r="Y9" s="106">
+      <c r="Y9" s="105">
         <v>5.0900000000000001E-2</v>
       </c>
-      <c r="Z9" s="106">
+      <c r="Z9" s="105">
         <v>5.5500000000000001E-2</v>
       </c>
-      <c r="AA9" s="106">
+      <c r="AA9" s="105">
         <v>0.26950000000000002</v>
       </c>
-      <c r="AB9" s="106">
+      <c r="AB9" s="105">
         <v>6.6600000000000006E-2</v>
       </c>
-      <c r="AC9" s="106">
+      <c r="AC9" s="105">
         <v>8.8999999999999999E-3</v>
       </c>
-      <c r="AD9" s="106">
+      <c r="AD9" s="105">
         <v>0.1022</v>
       </c>
-      <c r="AE9" s="106">
+      <c r="AE9" s="105">
         <v>0.1086</v>
       </c>
-      <c r="AF9" s="106">
+      <c r="AF9" s="105">
         <v>5.6599999999999998E-2</v>
       </c>
-      <c r="AG9" s="106">
+      <c r="AG9" s="105">
         <v>1.1599999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" s="100" t="s">
+      <c r="A10" s="99" t="s">
         <v>480</v>
       </c>
-      <c r="B10" s="100" t="s">
+      <c r="B10" s="99" t="s">
         <v>533</v>
       </c>
-      <c r="C10" s="101">
+      <c r="C10" s="100">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D10" s="102">
+      <c r="D10" s="101">
         <v>883</v>
       </c>
-      <c r="E10" s="103">
+      <c r="E10" s="102">
         <v>0.16</v>
       </c>
-      <c r="F10" s="101" t="s">
+      <c r="F10" s="100" t="s">
         <v>531</v>
       </c>
-      <c r="G10" s="102">
+      <c r="G10" s="101">
         <v>3</v>
       </c>
-      <c r="H10" s="104">
+      <c r="H10" s="103">
         <v>3.0599999999999999E-2</v>
       </c>
-      <c r="I10" s="104">
+      <c r="I10" s="103">
         <v>3.2199999999999999E-2</v>
       </c>
-      <c r="J10" s="104">
+      <c r="J10" s="103">
         <v>4.1399999999999999E-2</v>
       </c>
-      <c r="K10" s="104"/>
-      <c r="L10" s="105">
+      <c r="K10" s="103"/>
+      <c r="L10" s="104">
         <v>0</v>
       </c>
-      <c r="M10" s="105">
+      <c r="M10" s="104">
         <v>0.39419999999999999</v>
       </c>
-      <c r="N10" s="105">
+      <c r="N10" s="104">
         <v>0</v>
       </c>
-      <c r="O10" s="105">
+      <c r="O10" s="104">
         <v>0.47170000000000001</v>
       </c>
-      <c r="P10" s="105">
+      <c r="P10" s="104">
         <v>2.4500000000000001E-2</v>
       </c>
-      <c r="Q10" s="105">
+      <c r="Q10" s="104">
         <v>9.7199999999999995E-2</v>
       </c>
-      <c r="R10" s="105">
+      <c r="R10" s="104">
         <v>2E-3</v>
       </c>
-      <c r="S10" s="105">
+      <c r="S10" s="104">
         <v>0</v>
       </c>
-      <c r="T10" s="105">
+      <c r="T10" s="104">
         <v>0</v>
       </c>
-      <c r="U10" s="105">
+      <c r="U10" s="104">
         <v>0</v>
       </c>
-      <c r="V10" s="105">
+      <c r="V10" s="104">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="W10" s="106">
+      <c r="W10" s="105">
         <v>0.2104</v>
       </c>
-      <c r="X10" s="106">
+      <c r="X10" s="105">
         <v>0.18629999999999999</v>
       </c>
-      <c r="Y10" s="106">
+      <c r="Y10" s="105">
         <v>0.15629999999999999</v>
       </c>
-      <c r="Z10" s="106">
+      <c r="Z10" s="105">
         <v>0.1424</v>
       </c>
-      <c r="AA10" s="106">
+      <c r="AA10" s="105">
         <v>4.6300000000000001E-2</v>
       </c>
-      <c r="AB10" s="106">
+      <c r="AB10" s="105">
         <v>5.67E-2</v>
       </c>
-      <c r="AC10" s="106">
+      <c r="AC10" s="105">
         <v>4.07E-2</v>
       </c>
-      <c r="AD10" s="106">
+      <c r="AD10" s="105">
         <v>5.0099999999999999E-2</v>
       </c>
-      <c r="AE10" s="106">
+      <c r="AE10" s="105">
         <v>4.7100000000000003E-2</v>
       </c>
-      <c r="AF10" s="106">
+      <c r="AF10" s="105">
         <v>1.89E-2</v>
       </c>
-      <c r="AG10" s="106">
+      <c r="AG10" s="105">
         <v>2.76E-2</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" s="100"/>
-      <c r="B11" s="100"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="104"/>
-      <c r="I11" s="104"/>
-      <c r="J11" s="104"/>
-      <c r="K11" s="104"/>
-      <c r="L11" s="105"/>
-      <c r="M11" s="105"/>
-      <c r="N11" s="105"/>
-      <c r="O11" s="105"/>
-      <c r="P11" s="105"/>
-      <c r="Q11" s="105"/>
-      <c r="R11" s="105"/>
-      <c r="S11" s="105"/>
-      <c r="T11" s="105"/>
-      <c r="U11" s="105"/>
-      <c r="V11" s="105"/>
-      <c r="W11" s="106"/>
-      <c r="X11" s="106"/>
-      <c r="Y11" s="106"/>
-      <c r="Z11" s="106"/>
-      <c r="AA11" s="106"/>
-      <c r="AB11" s="106"/>
-      <c r="AC11" s="106"/>
-      <c r="AD11" s="106"/>
-      <c r="AE11" s="106"/>
-      <c r="AF11" s="106"/>
-      <c r="AG11" s="106"/>
+      <c r="A11" s="99"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="100"/>
+      <c r="D11" s="101"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="100"/>
+      <c r="G11" s="101"/>
+      <c r="H11" s="103"/>
+      <c r="I11" s="103"/>
+      <c r="J11" s="103"/>
+      <c r="K11" s="103"/>
+      <c r="L11" s="104"/>
+      <c r="M11" s="104"/>
+      <c r="N11" s="104"/>
+      <c r="O11" s="104"/>
+      <c r="P11" s="104"/>
+      <c r="Q11" s="104"/>
+      <c r="R11" s="104"/>
+      <c r="S11" s="104"/>
+      <c r="T11" s="104"/>
+      <c r="U11" s="104"/>
+      <c r="V11" s="104"/>
+      <c r="W11" s="105"/>
+      <c r="X11" s="105"/>
+      <c r="Y11" s="105"/>
+      <c r="Z11" s="105"/>
+      <c r="AA11" s="105"/>
+      <c r="AB11" s="105"/>
+      <c r="AC11" s="105"/>
+      <c r="AD11" s="105"/>
+      <c r="AE11" s="105"/>
+      <c r="AF11" s="105"/>
+      <c r="AG11" s="105"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG10" xr:uid="{354A7ECD-5F19-4009-838D-52EE93D742A5}">
@@ -24553,7 +24536,7 @@
     <col min="11" max="11" width="11.28515625" style="14" bestFit="1" customWidth="1"/>
     <col min="12" max="15" width="9.140625" style="14"/>
     <col min="16" max="16" width="13.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" style="92" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" style="91" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
@@ -24561,7 +24544,7 @@
       <c r="A1" s="14" t="s">
         <v>453</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="90" t="s">
         <v>453</v>
       </c>
       <c r="I1" s="14" t="s">
@@ -24573,7 +24556,7 @@
       <c r="K1" s="14" t="s">
         <v>504</v>
       </c>
-      <c r="P1" s="97" t="s">
+      <c r="P1" s="96" t="s">
         <v>508</v>
       </c>
       <c r="Q1" t="s">
@@ -24585,41 +24568,41 @@
       <c r="A2" s="14" t="s">
         <v>481</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="90" t="s">
         <v>451</v>
       </c>
       <c r="I2" s="14" t="s">
         <v>452</v>
       </c>
-      <c r="J2" s="91">
+      <c r="J2" s="90">
         <v>0.47170000000000001</v>
       </c>
       <c r="K2" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I2,A:B,2,FALSE),"")</f>
+        <f t="shared" ref="K2:K22" si="0">IFERROR(VLOOKUP(I2,A:B,2,FALSE),"")</f>
         <v>China</v>
       </c>
       <c r="P2"/>
-      <c r="Q2" s="99"/>
+      <c r="Q2" s="98"/>
       <c r="R2"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>451</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>521</v>
       </c>
-      <c r="J3" s="91">
+      <c r="J3" s="90">
         <v>0.1641</v>
       </c>
       <c r="K3" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I3,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>Asia</v>
       </c>
-      <c r="P3" s="97" t="s">
+      <c r="P3" s="96" t="s">
         <v>510</v>
       </c>
       <c r="Q3" t="s">
@@ -24631,44 +24614,44 @@
       <c r="A4" s="14" t="s">
         <v>483</v>
       </c>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="90" t="s">
         <v>451</v>
       </c>
       <c r="I4" s="14" t="s">
         <v>502</v>
       </c>
-      <c r="J4" s="91">
+      <c r="J4" s="90">
         <v>0.14430000000000001</v>
       </c>
       <c r="K4" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I4,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>Asia</v>
       </c>
-      <c r="P4" s="98"/>
-      <c r="Q4" s="96"/>
+      <c r="P4" s="97"/>
+      <c r="Q4" s="95"/>
       <c r="R4"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>484</v>
       </c>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="90" t="s">
         <v>484</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>458</v>
       </c>
-      <c r="J5" s="91">
+      <c r="J5" s="90">
         <v>9.7199999999999995E-2</v>
       </c>
       <c r="K5" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I5,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>India</v>
       </c>
-      <c r="P5" s="98" t="s">
+      <c r="P5" s="97" t="s">
         <v>505</v>
       </c>
-      <c r="Q5" s="96">
+      <c r="Q5" s="95">
         <v>0.39420000000000005</v>
       </c>
       <c r="R5"/>
@@ -24677,23 +24660,23 @@
       <c r="A6" s="14" t="s">
         <v>485</v>
       </c>
-      <c r="B6" s="91" t="s">
+      <c r="B6" s="90" t="s">
         <v>451</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>522</v>
       </c>
-      <c r="J6" s="91">
+      <c r="J6" s="90">
         <v>2.6800000000000001E-2</v>
       </c>
       <c r="K6" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I6,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>Asia</v>
       </c>
-      <c r="P6" s="98" t="s">
+      <c r="P6" s="97" t="s">
         <v>452</v>
       </c>
-      <c r="Q6" s="96">
+      <c r="Q6" s="95">
         <v>0.47170000000000001</v>
       </c>
       <c r="R6"/>
@@ -24702,23 +24685,23 @@
       <c r="A7" s="14" t="s">
         <v>486</v>
       </c>
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="90" t="s">
         <v>451</v>
       </c>
       <c r="I7" s="14" t="s">
         <v>519</v>
       </c>
-      <c r="J7" s="91">
+      <c r="J7" s="90">
         <v>2.35E-2</v>
       </c>
       <c r="K7" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I7,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>Asia</v>
       </c>
-      <c r="P7" s="98" t="s">
+      <c r="P7" s="97" t="s">
         <v>451</v>
       </c>
-      <c r="Q7" s="96">
+      <c r="Q7" s="95">
         <v>2.4499999999999997E-2</v>
       </c>
       <c r="R7"/>
@@ -24727,23 +24710,23 @@
       <c r="A8" s="14" t="s">
         <v>487</v>
       </c>
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="90" t="s">
         <v>451</v>
       </c>
       <c r="I8" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="J8" s="91">
+      <c r="J8" s="90">
         <v>2.1299999999999999E-2</v>
       </c>
       <c r="K8" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I8,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>Europe</v>
       </c>
-      <c r="P8" s="98" t="s">
+      <c r="P8" s="97" t="s">
         <v>458</v>
       </c>
-      <c r="Q8" s="96">
+      <c r="Q8" s="95">
         <v>9.7199999999999995E-2</v>
       </c>
       <c r="R8"/>
@@ -24752,23 +24735,23 @@
       <c r="A9" s="14" t="s">
         <v>488</v>
       </c>
-      <c r="B9" s="91" t="s">
+      <c r="B9" s="90" t="s">
         <v>450</v>
       </c>
       <c r="I9" s="14" t="s">
         <v>523</v>
       </c>
-      <c r="J9" s="91">
+      <c r="J9" s="90">
         <v>1.38E-2</v>
       </c>
       <c r="K9" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I9,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>Asia</v>
       </c>
-      <c r="P9" s="98" t="s">
+      <c r="P9" s="97" t="s">
         <v>453</v>
       </c>
-      <c r="Q9" s="96">
+      <c r="Q9" s="95">
         <v>2E-3</v>
       </c>
       <c r="R9"/>
@@ -24777,23 +24760,23 @@
       <c r="A10" s="14" t="s">
         <v>489</v>
       </c>
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="90" t="s">
         <v>505</v>
       </c>
       <c r="I10" s="14" t="s">
         <v>493</v>
       </c>
-      <c r="J10" s="91">
+      <c r="J10" s="90">
         <v>1.06E-2</v>
       </c>
       <c r="K10" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I10,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>Asia</v>
       </c>
-      <c r="P10" s="98" t="s">
+      <c r="P10" s="97" t="s">
         <v>450</v>
       </c>
-      <c r="Q10" s="96">
+      <c r="Q10" s="95">
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="R10"/>
@@ -24802,46 +24785,46 @@
       <c r="A11" s="14" t="s">
         <v>490</v>
       </c>
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="90" t="s">
         <v>451</v>
       </c>
       <c r="I11" s="14" t="s">
         <v>524</v>
       </c>
-      <c r="J11" s="91">
+      <c r="J11" s="90">
         <v>1.01E-2</v>
       </c>
       <c r="K11" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I11,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>Asia</v>
       </c>
-      <c r="P11" s="98" t="s">
+      <c r="P11" s="97" t="s">
         <v>511</v>
       </c>
-      <c r="Q11" s="96"/>
+      <c r="Q11" s="95"/>
       <c r="R11"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>491</v>
       </c>
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="90" t="s">
         <v>451</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>488</v>
       </c>
-      <c r="J12" s="91">
+      <c r="J12" s="90">
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="K12" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I12,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>US</v>
       </c>
-      <c r="P12" s="98" t="s">
+      <c r="P12" s="97" t="s">
         <v>512</v>
       </c>
-      <c r="Q12" s="96">
+      <c r="Q12" s="95">
         <v>0.99230000000000007</v>
       </c>
       <c r="R12"/>
@@ -24850,17 +24833,17 @@
       <c r="A13" s="14" t="s">
         <v>492</v>
       </c>
-      <c r="B13" s="91" t="s">
+      <c r="B13" s="90" t="s">
         <v>451</v>
       </c>
       <c r="I13" s="14" t="s">
         <v>453</v>
       </c>
-      <c r="J13" s="91">
+      <c r="J13" s="90">
         <v>2E-3</v>
       </c>
       <c r="K13" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I13,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>Japan</v>
       </c>
       <c r="P13"/>
@@ -24871,122 +24854,122 @@
       <c r="A14" s="14" t="s">
         <v>493</v>
       </c>
-      <c r="B14" s="91" t="s">
+      <c r="B14" s="90" t="s">
         <v>505</v>
       </c>
       <c r="I14" s="14" t="s">
         <v>481</v>
       </c>
-      <c r="J14" s="91">
+      <c r="J14" s="90">
         <v>1.4E-3</v>
       </c>
       <c r="K14" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I14,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>Europe</v>
       </c>
       <c r="P14"/>
-      <c r="Q14" s="99"/>
+      <c r="Q14" s="98"/>
       <c r="R14"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>494</v>
       </c>
-      <c r="B15" s="91" t="s">
+      <c r="B15" s="90" t="s">
         <v>507</v>
       </c>
       <c r="I15" s="14" t="s">
         <v>486</v>
       </c>
-      <c r="J15" s="91">
+      <c r="J15" s="90">
         <v>1E-3</v>
       </c>
       <c r="K15" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I15,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>Europe</v>
       </c>
       <c r="P15"/>
-      <c r="Q15" s="99"/>
+      <c r="Q15" s="98"/>
       <c r="R15"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>495</v>
       </c>
-      <c r="B16" s="91" t="s">
+      <c r="B16" s="90" t="s">
         <v>505</v>
       </c>
       <c r="I16" s="14" t="s">
         <v>485</v>
       </c>
-      <c r="J16" s="91">
+      <c r="J16" s="90">
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="K16" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I16,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>Europe</v>
       </c>
       <c r="P16"/>
-      <c r="Q16" s="99"/>
+      <c r="Q16" s="98"/>
       <c r="R16"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>452</v>
       </c>
-      <c r="B17" s="91" t="s">
+      <c r="B17" s="90" t="s">
         <v>452</v>
       </c>
       <c r="I17" s="14" t="s">
         <v>532</v>
       </c>
-      <c r="J17" s="91">
+      <c r="J17" s="90">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="K17" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I17,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P17"/>
-      <c r="Q17" s="99"/>
+      <c r="Q17" s="98"/>
       <c r="R17"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>496</v>
       </c>
-      <c r="B18" s="91" t="s">
+      <c r="B18" s="90" t="s">
         <v>451</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>501</v>
       </c>
-      <c r="J18" s="91">
+      <c r="J18" s="90">
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="K18" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I18,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>Asia</v>
       </c>
       <c r="P18"/>
-      <c r="Q18" s="99"/>
+      <c r="Q18" s="98"/>
       <c r="R18"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>497</v>
       </c>
-      <c r="B19" s="91" t="s">
+      <c r="B19" s="90" t="s">
         <v>451</v>
       </c>
       <c r="I19" s="14" t="s">
         <v>526</v>
       </c>
-      <c r="J19" s="91">
+      <c r="J19" s="90">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="K19" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I19,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>Asia</v>
       </c>
     </row>
@@ -24994,17 +24977,17 @@
       <c r="A20" s="14" t="s">
         <v>498</v>
       </c>
-      <c r="B20" s="91" t="s">
+      <c r="B20" s="90" t="s">
         <v>506</v>
       </c>
       <c r="I20" s="14" t="s">
         <v>525</v>
       </c>
-      <c r="J20" s="91">
+      <c r="J20" s="90">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="K20" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I20,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>Asia</v>
       </c>
     </row>
@@ -25012,17 +24995,17 @@
       <c r="A21" s="14" t="s">
         <v>499</v>
       </c>
-      <c r="B21" s="91" t="s">
+      <c r="B21" s="90" t="s">
         <v>451</v>
       </c>
       <c r="I21" s="14" t="s">
         <v>487</v>
       </c>
-      <c r="J21" s="91">
+      <c r="J21" s="90">
         <v>1E-4</v>
       </c>
       <c r="K21" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I21,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>Europe</v>
       </c>
     </row>
@@ -25030,12 +25013,12 @@
       <c r="A22" s="14" t="s">
         <v>500</v>
       </c>
-      <c r="B22" s="91" t="s">
+      <c r="B22" s="90" t="s">
         <v>451</v>
       </c>
-      <c r="J22" s="91"/>
+      <c r="J22" s="90"/>
       <c r="K22" s="14" t="str">
-        <f>IFERROR(VLOOKUP(I22,A:B,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -25043,28 +25026,28 @@
       <c r="A23" s="14" t="s">
         <v>501</v>
       </c>
-      <c r="B23" s="91" t="s">
+      <c r="B23" s="90" t="s">
         <v>505</v>
       </c>
-      <c r="J23" s="91"/>
+      <c r="J23" s="90"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>502</v>
       </c>
-      <c r="B24" s="91" t="s">
+      <c r="B24" s="90" t="s">
         <v>505</v>
       </c>
-      <c r="J24" s="91"/>
+      <c r="J24" s="90"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>503</v>
       </c>
-      <c r="B25" s="91" t="s">
+      <c r="B25" s="90" t="s">
         <v>505</v>
       </c>
-      <c r="J25" s="91"/>
+      <c r="J25" s="90"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
@@ -25073,7 +25056,7 @@
       <c r="B26" s="14" t="s">
         <v>458</v>
       </c>
-      <c r="J26" s="91"/>
+      <c r="J26" s="90"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
@@ -25082,7 +25065,7 @@
       <c r="B27" s="14" t="s">
         <v>459</v>
       </c>
-      <c r="J27" s="91"/>
+      <c r="J27" s="90"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
@@ -25182,21 +25165,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D95AC4467A64E54FAB628610D0FE135F" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="79e84842eaddaeb917644b39e1597e3c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e8f9595b-0d5a-46b2-8488-c972c1ea4246" xmlns:ns4="6bcbbac3-d60f-4c54-b2b4-d245c065548d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb8f6ae9099bbec0b468ebfdbf5b501b" ns3:_="" ns4:_="">
     <xsd:import namespace="e8f9595b-0d5a-46b2-8488-c972c1ea4246"/>
@@ -25419,32 +25387,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DB5870C-189D-475E-8E58-449C30115ACA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401ADED5-CC5A-4072-B36A-6DA217C5A368}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6bcbbac3-d60f-4c54-b2b4-d245c065548d"/>
-    <ds:schemaRef ds:uri="e8f9595b-0d5a-46b2-8488-c972c1ea4246"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11321DBA-FDAB-45E8-A045-E3E44A7AE235}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25461,4 +25419,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401ADED5-CC5A-4072-B36A-6DA217C5A368}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e8f9595b-0d5a-46b2-8488-c972c1ea4246"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6bcbbac3-d60f-4c54-b2b4-d245c065548d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DB5870C-189D-475E-8E58-449C30115ACA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>